<commit_message>
Spreadsheet with performance results has been updated
</commit_message>
<xml_diff>
--- a/sbp-accuracy-other-predictors.xlsx
+++ b/sbp-accuracy-other-predictors.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelktistakis/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelktistakis/Repositories/sBP/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="500"/>
+    <workbookView xWindow="51200" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="38">
   <si>
     <t>Test Time</t>
   </si>
@@ -101,17 +101,56 @@
     <t>Overall Accur</t>
   </si>
   <si>
-    <t>subSeq (Java baseline)</t>
+    <t>subSeq (BWT implementationi)</t>
   </si>
   <si>
-    <t>subSeq (BWT implementationi)</t>
+    <t>Test Time (ms)</t>
+  </si>
+  <si>
+    <t>Time: subSeq/CPT+</t>
+  </si>
+  <si>
+    <t>Memory: CPT+/subSeq</t>
+  </si>
+  <si>
+    <t>CPT+ bits per sequence</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>subSeq bits per sequence</t>
+  </si>
+  <si>
+    <t>BIBLE_CHAR, rough space estimation per sequence</t>
+  </si>
+  <si>
+    <t>WT for L</t>
+  </si>
+  <si>
+    <t>WT for alphabet</t>
+  </si>
+  <si>
+    <t>int vector for counters</t>
+  </si>
+  <si>
+    <t>Trie</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>II</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -143,8 +182,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,12 +209,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -179,7 +219,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="801">
+  <cellStyleXfs count="821">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -981,29 +1021,37 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1013,23 +1061,35 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="801">
+  <cellStyles count="821">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1430,6 +1490,16 @@
     <cellStyle name="Followed Hyperlink" xfId="796" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="798" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="800" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="802" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="804" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="806" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="808" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="810" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="812" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="814" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="816" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="818" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="820" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1830,6 +1900,16 @@
     <cellStyle name="Hyperlink" xfId="795" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="797" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="799" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="801" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="803" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="805" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="807" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="809" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="811" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="813" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="815" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="817" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="819" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2105,58 +2185,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R91"/>
+  <dimension ref="A1:Q91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="18"/>
-    <col min="18" max="18" width="117.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="5"/>
+    <col min="17" max="17" width="117.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="7" t="s">
+    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="B2" s="4" t="s">
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="9"/>
+    </row>
+    <row r="2" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -2172,17 +2254,17 @@
       <c r="E3">
         <v>36.186</v>
       </c>
+      <c r="G3">
+        <v>31.343</v>
+      </c>
       <c r="H3">
-        <v>31.343</v>
+        <v>31.033999999999999</v>
       </c>
       <c r="I3">
-        <v>31.033999999999999</v>
-      </c>
-      <c r="J3">
         <v>32.58</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2198,17 +2280,17 @@
       <c r="E4">
         <v>63.814</v>
       </c>
+      <c r="G4">
+        <v>68.656999999999996</v>
+      </c>
       <c r="H4">
-        <v>68.656999999999996</v>
+        <v>68.965999999999994</v>
       </c>
       <c r="I4">
-        <v>68.965999999999994</v>
-      </c>
-      <c r="J4">
         <v>67.42</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2224,17 +2306,17 @@
       <c r="E5">
         <v>0.308</v>
       </c>
+      <c r="G5">
+        <v>0.185</v>
+      </c>
       <c r="H5">
         <v>0.185</v>
       </c>
       <c r="I5">
-        <v>0.185</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2250,170 +2332,178 @@
       <c r="E6">
         <v>0</v>
       </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="19">
         <v>36.115000000000002</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="19">
         <v>6.68</v>
       </c>
-      <c r="D7" s="15">
-        <v>36.978000000000002</v>
-      </c>
-      <c r="E7" s="15">
-        <v>36.073999999999998</v>
-      </c>
-      <c r="F7" s="19">
-        <f>AVERAGE(0.24013157, 0.24259868, 0.27302632, 0.24157766)*100</f>
-        <v>24.93335575</v>
-      </c>
-      <c r="G7" s="15">
-        <v>29</v>
-      </c>
-      <c r="H7" s="15">
-        <v>31.285</v>
-      </c>
-      <c r="I7" s="15">
+      <c r="D7" s="19">
+        <v>38</v>
+      </c>
+      <c r="E7" s="19">
+        <v>37</v>
+      </c>
+      <c r="F7" s="15">
+        <v>33</v>
+      </c>
+      <c r="G7" s="19">
+        <v>30</v>
+      </c>
+      <c r="H7" s="19">
         <v>30.975999999999999</v>
       </c>
-      <c r="J7" s="15">
+      <c r="I7" s="19">
         <v>32.58</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="15">
-        <v>0.189</v>
-      </c>
-      <c r="C8" s="15">
-        <v>4.5780000000000003</v>
-      </c>
-      <c r="D8" s="15">
-        <v>0.30399999999999999</v>
-      </c>
-      <c r="E8" s="15">
-        <v>0.52200000000000002</v>
-      </c>
-      <c r="F8" s="19"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15">
+      <c r="B8" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="C8" s="10">
+        <v>5.6</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0.37</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0.64</v>
+      </c>
+      <c r="F8" s="14">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G8" s="10">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="I8" s="15">
-        <v>0.89200000000000002</v>
-      </c>
-      <c r="J8" s="15">
-        <v>0.19400000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H8" s="10">
+        <v>1.07</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0.23</v>
+      </c>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10">
+        <f>D8/F8</f>
+        <v>2.6428571428571428</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="10">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="10">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="10">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15">
+      <c r="F9" s="15"/>
+      <c r="G9" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="I9" s="15">
+      <c r="H9" s="10">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="J9" s="15">
+      <c r="I9" s="10">
         <v>1.4E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="15">
-        <v>2E-3</v>
-      </c>
-      <c r="C10" s="15">
-        <v>1E-3</v>
-      </c>
-      <c r="D10" s="15">
-        <v>0.316</v>
-      </c>
-      <c r="E10" s="15">
-        <v>0.40799999999999997</v>
-      </c>
-      <c r="F10" s="19"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15">
-        <v>1E-3</v>
-      </c>
-      <c r="I10" s="15">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="J10" s="15">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="10">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0.85</v>
+      </c>
+      <c r="D10" s="10">
+        <v>136.5</v>
+      </c>
+      <c r="E10" s="10">
+        <v>96.6</v>
+      </c>
+      <c r="F10" s="15">
+        <f>3.21*1000</f>
+        <v>3210</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0.35</v>
+      </c>
+      <c r="H10" s="10">
+        <v>1.21</v>
+      </c>
+      <c r="I10" s="10">
+        <v>3.14</v>
+      </c>
+      <c r="L10" s="10">
+        <f>F10/D10</f>
+        <v>23.516483516483518</v>
+      </c>
+      <c r="M10" s="10"/>
+    </row>
+    <row r="11" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
       <c r="F11" s="16"/>
-      <c r="G11" s="14"/>
-    </row>
-    <row r="12" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="10" t="s">
+    </row>
+    <row r="12" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F12" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="10" t="s">
+      <c r="G12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="H12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="I12" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -2429,17 +2519,18 @@
       <c r="E13">
         <v>34.247</v>
       </c>
+      <c r="F13" s="15"/>
+      <c r="G13">
+        <v>4.1100000000000003</v>
+      </c>
       <c r="H13">
-        <v>4.1100000000000003</v>
+        <v>8.2189999999999994</v>
       </c>
       <c r="I13">
-        <v>8.2189999999999994</v>
-      </c>
-      <c r="J13">
         <v>5.4790000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2455,17 +2546,18 @@
       <c r="E14">
         <v>65.753</v>
       </c>
+      <c r="F14" s="15"/>
+      <c r="G14">
+        <v>95.89</v>
+      </c>
       <c r="H14">
-        <v>95.89</v>
+        <v>91.781000000000006</v>
       </c>
       <c r="I14">
-        <v>91.781000000000006</v>
-      </c>
-      <c r="J14">
         <v>94.521000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -2481,17 +2573,18 @@
       <c r="E15">
         <v>0</v>
       </c>
+      <c r="F15" s="15"/>
+      <c r="G15">
+        <v>0</v>
+      </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:13" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -2507,170 +2600,175 @@
       <c r="E16">
         <v>0</v>
       </c>
+      <c r="F16" s="15"/>
+      <c r="G16">
+        <v>0</v>
+      </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="15">
-        <v>2.4660000000000002</v>
-      </c>
-      <c r="C17" s="15">
-        <v>0</v>
-      </c>
-      <c r="D17" s="15">
-        <v>33.424999999999997</v>
-      </c>
-      <c r="E17" s="15">
-        <v>34.247</v>
-      </c>
-      <c r="F17" s="19">
-        <f>AVERAGE(0.14835165, 0.115384616, 0.27302632, 0.14673913)*100</f>
-        <v>17.087542900000003</v>
-      </c>
-      <c r="G17" s="15">
-        <v>22</v>
-      </c>
-      <c r="H17" s="15">
+      <c r="B17" s="19">
+        <v>2.0550000000000002</v>
+      </c>
+      <c r="C17" s="19">
+        <v>0</v>
+      </c>
+      <c r="D17" s="19">
+        <v>34</v>
+      </c>
+      <c r="E17" s="19">
+        <v>34</v>
+      </c>
+      <c r="F17" s="15">
+        <v>23</v>
+      </c>
+      <c r="G17" s="19">
         <v>4.1100000000000003</v>
       </c>
-      <c r="I17" s="15">
-        <v>8.2189999999999994</v>
-      </c>
-      <c r="J17" s="15">
+      <c r="H17" s="19">
+        <v>7</v>
+      </c>
+      <c r="I17" s="19">
         <v>5.4790000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="15">
-        <v>0.19700000000000001</v>
-      </c>
-      <c r="C18" s="15">
-        <v>7.149</v>
-      </c>
-      <c r="D18" s="15">
-        <v>3.1E-2</v>
-      </c>
-      <c r="E18" s="15">
-        <v>0.626</v>
-      </c>
-      <c r="F18" s="19"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15">
-        <v>0.11</v>
-      </c>
-      <c r="I18" s="15">
-        <v>2.222</v>
-      </c>
-      <c r="J18" s="15">
-        <v>0.30299999999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="10">
+        <v>0.21</v>
+      </c>
+      <c r="C18" s="10">
+        <v>8.83</v>
+      </c>
+      <c r="D18" s="10">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0.77</v>
+      </c>
+      <c r="F18" s="14">
+        <v>0.22</v>
+      </c>
+      <c r="G18" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="H18" s="10">
+        <v>2.7</v>
+      </c>
+      <c r="I18" s="10">
+        <v>0.36</v>
+      </c>
+      <c r="M18" s="10">
+        <f>D18/F18</f>
+        <v>0.17272727272727273</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="10">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="10">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="10">
         <v>0.23</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="10">
         <v>2E-3</v>
       </c>
-      <c r="F19" s="19"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15">
+      <c r="F19" s="15"/>
+      <c r="G19" s="10">
         <v>2E-3</v>
       </c>
-      <c r="I19" s="15">
+      <c r="H19" s="10">
         <v>0.16900000000000001</v>
       </c>
-      <c r="J19" s="15">
+      <c r="I19" s="10">
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="15">
-        <v>1E-3</v>
-      </c>
-      <c r="C20" s="15">
-        <v>1E-3</v>
-      </c>
-      <c r="D20" s="15">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="E20" s="15">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15">
-        <v>1E-3</v>
-      </c>
-      <c r="I20" s="15">
-        <v>0</v>
-      </c>
-      <c r="J20" s="15">
-        <v>6.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="C20" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D20" s="10">
+        <v>32.42</v>
+      </c>
+      <c r="E20" s="10">
+        <v>41.21</v>
+      </c>
+      <c r="F20" s="15">
+        <f>1.69*1000</f>
+        <v>1690</v>
+      </c>
+      <c r="G20" s="10">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H20" s="10">
+        <v>0.42</v>
+      </c>
+      <c r="I20" s="10">
+        <v>2.14</v>
+      </c>
+      <c r="L20" s="21">
+        <f>F20/D20</f>
+        <v>52.128315854410857</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C21" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B22" s="5" t="s">
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F22" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="5" t="s">
+      <c r="G22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="H22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J22" s="5" t="s">
+      <c r="I22" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -2686,17 +2784,18 @@
       <c r="E23">
         <v>59.12</v>
       </c>
+      <c r="F23" s="15"/>
+      <c r="G23">
+        <v>38.06</v>
+      </c>
       <c r="H23">
-        <v>38.06</v>
+        <v>47.38</v>
       </c>
       <c r="I23">
-        <v>47.38</v>
-      </c>
-      <c r="J23">
         <v>43.3</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -2712,17 +2811,18 @@
       <c r="E24">
         <v>40.880000000000003</v>
       </c>
+      <c r="F24" s="15"/>
+      <c r="G24">
+        <v>61.94</v>
+      </c>
       <c r="H24">
-        <v>61.94</v>
+        <v>52.62</v>
       </c>
       <c r="I24">
-        <v>52.62</v>
-      </c>
-      <c r="J24">
         <v>56.7</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -2738,17 +2838,18 @@
       <c r="E25">
         <v>0</v>
       </c>
+      <c r="F25" s="15"/>
+      <c r="G25">
+        <v>0</v>
+      </c>
       <c r="H25">
         <v>0</v>
       </c>
       <c r="I25">
         <v>0</v>
       </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -2764,170 +2865,175 @@
       <c r="E26">
         <v>0</v>
       </c>
+      <c r="F26" s="15"/>
+      <c r="G26">
+        <v>0</v>
+      </c>
       <c r="H26">
         <v>0</v>
       </c>
       <c r="I26">
         <v>0</v>
       </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B27" s="19">
         <v>55.08</v>
       </c>
-      <c r="C27" s="15">
-        <v>30.2</v>
-      </c>
-      <c r="D27" s="15">
+      <c r="C27" s="19">
+        <v>31</v>
+      </c>
+      <c r="D27" s="19">
         <v>59.08</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E27" s="19">
         <v>59.12</v>
       </c>
-      <c r="F27" s="19">
-        <f>AVERAGE(0.6488, 0.6176, 0.6176, 0.6416)*100</f>
-        <v>63.139999999999993</v>
-      </c>
-      <c r="G27" s="15">
+      <c r="F27" s="15">
         <v>64</v>
       </c>
-      <c r="H27" s="15">
+      <c r="G27" s="19">
         <v>38.06</v>
       </c>
-      <c r="I27" s="15">
-        <v>47.38</v>
-      </c>
-      <c r="J27" s="15">
+      <c r="H27" s="19">
+        <v>48</v>
+      </c>
+      <c r="I27" s="19">
         <v>43.3</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28" s="20">
         <v>2E-3</v>
       </c>
-      <c r="C28" s="15">
-        <v>4.4909999999999997</v>
-      </c>
-      <c r="D28" s="15">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="E28" s="15">
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="F28" s="19"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15">
+      <c r="C28" s="10">
+        <v>5.53</v>
+      </c>
+      <c r="D28" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="E28" s="10">
+        <v>0.17</v>
+      </c>
+      <c r="F28" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="G28" s="20">
         <v>2E-3</v>
       </c>
-      <c r="I28" s="15">
-        <v>0.372</v>
-      </c>
-      <c r="J28" s="15">
-        <v>0.111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H28" s="10">
+        <v>0.43</v>
+      </c>
+      <c r="I28" s="10">
+        <v>0.13</v>
+      </c>
+      <c r="M28" s="10">
+        <f>D28/F28</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="15">
+      <c r="B29" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29" s="10">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="D29" s="15">
+      <c r="D29" s="10">
         <v>3.1E-2</v>
       </c>
-      <c r="E29" s="15">
+      <c r="E29" s="10">
         <v>1E-3</v>
       </c>
-      <c r="F29" s="19"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15">
+      <c r="F29" s="15"/>
+      <c r="G29" s="10">
         <v>1E-3</v>
       </c>
-      <c r="I29" s="15">
+      <c r="H29" s="10">
         <v>0.03</v>
       </c>
-      <c r="J29" s="15">
+      <c r="I29" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="15">
-        <v>1E-3</v>
-      </c>
-      <c r="C30" s="15">
-        <v>1E-3</v>
-      </c>
-      <c r="D30" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="E30" s="15">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="F30" s="19"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15">
-        <v>0</v>
-      </c>
-      <c r="I30" s="15">
-        <v>2E-3</v>
-      </c>
-      <c r="J30" s="15">
-        <v>6.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C31" s="7" t="s">
+      <c r="B30" s="10">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C30" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D30" s="10">
+        <v>49.7</v>
+      </c>
+      <c r="E30" s="10">
+        <v>24.14</v>
+      </c>
+      <c r="F30" s="15">
+        <f>0.8*1000</f>
+        <v>800</v>
+      </c>
+      <c r="G30" s="10">
+        <v>0</v>
+      </c>
+      <c r="H30" s="10">
+        <v>0.64</v>
+      </c>
+      <c r="I30" s="10">
+        <v>3.07</v>
+      </c>
+      <c r="L30" s="10">
+        <f>F30/D30</f>
+        <v>16.096579476861166</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C31" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
       <c r="F31" s="16"/>
-      <c r="G31" s="8"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B32" s="5" t="s">
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B32" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F32" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="G32" s="4"/>
-      <c r="H32" s="5" t="s">
+      <c r="G32" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I32" s="5" t="s">
+      <c r="H32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J32" s="5" t="s">
+      <c r="I32" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -2943,17 +3049,18 @@
       <c r="E33">
         <v>26.513999999999999</v>
       </c>
+      <c r="F33" s="15"/>
+      <c r="G33">
+        <v>11.561</v>
+      </c>
       <c r="H33">
-        <v>11.561</v>
+        <v>31.068999999999999</v>
       </c>
       <c r="I33">
-        <v>31.068999999999999</v>
-      </c>
-      <c r="J33">
         <v>17.13</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -2969,17 +3076,18 @@
       <c r="E34">
         <v>73.486000000000004</v>
       </c>
+      <c r="F34" s="15"/>
+      <c r="G34">
+        <v>88.438999999999993</v>
+      </c>
       <c r="H34">
-        <v>88.438999999999993</v>
+        <v>68.930999999999997</v>
       </c>
       <c r="I34">
-        <v>68.930999999999997</v>
-      </c>
-      <c r="J34">
         <v>82.87</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -2995,17 +3103,18 @@
       <c r="E35">
         <v>7.6420000000000003</v>
       </c>
+      <c r="F35" s="15"/>
+      <c r="G35">
+        <v>1.804</v>
+      </c>
       <c r="H35">
         <v>1.804</v>
       </c>
       <c r="I35">
-        <v>1.804</v>
-      </c>
-      <c r="J35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -3021,170 +3130,175 @@
       <c r="E36">
         <v>0</v>
       </c>
+      <c r="F36" s="15"/>
+      <c r="G36">
+        <v>0</v>
+      </c>
       <c r="H36">
         <v>0</v>
       </c>
       <c r="I36">
         <v>0</v>
       </c>
-      <c r="J36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="15">
+      <c r="B37" s="19">
         <v>5.6959999999999997</v>
       </c>
-      <c r="C37" s="15">
-        <v>21.507999999999999</v>
-      </c>
-      <c r="D37" s="15">
-        <v>20.9</v>
-      </c>
-      <c r="E37" s="15">
+      <c r="C37" s="19">
+        <v>23</v>
+      </c>
+      <c r="D37" s="19">
+        <v>22</v>
+      </c>
+      <c r="E37" s="19">
         <v>24.488</v>
       </c>
-      <c r="F37" s="19">
-        <f>AVERAGE(0.11678832, 0.12895377, 0.12489862,  0.1337115)*100</f>
-        <v>12.60880525</v>
-      </c>
-      <c r="G37" s="15">
+      <c r="F37" s="15">
         <v>29</v>
       </c>
-      <c r="H37" s="15">
+      <c r="G37" s="19">
         <v>11.352</v>
       </c>
-      <c r="I37" s="15">
-        <v>30.509</v>
-      </c>
-      <c r="J37" s="15">
-        <v>17.13</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H37" s="19">
+        <v>32</v>
+      </c>
+      <c r="I37" s="19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>20</v>
       </c>
-      <c r="B38" s="15">
-        <v>0.80600000000000005</v>
-      </c>
-      <c r="C38" s="15">
-        <v>9.641</v>
-      </c>
-      <c r="D38" s="15">
-        <v>1.288</v>
-      </c>
-      <c r="E38" s="15">
-        <v>1.4430000000000001</v>
-      </c>
-      <c r="F38" s="19"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15">
-        <v>0.23400000000000001</v>
-      </c>
-      <c r="I38" s="15">
-        <v>2.6440000000000001</v>
-      </c>
-      <c r="J38" s="15">
-        <v>0.434</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="10">
+        <v>0.93</v>
+      </c>
+      <c r="C38" s="10">
+        <v>11.9</v>
+      </c>
+      <c r="D38" s="10">
+        <v>1.7</v>
+      </c>
+      <c r="E38" s="10">
+        <v>1.95</v>
+      </c>
+      <c r="F38" s="14">
+        <v>0.26</v>
+      </c>
+      <c r="G38" s="10">
+        <v>0.26</v>
+      </c>
+      <c r="H38" s="10">
+        <v>3.19</v>
+      </c>
+      <c r="I38" s="10">
+        <v>0.52</v>
+      </c>
+      <c r="M38" s="10">
+        <f>D38/F38</f>
+        <v>6.5384615384615383</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="15">
+      <c r="B39" s="10">
         <v>0.13400000000000001</v>
       </c>
-      <c r="C39" s="15">
+      <c r="C39" s="10">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="D39" s="15">
+      <c r="D39" s="10">
         <v>0.251</v>
       </c>
-      <c r="E39" s="15">
+      <c r="E39" s="10">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="F39" s="19"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="15">
+      <c r="F39" s="15"/>
+      <c r="G39" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="I39" s="15">
+      <c r="H39" s="10">
         <v>0.11700000000000001</v>
       </c>
-      <c r="J39" s="15">
+      <c r="I39" s="10">
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="15">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C40" s="15">
-        <v>1E-3</v>
-      </c>
-      <c r="D40" s="15">
-        <v>0.192</v>
-      </c>
-      <c r="E40" s="15">
-        <v>0.02</v>
-      </c>
-      <c r="F40" s="19"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="I40" s="15">
-        <v>2E-3</v>
-      </c>
-      <c r="J40" s="15">
-        <v>0.09</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C41" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="10">
+        <v>2.35</v>
+      </c>
+      <c r="C40" s="10">
+        <v>0.42</v>
+      </c>
+      <c r="D40" s="10">
+        <v>69.42</v>
+      </c>
+      <c r="E40" s="10">
+        <v>7.07</v>
+      </c>
+      <c r="F40" s="15">
+        <f>0.59*1000</f>
+        <v>590</v>
+      </c>
+      <c r="G40" s="10">
+        <v>1.07</v>
+      </c>
+      <c r="H40" s="10">
+        <v>0.92</v>
+      </c>
+      <c r="I40" s="10">
+        <v>17.920000000000002</v>
+      </c>
+      <c r="L40" s="10">
+        <f>F40/D40</f>
+        <v>8.4989916450590606</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C41" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
       <c r="F41" s="16"/>
-      <c r="G41" s="8"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B42" s="5" t="s">
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B42" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E42" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F42" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="G42" s="4"/>
-      <c r="H42" s="5" t="s">
+      <c r="G42" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I42" s="5" t="s">
+      <c r="H42" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J42" s="5" t="s">
+      <c r="I42" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -3200,17 +3314,18 @@
       <c r="E43">
         <v>80.56</v>
       </c>
+      <c r="F43" s="15"/>
+      <c r="G43">
+        <v>16.12</v>
+      </c>
       <c r="H43">
-        <v>16.12</v>
+        <v>80.599999999999994</v>
       </c>
       <c r="I43">
-        <v>80.599999999999994</v>
-      </c>
-      <c r="J43">
         <v>64.239999999999995</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -3226,17 +3341,18 @@
       <c r="E44">
         <v>19.440000000000001</v>
       </c>
+      <c r="F44" s="15"/>
+      <c r="G44">
+        <v>83.88</v>
+      </c>
       <c r="H44">
-        <v>83.88</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="I44">
-        <v>19.399999999999999</v>
-      </c>
-      <c r="J44">
         <v>35.76</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>18</v>
       </c>
@@ -3252,17 +3368,18 @@
       <c r="E45">
         <v>0</v>
       </c>
+      <c r="F45" s="15"/>
+      <c r="G45">
+        <v>0</v>
+      </c>
       <c r="H45">
         <v>0</v>
       </c>
       <c r="I45">
         <v>0</v>
       </c>
-      <c r="J45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>19</v>
       </c>
@@ -3278,170 +3395,175 @@
       <c r="E46">
         <v>0</v>
       </c>
+      <c r="F46" s="15"/>
+      <c r="G46">
+        <v>0</v>
+      </c>
       <c r="H46">
         <v>0</v>
       </c>
       <c r="I46">
         <v>0</v>
       </c>
-      <c r="J46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>23</v>
       </c>
-      <c r="B47" s="15">
+      <c r="B47" s="19">
         <v>3.46</v>
       </c>
-      <c r="C47" s="15">
-        <v>78.22</v>
-      </c>
-      <c r="D47" s="15">
+      <c r="C47" s="19">
+        <v>79</v>
+      </c>
+      <c r="D47" s="19">
         <v>80.400000000000006</v>
       </c>
-      <c r="E47" s="15">
-        <v>80.56</v>
-      </c>
-      <c r="F47" s="19">
-        <f>AVERAGE(0.6072, 0.6336, 0.628, 0.6376)*100</f>
-        <v>62.660000000000004</v>
-      </c>
-      <c r="G47" s="15">
-        <v>62</v>
-      </c>
-      <c r="H47" s="15">
+      <c r="E47" s="19">
+        <v>80</v>
+      </c>
+      <c r="F47" s="15">
+        <v>88</v>
+      </c>
+      <c r="G47" s="19">
         <v>16.12</v>
       </c>
-      <c r="I47" s="15">
+      <c r="H47" s="19">
         <v>80.599999999999994</v>
       </c>
-      <c r="J47" s="15">
-        <v>64.239999999999995</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I47" s="19">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>20</v>
       </c>
-      <c r="B48" s="15">
+      <c r="B48" s="10">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="C48" s="15">
-        <v>70.34</v>
-      </c>
-      <c r="D48" s="15">
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="E48" s="15">
-        <v>0.18</v>
-      </c>
-      <c r="F48" s="19"/>
-      <c r="G48" s="15"/>
-      <c r="H48" s="15">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="I48" s="15">
-        <v>1.5329999999999999</v>
-      </c>
-      <c r="J48" s="15">
-        <v>1.157</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C48" s="10">
+        <v>87.4</v>
+      </c>
+      <c r="D48" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="E48" s="10">
+        <v>0.21</v>
+      </c>
+      <c r="F48" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="G48" s="10">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="H48" s="10">
+        <v>1.68</v>
+      </c>
+      <c r="I48" s="10">
+        <v>1.39</v>
+      </c>
+      <c r="M48" s="10">
+        <f>D48/F48</f>
+        <v>0.73333333333333339</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>21</v>
       </c>
-      <c r="B49" s="15">
+      <c r="B49" s="10">
         <v>0.13100000000000001</v>
       </c>
-      <c r="C49" s="15">
+      <c r="C49" s="10">
         <v>0.31900000000000001</v>
       </c>
-      <c r="D49" s="15">
+      <c r="D49" s="10">
         <v>0.315</v>
       </c>
-      <c r="E49" s="15">
+      <c r="E49" s="10">
         <v>2E-3</v>
       </c>
-      <c r="F49" s="19"/>
-      <c r="G49" s="15"/>
-      <c r="H49" s="15">
+      <c r="F49" s="15"/>
+      <c r="G49" s="10">
         <v>1.6E-2</v>
       </c>
-      <c r="I49" s="15">
+      <c r="H49" s="10">
         <v>0.71699999999999997</v>
       </c>
-      <c r="J49" s="15">
+      <c r="I49" s="10">
         <v>0.158</v>
       </c>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>0</v>
       </c>
-      <c r="B50" s="15">
-        <v>1E-3</v>
-      </c>
-      <c r="C50" s="15">
-        <v>1E-3</v>
-      </c>
-      <c r="D50" s="15">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="E50" s="15">
-        <v>1.9E-2</v>
-      </c>
-      <c r="F50" s="19"/>
-      <c r="G50" s="15"/>
-      <c r="H50" s="15">
-        <v>0</v>
-      </c>
-      <c r="I50" s="15">
-        <v>1E-3</v>
-      </c>
-      <c r="J50" s="15">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C51" s="7" t="s">
+      <c r="B50" s="10">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C50" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D50" s="10">
+        <v>15.7</v>
+      </c>
+      <c r="E50" s="10">
+        <v>7.35</v>
+      </c>
+      <c r="F50" s="15">
+        <f>0.43*1000</f>
+        <v>430</v>
+      </c>
+      <c r="G50" s="10">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H50" s="10">
+        <v>0.21</v>
+      </c>
+      <c r="I50" s="10">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="L50" s="10">
+        <f>F50/D50</f>
+        <v>27.388535031847134</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C51" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
       <c r="F51" s="16"/>
-      <c r="G51" s="8"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B52" s="5" t="s">
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B52" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D52" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E52" s="5" t="s">
+      <c r="E52" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F52" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="G52" s="4"/>
-      <c r="H52" s="5" t="s">
+      <c r="G52" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I52" s="5" t="s">
+      <c r="H52" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J52" s="5" t="s">
+      <c r="I52" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>16</v>
       </c>
@@ -3457,17 +3579,18 @@
       <c r="E53">
         <v>36.713999999999999</v>
       </c>
+      <c r="F53" s="15"/>
+      <c r="G53">
+        <v>25.684999999999999</v>
+      </c>
       <c r="H53">
-        <v>25.684999999999999</v>
+        <v>22.35</v>
       </c>
       <c r="I53">
-        <v>22.35</v>
-      </c>
-      <c r="J53">
         <v>24.228999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>17</v>
       </c>
@@ -3483,17 +3606,18 @@
       <c r="E54">
         <v>63.286000000000001</v>
       </c>
+      <c r="F54" s="15"/>
+      <c r="G54">
+        <v>74.314999999999998</v>
+      </c>
       <c r="H54">
-        <v>74.314999999999998</v>
+        <v>77.650000000000006</v>
       </c>
       <c r="I54">
-        <v>77.650000000000006</v>
-      </c>
-      <c r="J54">
         <v>75.771000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>18</v>
       </c>
@@ -3509,17 +3633,18 @@
       <c r="E55">
         <v>0.49099999999999999</v>
       </c>
+      <c r="F55" s="15"/>
+      <c r="G55">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="H55">
         <v>1.1000000000000001</v>
       </c>
       <c r="I55">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>19</v>
       </c>
@@ -3535,170 +3660,175 @@
       <c r="E56">
         <v>0</v>
       </c>
+      <c r="F56" s="15"/>
+      <c r="G56">
+        <v>0</v>
+      </c>
       <c r="H56">
         <v>0</v>
       </c>
       <c r="I56">
         <v>0</v>
       </c>
-      <c r="J56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>23</v>
       </c>
-      <c r="B57" s="15">
-        <v>31.838000000000001</v>
-      </c>
-      <c r="C57" s="15">
-        <v>1.889</v>
-      </c>
-      <c r="D57" s="15">
-        <v>41.273000000000003</v>
-      </c>
-      <c r="E57" s="15">
-        <v>36.533000000000001</v>
-      </c>
-      <c r="F57" s="19">
-        <f>AVERAGE(0.26124445, 0.02551111, 0.022844445, 0.0077333334)*100</f>
-        <v>7.9333334600000001</v>
-      </c>
-      <c r="G57" s="15">
-        <v>28</v>
-      </c>
-      <c r="H57" s="15">
-        <v>25.402000000000001</v>
-      </c>
-      <c r="I57" s="15">
-        <v>22.103999999999999</v>
-      </c>
-      <c r="J57" s="15">
-        <v>24.228999999999999</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="19">
+        <v>30</v>
+      </c>
+      <c r="C57" s="19">
+        <v>1</v>
+      </c>
+      <c r="D57" s="19">
+        <v>37</v>
+      </c>
+      <c r="E57" s="19">
+        <v>29</v>
+      </c>
+      <c r="F57" s="15">
+        <v>34</v>
+      </c>
+      <c r="G57" s="19">
+        <v>23</v>
+      </c>
+      <c r="H57" s="19">
+        <v>20</v>
+      </c>
+      <c r="I57" s="19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>20</v>
       </c>
-      <c r="B58" s="15">
-        <v>7.2290000000000001</v>
-      </c>
-      <c r="C58" s="15">
-        <v>125.218</v>
-      </c>
-      <c r="D58" s="15">
-        <v>75.524000000000001</v>
-      </c>
-      <c r="E58" s="15">
-        <v>80.423000000000002</v>
-      </c>
-      <c r="F58" s="19"/>
-      <c r="G58" s="15"/>
-      <c r="H58" s="15">
-        <v>1.974</v>
-      </c>
-      <c r="I58" s="15">
-        <v>31.009</v>
-      </c>
-      <c r="J58" s="15">
-        <v>4.9109999999999996</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="10">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="C58" s="10">
+        <v>155.87</v>
+      </c>
+      <c r="D58" s="10">
+        <v>100.08</v>
+      </c>
+      <c r="E58" s="10">
+        <v>106.14</v>
+      </c>
+      <c r="F58" s="14">
+        <v>2.25</v>
+      </c>
+      <c r="G58" s="10">
+        <v>26</v>
+      </c>
+      <c r="H58" s="10">
+        <v>37.6</v>
+      </c>
+      <c r="I58" s="10">
+        <v>5.97</v>
+      </c>
+      <c r="M58" s="10">
+        <f>D58/F58</f>
+        <v>44.48</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>21</v>
       </c>
-      <c r="B59" s="15">
+      <c r="B59" s="10">
         <v>5.843</v>
       </c>
-      <c r="C59" s="15">
+      <c r="C59" s="10">
         <v>1.6910000000000001</v>
       </c>
-      <c r="D59" s="15">
+      <c r="D59" s="10">
         <v>12.717000000000001</v>
       </c>
-      <c r="E59" s="15">
+      <c r="E59" s="10">
         <v>0.45500000000000002</v>
       </c>
-      <c r="F59" s="19"/>
-      <c r="G59" s="15"/>
-      <c r="H59" s="15">
+      <c r="F59" s="15"/>
+      <c r="G59" s="10">
         <v>0.16300000000000001</v>
       </c>
-      <c r="I59" s="15">
+      <c r="H59" s="10">
         <v>2.38</v>
       </c>
-      <c r="J59" s="15">
+      <c r="I59" s="10">
         <v>0.40400000000000003</v>
       </c>
     </row>
-    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>0</v>
       </c>
-      <c r="B60" s="15">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="C60" s="15">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="D60" s="15">
-        <v>20.097000000000001</v>
-      </c>
-      <c r="E60" s="15">
-        <v>17.048999999999999</v>
-      </c>
-      <c r="F60" s="19"/>
-      <c r="G60" s="15"/>
-      <c r="H60" s="15">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="I60" s="15">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="J60" s="15">
-        <v>1.2130000000000001</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C61" s="7" t="s">
+      <c r="B60" s="10">
+        <v>25</v>
+      </c>
+      <c r="C60" s="10">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="D60" s="10">
+        <v>5990</v>
+      </c>
+      <c r="E60" s="10">
+        <v>5897</v>
+      </c>
+      <c r="F60" s="15">
+        <f>344*1000</f>
+        <v>344000</v>
+      </c>
+      <c r="G60" s="10">
+        <v>23.92</v>
+      </c>
+      <c r="H60" s="10">
+        <v>9.92</v>
+      </c>
+      <c r="I60" s="10">
+        <v>434</v>
+      </c>
+      <c r="L60" s="10">
+        <f>F60/D60</f>
+        <v>57.42904841402337</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C61" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
       <c r="F61" s="16"/>
-      <c r="G61" s="8"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B62" s="5" t="s">
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B62" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E62" s="5" t="s">
+      <c r="E62" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F62" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="G62" s="4"/>
-      <c r="H62" s="5" t="s">
+      <c r="G62" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I62" s="5" t="s">
+      <c r="H62" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J62" s="5" t="s">
+      <c r="I62" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>16</v>
       </c>
@@ -3714,17 +3844,18 @@
       <c r="E63">
         <v>34.033999999999999</v>
       </c>
+      <c r="F63" s="15"/>
+      <c r="G63">
+        <v>23.254000000000001</v>
+      </c>
       <c r="H63">
-        <v>23.254000000000001</v>
+        <v>26.04</v>
       </c>
       <c r="I63">
-        <v>26.04</v>
-      </c>
-      <c r="J63">
         <v>24.026</v>
       </c>
     </row>
-    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>17</v>
       </c>
@@ -3740,17 +3871,18 @@
       <c r="E64">
         <v>65.965999999999994</v>
       </c>
+      <c r="F64" s="15"/>
+      <c r="G64">
+        <v>76.745999999999995</v>
+      </c>
       <c r="H64">
-        <v>76.745999999999995</v>
+        <v>73.959999999999994</v>
       </c>
       <c r="I64">
-        <v>73.959999999999994</v>
-      </c>
-      <c r="J64">
         <v>75.974000000000004</v>
       </c>
     </row>
-    <row r="65" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>18</v>
       </c>
@@ -3766,17 +3898,18 @@
       <c r="E65">
         <v>0.74</v>
       </c>
+      <c r="F65" s="15"/>
+      <c r="G65">
+        <v>0.56000000000000005</v>
+      </c>
       <c r="H65">
         <v>0.56000000000000005</v>
       </c>
       <c r="I65">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="J65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>19</v>
       </c>
@@ -3792,195 +3925,260 @@
       <c r="E66">
         <v>0.36</v>
       </c>
+      <c r="F66" s="15"/>
+      <c r="G66">
+        <v>0.36</v>
+      </c>
       <c r="H66">
         <v>0.36</v>
       </c>
       <c r="I66">
         <v>0.36</v>
       </c>
-      <c r="J66">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>23</v>
       </c>
-      <c r="B67" s="15">
+      <c r="B67" s="19">
         <v>24.7</v>
       </c>
-      <c r="C67" s="15">
+      <c r="C67" s="19">
         <v>6.98</v>
       </c>
-      <c r="D67" s="15">
+      <c r="D67" s="19">
         <v>34</v>
       </c>
-      <c r="E67" s="15">
+      <c r="E67" s="19">
         <v>33.659999999999997</v>
       </c>
-      <c r="F67" s="19">
-        <f>AVERAGE(0.24819277, 0.24196142, 0.25120386, 0.25260624)*100</f>
-        <v>24.849107250000003</v>
-      </c>
-      <c r="G67" s="15">
+      <c r="F67" s="15">
         <v>29</v>
       </c>
-      <c r="H67" s="15">
+      <c r="G67" s="19">
         <v>23.04</v>
       </c>
-      <c r="I67" s="15">
+      <c r="H67" s="19">
         <v>25.8</v>
       </c>
-      <c r="J67" s="15">
-        <v>23.94</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I67" s="19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>20</v>
       </c>
-      <c r="B68" s="15">
-        <v>0.73799999999999999</v>
-      </c>
-      <c r="C68" s="15">
-        <v>20.472999999999999</v>
-      </c>
-      <c r="D68" s="15">
-        <v>1.042</v>
-      </c>
-      <c r="E68" s="15">
-        <v>1.4370000000000001</v>
-      </c>
-      <c r="F68" s="19"/>
-      <c r="G68" s="15"/>
-      <c r="H68" s="15">
-        <v>0.28799999999999998</v>
-      </c>
-      <c r="I68" s="15">
-        <v>5.4189999999999996</v>
-      </c>
-      <c r="J68" s="15">
-        <v>0.83199999999999996</v>
-      </c>
-    </row>
-    <row r="69" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="C68" s="10">
+        <v>25.28</v>
+      </c>
+      <c r="D68" s="10">
+        <v>1.36</v>
+      </c>
+      <c r="E68" s="10">
+        <v>1.85</v>
+      </c>
+      <c r="F68" s="14">
+        <v>0.61</v>
+      </c>
+      <c r="G68" s="10">
+        <v>0.32</v>
+      </c>
+      <c r="H68" s="10">
+        <v>6.52</v>
+      </c>
+      <c r="I68" s="10">
+        <v>1</v>
+      </c>
+      <c r="M68" s="10">
+        <f>D68/F68</f>
+        <v>2.2295081967213117</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>21</v>
       </c>
-      <c r="B69" s="15">
+      <c r="B69" s="10">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="C69" s="15">
+      <c r="C69" s="10">
         <v>0.24299999999999999</v>
       </c>
-      <c r="D69" s="15">
+      <c r="D69" s="10">
         <v>0.48599999999999999</v>
       </c>
-      <c r="E69" s="15">
+      <c r="E69" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F69" s="19"/>
-      <c r="G69" s="15"/>
-      <c r="H69" s="15">
+      <c r="F69" s="14"/>
+      <c r="G69" s="10">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="I69" s="15">
+      <c r="H69" s="10">
         <v>0.27400000000000002</v>
       </c>
-      <c r="J69" s="15">
+      <c r="I69" s="10">
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>0</v>
       </c>
-      <c r="B70" s="15">
-        <v>2E-3</v>
-      </c>
-      <c r="C70" s="15">
-        <v>2E-3</v>
-      </c>
-      <c r="D70" s="15">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="E70" s="15">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="F70" s="19"/>
-      <c r="G70" s="15"/>
-      <c r="H70" s="15">
-        <v>2E-3</v>
-      </c>
-      <c r="I70" s="15">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="J70" s="15">
-        <v>1.7000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R71" s="1"/>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R72" s="1"/>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R73" s="1"/>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R74" s="1"/>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R75" s="1"/>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R76" s="1"/>
-    </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R77" s="1"/>
-    </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R78" s="1"/>
-    </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R79" s="1"/>
-    </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R80" s="1"/>
-    </row>
-    <row r="81" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R81" s="1"/>
-    </row>
-    <row r="82" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R82" s="1"/>
-    </row>
-    <row r="83" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R83" s="1"/>
-    </row>
-    <row r="84" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R84" s="1"/>
-    </row>
-    <row r="85" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R85" s="1"/>
-    </row>
-    <row r="86" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R86" s="1"/>
-    </row>
-    <row r="87" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R87" s="1"/>
-    </row>
-    <row r="88" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R88" s="1"/>
-    </row>
-    <row r="89" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R89" s="1"/>
-    </row>
-    <row r="90" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R90" s="1"/>
-    </row>
-    <row r="91" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R91" s="1"/>
+      <c r="B70" s="10">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="C70" s="10">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D70" s="10">
+        <v>65.209999999999994</v>
+      </c>
+      <c r="E70" s="10">
+        <v>15</v>
+      </c>
+      <c r="F70" s="14">
+        <f>6.75*1000</f>
+        <v>6750</v>
+      </c>
+      <c r="G70" s="10">
+        <v>0.78</v>
+      </c>
+      <c r="H70" s="10">
+        <v>1</v>
+      </c>
+      <c r="I70" s="10">
+        <v>7.21</v>
+      </c>
+      <c r="L70" s="10">
+        <f>F70/D70</f>
+        <v>103.5117313295507</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q71" s="1"/>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q72" s="1"/>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q73" s="1"/>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q74" s="1"/>
+    </row>
+    <row r="75" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C75" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q75" s="22"/>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D76" t="s">
+        <v>28</v>
+      </c>
+      <c r="G76" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q76" s="1"/>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D77">
+        <v>26</v>
+      </c>
+      <c r="E77" t="s">
+        <v>37</v>
+      </c>
+      <c r="G77">
+        <v>625</v>
+      </c>
+      <c r="H77" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q77" s="1"/>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D78">
+        <v>64</v>
+      </c>
+      <c r="E78" t="s">
+        <v>36</v>
+      </c>
+      <c r="G78">
+        <v>122</v>
+      </c>
+      <c r="H78" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q78" s="1"/>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D79">
+        <f>12*8*8</f>
+        <v>768</v>
+      </c>
+      <c r="E79" t="s">
+        <v>35</v>
+      </c>
+      <c r="G79">
+        <f>32+26*4*8</f>
+        <v>864</v>
+      </c>
+      <c r="H79" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q79" s="1"/>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C80" t="s">
+        <v>29</v>
+      </c>
+      <c r="D80" s="3">
+        <f>D77+D78+D79</f>
+        <v>858</v>
+      </c>
+      <c r="G80" s="3">
+        <f>G77+G78+G79</f>
+        <v>1611</v>
+      </c>
+      <c r="Q80" s="1"/>
+    </row>
+    <row r="81" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q81" s="1"/>
+    </row>
+    <row r="82" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q82" s="1"/>
+    </row>
+    <row r="83" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q83" s="1"/>
+    </row>
+    <row r="84" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q84" s="1"/>
+    </row>
+    <row r="85" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q85" s="1"/>
+    </row>
+    <row r="86" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q86" s="1"/>
+    </row>
+    <row r="87" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q87" s="1"/>
+    </row>
+    <row r="88" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q88" s="1"/>
+    </row>
+    <row r="89" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q89" s="1"/>
+    </row>
+    <row r="90" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q90" s="1"/>
+    </row>
+    <row r="91" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q91" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Spreadsheet now contains data from performance results
</commit_message>
<xml_diff>
--- a/sbp-accuracy-other-predictors.xlsx
+++ b/sbp-accuracy-other-predictors.xlsx
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="38">
-  <si>
-    <t>Test Time</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="50">
   <si>
     <t>subSeq</t>
   </si>
@@ -142,13 +139,53 @@
   <si>
     <t>II</t>
   </si>
+  <si>
+    <t>SPiCe (Spectral Learning Baseline)</t>
+  </si>
+  <si>
+    <t>SPICE</t>
+  </si>
+  <si>
+    <t>subSeq / Binary Size</t>
+  </si>
+  <si>
+    <t>CPT+ / Binary Size</t>
+  </si>
+  <si>
+    <t>Dataset Length **</t>
+  </si>
+  <si>
+    <t>Alphabet Size **</t>
+  </si>
+  <si>
+    <t>Number of Sequencies **</t>
+  </si>
+  <si>
+    <t>Number of Queries **</t>
+  </si>
+  <si>
+    <t>Average Query Length **</t>
+  </si>
+  <si>
+    <t>Binary Size (MB) **</t>
+  </si>
+  <si>
+    <t>** Every Dataset was split into 14 folds. The above stats correspond to the average stats of one fold</t>
+  </si>
+  <si>
+    <t>Average Sequence Length **</t>
+  </si>
+  <si>
+    <t>CPT+ in this case only stores the last 8 items of every training sequence. On the other hand subSeq stores the whole 133 items of a sequence</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -190,7 +227,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,6 +246,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -219,7 +262,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="821">
+  <cellStyleXfs count="911">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1041,8 +1084,98 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1062,15 +1195,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -1088,8 +1212,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="821">
+  <cellStyles count="911">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1500,6 +1638,51 @@
     <cellStyle name="Followed Hyperlink" xfId="816" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="818" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="820" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="822" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="824" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="826" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="828" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="830" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="832" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="834" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="836" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="838" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="840" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="842" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="844" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="846" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="848" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="850" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="852" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="854" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="856" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="858" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="860" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="862" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="864" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="866" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="868" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="870" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="872" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="874" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="876" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="878" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="880" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="882" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="884" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="886" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="888" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="890" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="892" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="894" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="896" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="898" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="900" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="902" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="904" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="906" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="908" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="910" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1910,6 +2093,51 @@
     <cellStyle name="Hyperlink" xfId="815" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="817" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="819" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="821" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="823" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="825" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="827" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="829" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="831" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="833" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="835" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="837" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="839" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="841" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="843" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="845" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="847" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="849" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="851" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="853" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="855" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="857" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="859" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="861" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="863" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="865" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="867" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="869" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="871" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="873" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="875" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="877" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="879" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="881" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="883" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="885" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="887" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="889" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="891" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="893" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="895" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="897" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="899" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="901" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="903" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="905" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="907" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="909" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1920,6 +2148,1043 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Predictors</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Memory</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> / Binary Size</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0915563996336103"/>
+          <c:y val="0.13178002894356"/>
+          <c:w val="0.640876814090875"/>
+          <c:h val="0.805417459575874"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$X$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>subSeq / Binary Size</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>(Sheet1!$X$10,Sheet1!$X$20,Sheet1!$X$30,Sheet1!$X$40,Sheet1!$X$50,Sheet1!$X$60,Sheet1!$X$70)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.295081967213115</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.098591549295775</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.847953216374269</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.625</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.277777777777778</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.978260869565217</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.178571428571428</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Y$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CPT+ / Binary Size</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>(Sheet1!$Y$10,Sheet1!$Y$20,Sheet1!$Y$30,Sheet1!$Y$40,Sheet1!$Y$50,Sheet1!$Y$60,Sheet1!$Y$70)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.065573770491803</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.535211267605634</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.923976608187134</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.625</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.203703703703704</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43.51304347826087</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.857142857142857</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="27384768"/>
+        <c:axId val="-42929616"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="27384768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-42929616"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-42929616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="27384768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2185,62 +3450,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q91"/>
+  <dimension ref="A1:Y91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
+      <selection activeCell="O70" sqref="O70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="5"/>
-    <col min="17" max="17" width="117.6640625" customWidth="1"/>
+    <col min="6" max="7" width="10.83203125" style="5"/>
+    <col min="19" max="19" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+    <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
       <c r="F1" s="9"/>
-    </row>
-    <row r="2" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+      <c r="G1" s="20"/>
+    </row>
+    <row r="2" spans="1:25" ht="64" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="F2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>36.115000000000002</v>
@@ -2254,19 +3550,19 @@
       <c r="E3">
         <v>36.186</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>31.343</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>31.033999999999999</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>32.58</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>63.884999999999998</v>
@@ -2280,19 +3576,19 @@
       <c r="E4">
         <v>63.814</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>68.656999999999996</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>68.965999999999994</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>67.42</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -2306,74 +3602,77 @@
       <c r="E5">
         <v>0.308</v>
       </c>
-      <c r="G5">
-        <v>0.185</v>
-      </c>
       <c r="H5">
         <v>0.185</v>
       </c>
       <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.185</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="16">
+        <v>36.115000000000002</v>
+      </c>
+      <c r="C7" s="16">
+        <v>6.68</v>
+      </c>
+      <c r="D7" s="16">
+        <v>38</v>
+      </c>
+      <c r="E7" s="16">
+        <v>37</v>
+      </c>
+      <c r="F7" s="12">
+        <v>33</v>
+      </c>
+      <c r="G7" s="11">
+        <v>0.19</v>
+      </c>
+      <c r="H7" s="16">
+        <v>30</v>
+      </c>
+      <c r="I7" s="16">
+        <v>30.975999999999999</v>
+      </c>
+      <c r="J7" s="16">
+        <v>32.58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>19</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="19">
-        <v>36.115000000000002</v>
-      </c>
-      <c r="C7" s="19">
-        <v>6.68</v>
-      </c>
-      <c r="D7" s="19">
-        <v>38</v>
-      </c>
-      <c r="E7" s="19">
-        <v>37</v>
-      </c>
-      <c r="F7" s="15">
-        <v>33</v>
-      </c>
-      <c r="G7" s="19">
-        <v>30</v>
-      </c>
-      <c r="H7" s="19">
-        <v>30.975999999999999</v>
-      </c>
-      <c r="I7" s="19">
-        <v>32.58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>20</v>
       </c>
       <c r="B8" s="10">
         <v>0.2</v>
@@ -2387,27 +3686,28 @@
       <c r="E8" s="10">
         <v>0.64</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="11">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="24"/>
+      <c r="H8" s="10">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="H8" s="10">
+      <c r="I8" s="10">
         <v>1.07</v>
       </c>
-      <c r="I8" s="10">
+      <c r="J8" s="10">
         <v>0.23</v>
       </c>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10">
+      <c r="M8" s="10"/>
+      <c r="N8" s="10">
         <f>D8/F8</f>
         <v>2.6428571428571428</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="10">
         <v>1.4999999999999999E-2</v>
@@ -2421,22 +3721,23 @@
       <c r="E9" s="10">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="10">
+      <c r="F9" s="12"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H9" s="10">
+      <c r="I9" s="10">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="I9" s="10">
+      <c r="J9" s="10">
         <v>1.4E-2</v>
       </c>
-      <c r="L9" s="10"/>
       <c r="M9" s="10"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9" s="10"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="10">
         <v>1.1399999999999999</v>
@@ -2450,68 +3751,105 @@
       <c r="E10" s="10">
         <v>96.6</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="12">
         <f>3.21*1000</f>
         <v>3210</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="12">
+        <f>370.903*1000</f>
+        <v>370903</v>
+      </c>
+      <c r="H10" s="10">
         <v>0.35</v>
       </c>
-      <c r="H10" s="10">
+      <c r="I10" s="10">
         <v>1.21</v>
       </c>
-      <c r="I10" s="10">
+      <c r="J10" s="10">
         <v>3.14</v>
       </c>
-      <c r="L10" s="10">
+      <c r="M10" s="10">
         <f>F10/D10</f>
         <v>23.516483516483518</v>
       </c>
-      <c r="M10" s="10"/>
-    </row>
-    <row r="11" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="16"/>
-    </row>
-    <row r="12" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N10" s="10"/>
+      <c r="P10">
+        <v>54979</v>
+      </c>
+      <c r="Q10">
+        <v>12</v>
+      </c>
+      <c r="R10">
+        <v>494</v>
+      </c>
+      <c r="S10">
+        <v>4518</v>
+      </c>
+      <c r="T10">
+        <v>347</v>
+      </c>
+      <c r="U10">
+        <v>5</v>
+      </c>
+      <c r="V10">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="X10" s="10">
+        <f>F8/V10</f>
+        <v>2.2950819672131151</v>
+      </c>
+      <c r="Y10" s="10">
+        <f>D8/V10</f>
+        <v>6.0655737704918034</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+    </row>
+    <row r="12" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="F12" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12" s="6" t="s">
+      <c r="I12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="J12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>4.0090000000000003</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13">
         <v>33.563000000000002</v>
@@ -2519,26 +3857,27 @@
       <c r="E13">
         <v>34.247</v>
       </c>
-      <c r="F13" s="15"/>
-      <c r="G13">
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13">
         <v>4.1100000000000003</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>8.2189999999999994</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>5.4790000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>95.991</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14">
         <v>66.436999999999998</v>
@@ -2546,20 +3885,21 @@
       <c r="E14">
         <v>65.753</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="G14">
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14">
         <v>95.89</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>91.781000000000006</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>94.521000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>38.493000000000002</v>
@@ -2573,76 +3913,81 @@
       <c r="E15">
         <v>0</v>
       </c>
-      <c r="F15" s="15"/>
-      <c r="G15">
-        <v>0</v>
-      </c>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="16">
+        <v>2.0550000000000002</v>
+      </c>
+      <c r="C17" s="16">
+        <v>0</v>
+      </c>
+      <c r="D17" s="16">
+        <v>34</v>
+      </c>
+      <c r="E17" s="16">
+        <v>34</v>
+      </c>
+      <c r="F17" s="12">
+        <v>23</v>
+      </c>
+      <c r="G17" s="12">
+        <v>3.64</v>
+      </c>
+      <c r="H17" s="16">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="I17" s="16">
+        <v>7</v>
+      </c>
+      <c r="J17" s="16">
+        <v>5.4790000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>19</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16" s="15"/>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="19">
-        <v>2.0550000000000002</v>
-      </c>
-      <c r="C17" s="19">
-        <v>0</v>
-      </c>
-      <c r="D17" s="19">
-        <v>34</v>
-      </c>
-      <c r="E17" s="19">
-        <v>34</v>
-      </c>
-      <c r="F17" s="15">
-        <v>23</v>
-      </c>
-      <c r="G17" s="19">
-        <v>4.1100000000000003</v>
-      </c>
-      <c r="H17" s="19">
-        <v>7</v>
-      </c>
-      <c r="I17" s="19">
-        <v>5.4790000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>20</v>
       </c>
       <c r="B18" s="10">
         <v>0.21</v>
@@ -2656,26 +4001,27 @@
       <c r="E18" s="10">
         <v>0.77</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="11">
         <v>0.22</v>
       </c>
-      <c r="G18" s="10">
+      <c r="G18" s="24"/>
+      <c r="H18" s="10">
         <v>0.12</v>
       </c>
-      <c r="H18" s="10">
+      <c r="I18" s="10">
         <v>2.7</v>
       </c>
-      <c r="I18" s="10">
+      <c r="J18" s="10">
         <v>0.36</v>
       </c>
-      <c r="M18" s="10">
+      <c r="N18" s="10">
         <f>D18/F18</f>
         <v>0.17272727272727273</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="10">
         <v>2.9000000000000001E-2</v>
@@ -2689,20 +4035,21 @@
       <c r="E19" s="10">
         <v>2E-3</v>
       </c>
-      <c r="F19" s="15"/>
-      <c r="G19" s="10">
+      <c r="F19" s="12"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="10">
         <v>2E-3</v>
       </c>
-      <c r="H19" s="10">
+      <c r="I19" s="10">
         <v>0.16900000000000001</v>
       </c>
-      <c r="I19" s="10">
+      <c r="J19" s="10">
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="10">
         <v>0.5</v>
@@ -2716,61 +4063,98 @@
       <c r="E20" s="10">
         <v>41.21</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="12">
         <f>1.69*1000</f>
         <v>1690</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G20" s="12">
+        <f>0.35*1000</f>
+        <v>350</v>
+      </c>
+      <c r="H20" s="10">
         <v>0.28000000000000003</v>
       </c>
-      <c r="H20" s="10">
+      <c r="I20" s="10">
         <v>0.42</v>
       </c>
-      <c r="I20" s="10">
+      <c r="J20" s="10">
         <v>2.14</v>
       </c>
-      <c r="L20" s="21">
+      <c r="M20" s="18">
         <f>F20/D20</f>
         <v>52.128315854410857</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C21" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="18"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P20">
+        <v>63586</v>
+      </c>
+      <c r="Q20">
+        <v>93</v>
+      </c>
+      <c r="R20">
+        <v>266</v>
+      </c>
+      <c r="S20">
+        <v>678</v>
+      </c>
+      <c r="T20">
+        <v>52</v>
+      </c>
+      <c r="U20">
+        <v>7</v>
+      </c>
+      <c r="V20">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="X20" s="10">
+        <f>F18/V20</f>
+        <v>3.098591549295775</v>
+      </c>
+      <c r="Y20" s="10">
+        <f>D18/V20</f>
+        <v>0.53521126760563387</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C21" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="F22" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F22" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G22" s="3" t="s">
+      <c r="I22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="J22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I22" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B23">
         <v>55.08</v>
@@ -2784,20 +4168,21 @@
       <c r="E23">
         <v>59.12</v>
       </c>
-      <c r="F23" s="15"/>
-      <c r="G23">
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23">
         <v>38.06</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>47.38</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>43.3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24">
         <v>44.92</v>
@@ -2811,20 +4196,21 @@
       <c r="E24">
         <v>40.880000000000003</v>
       </c>
-      <c r="F24" s="15"/>
-      <c r="G24">
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24">
         <v>61.94</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>52.62</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>56.7</v>
       </c>
     </row>
-    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -2838,78 +4224,83 @@
       <c r="E25">
         <v>0</v>
       </c>
-      <c r="F25" s="15"/>
-      <c r="G25">
-        <v>0</v>
-      </c>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
       <c r="H25">
         <v>0</v>
       </c>
       <c r="I25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="J25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="16">
+        <v>55.08</v>
+      </c>
+      <c r="C27" s="16">
+        <v>31</v>
+      </c>
+      <c r="D27" s="16">
+        <v>59.08</v>
+      </c>
+      <c r="E27" s="16">
+        <v>59.12</v>
+      </c>
+      <c r="F27" s="12">
+        <v>64</v>
+      </c>
+      <c r="G27" s="12">
+        <v>29.57</v>
+      </c>
+      <c r="H27" s="16">
+        <v>38.06</v>
+      </c>
+      <c r="I27" s="16">
+        <v>48</v>
+      </c>
+      <c r="J27" s="16">
+        <v>43.3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>19</v>
       </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26" s="15"/>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="19">
-        <v>55.08</v>
-      </c>
-      <c r="C27" s="19">
-        <v>31</v>
-      </c>
-      <c r="D27" s="19">
-        <v>59.08</v>
-      </c>
-      <c r="E27" s="19">
-        <v>59.12</v>
-      </c>
-      <c r="F27" s="15">
-        <v>64</v>
-      </c>
-      <c r="G27" s="19">
-        <v>38.06</v>
-      </c>
-      <c r="H27" s="19">
-        <v>48</v>
-      </c>
-      <c r="I27" s="19">
-        <v>43.3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="20">
+      <c r="B28" s="17">
         <v>2E-3</v>
       </c>
       <c r="C28" s="10">
@@ -2921,26 +4312,27 @@
       <c r="E28" s="10">
         <v>0.17</v>
       </c>
-      <c r="F28" s="14">
+      <c r="F28" s="11">
         <v>0.2</v>
       </c>
-      <c r="G28" s="20">
+      <c r="G28" s="24"/>
+      <c r="H28" s="17">
         <v>2E-3</v>
       </c>
-      <c r="H28" s="10">
+      <c r="I28" s="10">
         <v>0.43</v>
       </c>
-      <c r="I28" s="10">
+      <c r="J28" s="10">
         <v>0.13</v>
       </c>
-      <c r="M28" s="10">
+      <c r="N28" s="10">
         <f>D28/F28</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B29" s="10">
         <v>5.0000000000000001E-3</v>
@@ -2954,20 +4346,21 @@
       <c r="E29" s="10">
         <v>1E-3</v>
       </c>
-      <c r="F29" s="15"/>
-      <c r="G29" s="10">
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="10">
         <v>1E-3</v>
       </c>
-      <c r="H29" s="10">
+      <c r="I29" s="10">
         <v>0.03</v>
       </c>
-      <c r="I29" s="10">
+      <c r="J29" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B30" s="10">
         <v>0.28000000000000003</v>
@@ -2981,61 +4374,98 @@
       <c r="E30" s="10">
         <v>24.14</v>
       </c>
-      <c r="F30" s="15">
+      <c r="F30" s="12">
         <f>0.8*1000</f>
         <v>800</v>
       </c>
-      <c r="G30" s="10">
-        <v>0</v>
+      <c r="G30" s="12">
+        <f>0.11*1000</f>
+        <v>110</v>
       </c>
       <c r="H30" s="10">
+        <v>0</v>
+      </c>
+      <c r="I30" s="10">
         <v>0.64</v>
       </c>
-      <c r="I30" s="10">
+      <c r="J30" s="10">
         <v>3.07</v>
       </c>
-      <c r="L30" s="10">
+      <c r="M30" s="10">
         <f>F30/D30</f>
         <v>16.096579476861166</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C31" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="16"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P30">
+        <v>54727</v>
+      </c>
+      <c r="Q30">
+        <v>11</v>
+      </c>
+      <c r="R30">
+        <v>18</v>
+      </c>
+      <c r="S30">
+        <v>4643</v>
+      </c>
+      <c r="T30">
+        <v>357</v>
+      </c>
+      <c r="U30">
+        <v>5</v>
+      </c>
+      <c r="V30" s="17">
+        <v>3.4200000000000001E-2</v>
+      </c>
+      <c r="X30" s="10">
+        <f>F28/V30</f>
+        <v>5.8479532163742691</v>
+      </c>
+      <c r="Y30" s="10">
+        <f>D28/V30</f>
+        <v>2.9239766081871346</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C31" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="F32" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H32" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F32" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G32" s="3" t="s">
+      <c r="I32" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="J32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I32" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B33">
         <v>5.7030000000000003</v>
@@ -3049,20 +4479,21 @@
       <c r="E33">
         <v>26.513999999999999</v>
       </c>
-      <c r="F33" s="15"/>
-      <c r="G33">
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33">
         <v>11.561</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>31.068999999999999</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>17.13</v>
       </c>
     </row>
-    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B34">
         <v>94.296999999999997</v>
@@ -3076,20 +4507,21 @@
       <c r="E34">
         <v>73.486000000000004</v>
       </c>
-      <c r="F34" s="15"/>
-      <c r="G34">
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34">
         <v>88.438999999999993</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>68.930999999999997</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>82.87</v>
       </c>
     </row>
-    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B35">
         <v>0.122</v>
@@ -3103,76 +4535,81 @@
       <c r="E35">
         <v>7.6420000000000003</v>
       </c>
-      <c r="F35" s="15"/>
-      <c r="G35">
-        <v>1.804</v>
-      </c>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
       <c r="H35">
         <v>1.804</v>
       </c>
       <c r="I35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+        <v>1.804</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" s="16">
+        <v>5.6959999999999997</v>
+      </c>
+      <c r="C37" s="16">
+        <v>23</v>
+      </c>
+      <c r="D37" s="16">
+        <v>22</v>
+      </c>
+      <c r="E37" s="16">
+        <v>24.488</v>
+      </c>
+      <c r="F37" s="12">
+        <v>29</v>
+      </c>
+      <c r="G37" s="12">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="H37" s="16">
+        <v>11.352</v>
+      </c>
+      <c r="I37" s="16">
+        <v>32</v>
+      </c>
+      <c r="J37" s="16">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>19</v>
-      </c>
-      <c r="B36">
-        <v>0</v>
-      </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36" s="15"/>
-      <c r="G36">
-        <v>0</v>
-      </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-      <c r="I36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" s="19">
-        <v>5.6959999999999997</v>
-      </c>
-      <c r="C37" s="19">
-        <v>23</v>
-      </c>
-      <c r="D37" s="19">
-        <v>22</v>
-      </c>
-      <c r="E37" s="19">
-        <v>24.488</v>
-      </c>
-      <c r="F37" s="15">
-        <v>29</v>
-      </c>
-      <c r="G37" s="19">
-        <v>11.352</v>
-      </c>
-      <c r="H37" s="19">
-        <v>32</v>
-      </c>
-      <c r="I37" s="19">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>20</v>
       </c>
       <c r="B38" s="10">
         <v>0.93</v>
@@ -3186,26 +4623,27 @@
       <c r="E38" s="10">
         <v>1.95</v>
       </c>
-      <c r="F38" s="14">
+      <c r="F38" s="11">
         <v>0.26</v>
       </c>
-      <c r="G38" s="10">
+      <c r="G38" s="24"/>
+      <c r="H38" s="10">
         <v>0.26</v>
       </c>
-      <c r="H38" s="10">
+      <c r="I38" s="10">
         <v>3.19</v>
       </c>
-      <c r="I38" s="10">
+      <c r="J38" s="10">
         <v>0.52</v>
       </c>
-      <c r="M38" s="10">
+      <c r="N38" s="10">
         <f>D38/F38</f>
         <v>6.5384615384615383</v>
       </c>
     </row>
-    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B39" s="10">
         <v>0.13400000000000001</v>
@@ -3219,20 +4657,21 @@
       <c r="E39" s="10">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="F39" s="15"/>
-      <c r="G39" s="10">
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H39" s="10">
+      <c r="I39" s="10">
         <v>0.11700000000000001</v>
       </c>
-      <c r="I39" s="10">
+      <c r="J39" s="10">
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B40" s="10">
         <v>2.35</v>
@@ -3246,61 +4685,98 @@
       <c r="E40" s="10">
         <v>7.07</v>
       </c>
-      <c r="F40" s="15">
+      <c r="F40" s="12">
         <f>0.59*1000</f>
         <v>590</v>
       </c>
-      <c r="G40" s="10">
+      <c r="G40" s="12">
+        <f>26.4*1000</f>
+        <v>26400</v>
+      </c>
+      <c r="H40" s="10">
         <v>1.07</v>
       </c>
-      <c r="H40" s="10">
+      <c r="I40" s="10">
         <v>0.92</v>
       </c>
-      <c r="I40" s="10">
+      <c r="J40" s="10">
         <v>17.920000000000002</v>
       </c>
-      <c r="L40" s="10">
+      <c r="M40" s="10">
         <f>F40/D40</f>
         <v>8.4989916450590606</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C41" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="16"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P40">
+        <v>98575</v>
+      </c>
+      <c r="Q40">
+        <v>21</v>
+      </c>
+      <c r="R40">
+        <v>5243</v>
+      </c>
+      <c r="S40">
+        <v>4581</v>
+      </c>
+      <c r="T40">
+        <v>352</v>
+      </c>
+      <c r="U40">
+        <v>3</v>
+      </c>
+      <c r="V40">
+        <v>0.16</v>
+      </c>
+      <c r="X40" s="10">
+        <f>F38/V40</f>
+        <v>1.625</v>
+      </c>
+      <c r="Y40" s="10">
+        <f>D38/V40</f>
+        <v>10.625</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C41" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="F42" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G42" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H42" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F42" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G42" s="3" t="s">
+      <c r="I42" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H42" s="3" t="s">
+      <c r="J42" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I42" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B43">
         <v>3.46</v>
@@ -3314,20 +4790,21 @@
       <c r="E43">
         <v>80.56</v>
       </c>
-      <c r="F43" s="15"/>
-      <c r="G43">
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43">
         <v>16.12</v>
       </c>
-      <c r="H43">
+      <c r="I43">
         <v>80.599999999999994</v>
       </c>
-      <c r="I43">
+      <c r="J43">
         <v>64.239999999999995</v>
       </c>
     </row>
-    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B44">
         <v>96.54</v>
@@ -3341,20 +4818,21 @@
       <c r="E44">
         <v>19.440000000000001</v>
       </c>
-      <c r="F44" s="15"/>
-      <c r="G44">
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44">
         <v>83.88</v>
       </c>
-      <c r="H44">
+      <c r="I44">
         <v>19.399999999999999</v>
       </c>
-      <c r="I44">
+      <c r="J44">
         <v>35.76</v>
       </c>
     </row>
-    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -3368,76 +4846,81 @@
       <c r="E45">
         <v>0</v>
       </c>
-      <c r="F45" s="15"/>
-      <c r="G45">
-        <v>0</v>
-      </c>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
       <c r="H45">
         <v>0</v>
       </c>
       <c r="I45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="J45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" s="16">
+        <v>3.46</v>
+      </c>
+      <c r="C47" s="16">
+        <v>79</v>
+      </c>
+      <c r="D47" s="16">
+        <v>80.400000000000006</v>
+      </c>
+      <c r="E47" s="16">
+        <v>80</v>
+      </c>
+      <c r="F47" s="12">
+        <v>88</v>
+      </c>
+      <c r="G47" s="12">
+        <v>6.24</v>
+      </c>
+      <c r="H47" s="16">
+        <v>16.12</v>
+      </c>
+      <c r="I47" s="16">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="J47" s="16">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>19</v>
-      </c>
-      <c r="B46">
-        <v>0</v>
-      </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>0</v>
-      </c>
-      <c r="F46" s="15"/>
-      <c r="G46">
-        <v>0</v>
-      </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
-      <c r="I46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>23</v>
-      </c>
-      <c r="B47" s="19">
-        <v>3.46</v>
-      </c>
-      <c r="C47" s="19">
-        <v>79</v>
-      </c>
-      <c r="D47" s="19">
-        <v>80.400000000000006</v>
-      </c>
-      <c r="E47" s="19">
-        <v>80</v>
-      </c>
-      <c r="F47" s="15">
-        <v>88</v>
-      </c>
-      <c r="G47" s="19">
-        <v>16.12</v>
-      </c>
-      <c r="H47" s="19">
-        <v>80.599999999999994</v>
-      </c>
-      <c r="I47" s="19">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>20</v>
       </c>
       <c r="B48" s="10">
         <v>2.1999999999999999E-2</v>
@@ -3451,26 +4934,27 @@
       <c r="E48" s="10">
         <v>0.21</v>
       </c>
-      <c r="F48" s="14">
+      <c r="F48" s="11">
         <v>0.15</v>
       </c>
-      <c r="G48" s="10">
+      <c r="G48" s="24"/>
+      <c r="H48" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="H48" s="10">
+      <c r="I48" s="10">
         <v>1.68</v>
       </c>
-      <c r="I48" s="10">
+      <c r="J48" s="10">
         <v>1.39</v>
       </c>
-      <c r="M48" s="10">
+      <c r="N48" s="10">
         <f>D48/F48</f>
         <v>0.73333333333333339</v>
       </c>
     </row>
-    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B49" s="10">
         <v>0.13100000000000001</v>
@@ -3484,20 +4968,21 @@
       <c r="E49" s="10">
         <v>2E-3</v>
       </c>
-      <c r="F49" s="15"/>
-      <c r="G49" s="10">
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="10">
         <v>1.6E-2</v>
       </c>
-      <c r="H49" s="10">
+      <c r="I49" s="10">
         <v>0.71699999999999997</v>
       </c>
-      <c r="I49" s="10">
+      <c r="J49" s="10">
         <v>0.158</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B50" s="10">
         <v>0.28000000000000003</v>
@@ -3511,61 +4996,98 @@
       <c r="E50" s="10">
         <v>7.35</v>
       </c>
-      <c r="F50" s="15">
+      <c r="F50" s="12">
         <f>0.43*1000</f>
         <v>430</v>
       </c>
-      <c r="G50" s="10">
+      <c r="G50" s="12">
+        <f xml:space="preserve"> 0.77*1000</f>
+        <v>770</v>
+      </c>
+      <c r="H50" s="10">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H50" s="10">
+      <c r="I50" s="10">
         <v>0.21</v>
       </c>
-      <c r="I50" s="10">
+      <c r="J50" s="10">
         <v>4.1399999999999997</v>
       </c>
-      <c r="L50" s="10">
+      <c r="M50" s="10">
         <f>F50/D50</f>
         <v>27.388535031847134</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C51" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="16"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P50">
+        <v>620521</v>
+      </c>
+      <c r="Q50">
+        <v>133</v>
+      </c>
+      <c r="R50">
+        <v>75</v>
+      </c>
+      <c r="S50">
+        <v>4643</v>
+      </c>
+      <c r="T50">
+        <v>357</v>
+      </c>
+      <c r="U50">
+        <v>5</v>
+      </c>
+      <c r="V50">
+        <v>0.54</v>
+      </c>
+      <c r="X50" s="10">
+        <f>F48/V50</f>
+        <v>0.27777777777777773</v>
+      </c>
+      <c r="Y50" s="10">
+        <f>D48/V50</f>
+        <v>0.20370370370370369</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C51" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+    </row>
+    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B52" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="F52" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G52" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H52" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F52" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G52" s="3" t="s">
+      <c r="I52" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H52" s="3" t="s">
+      <c r="J52" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I52" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B53">
         <v>32.366</v>
@@ -3579,20 +5101,21 @@
       <c r="E53">
         <v>36.713999999999999</v>
       </c>
-      <c r="F53" s="15"/>
-      <c r="G53">
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53">
         <v>25.684999999999999</v>
       </c>
-      <c r="H53">
+      <c r="I53">
         <v>22.35</v>
       </c>
-      <c r="I53">
+      <c r="J53">
         <v>24.228999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B54">
         <v>67.634</v>
@@ -3606,20 +5129,21 @@
       <c r="E54">
         <v>63.286000000000001</v>
       </c>
-      <c r="F54" s="15"/>
-      <c r="G54">
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54">
         <v>74.314999999999998</v>
       </c>
-      <c r="H54">
+      <c r="I54">
         <v>77.650000000000006</v>
       </c>
-      <c r="I54">
+      <c r="J54">
         <v>75.771000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B55">
         <v>1.631</v>
@@ -3633,76 +5157,81 @@
       <c r="E55">
         <v>0.49099999999999999</v>
       </c>
-      <c r="F55" s="15"/>
-      <c r="G55">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
       <c r="H55">
         <v>1.1000000000000001</v>
       </c>
       <c r="I55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>18</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B57" s="16">
+        <v>30</v>
+      </c>
+      <c r="C57" s="16">
+        <v>1</v>
+      </c>
+      <c r="D57" s="16">
+        <v>37</v>
+      </c>
+      <c r="E57" s="16">
+        <v>29</v>
+      </c>
+      <c r="F57" s="12">
+        <v>34</v>
+      </c>
+      <c r="G57" s="25">
+        <v>0.6</v>
+      </c>
+      <c r="H57" s="16">
+        <v>23</v>
+      </c>
+      <c r="I57" s="16">
+        <v>20</v>
+      </c>
+      <c r="J57" s="16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>19</v>
-      </c>
-      <c r="B56">
-        <v>0</v>
-      </c>
-      <c r="C56">
-        <v>0</v>
-      </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-      <c r="E56">
-        <v>0</v>
-      </c>
-      <c r="F56" s="15"/>
-      <c r="G56">
-        <v>0</v>
-      </c>
-      <c r="H56">
-        <v>0</v>
-      </c>
-      <c r="I56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>23</v>
-      </c>
-      <c r="B57" s="19">
-        <v>30</v>
-      </c>
-      <c r="C57" s="19">
-        <v>1</v>
-      </c>
-      <c r="D57" s="19">
-        <v>37</v>
-      </c>
-      <c r="E57" s="19">
-        <v>29</v>
-      </c>
-      <c r="F57" s="15">
-        <v>34</v>
-      </c>
-      <c r="G57" s="19">
-        <v>23</v>
-      </c>
-      <c r="H57" s="19">
-        <v>20</v>
-      </c>
-      <c r="I57" s="19">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>20</v>
       </c>
       <c r="B58" s="10">
         <v>8.3000000000000007</v>
@@ -3716,26 +5245,27 @@
       <c r="E58" s="10">
         <v>106.14</v>
       </c>
-      <c r="F58" s="14">
+      <c r="F58" s="11">
         <v>2.25</v>
       </c>
-      <c r="G58" s="10">
+      <c r="G58" s="24"/>
+      <c r="H58" s="10">
         <v>26</v>
       </c>
-      <c r="H58" s="10">
+      <c r="I58" s="10">
         <v>37.6</v>
       </c>
-      <c r="I58" s="10">
+      <c r="J58" s="10">
         <v>5.97</v>
       </c>
-      <c r="M58" s="10">
+      <c r="N58" s="10">
         <f>D58/F58</f>
         <v>44.48</v>
       </c>
     </row>
-    <row r="59" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B59" s="10">
         <v>5.843</v>
@@ -3749,20 +5279,21 @@
       <c r="E59" s="10">
         <v>0.45500000000000002</v>
       </c>
-      <c r="F59" s="15"/>
-      <c r="G59" s="10">
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="10">
         <v>0.16300000000000001</v>
       </c>
-      <c r="H59" s="10">
+      <c r="I59" s="10">
         <v>2.38</v>
       </c>
-      <c r="I59" s="10">
+      <c r="J59" s="10">
         <v>0.40400000000000003</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B60" s="10">
         <v>25</v>
@@ -3776,61 +5307,95 @@
       <c r="E60" s="10">
         <v>5897</v>
       </c>
-      <c r="F60" s="15">
+      <c r="F60" s="12">
         <f>344*1000</f>
         <v>344000</v>
       </c>
-      <c r="G60" s="10">
+      <c r="G60" s="11"/>
+      <c r="H60" s="10">
         <v>23.92</v>
       </c>
-      <c r="H60" s="10">
+      <c r="I60" s="10">
         <v>9.92</v>
       </c>
-      <c r="I60" s="10">
+      <c r="J60" s="10">
         <v>434</v>
       </c>
-      <c r="L60" s="10">
+      <c r="M60" s="10">
         <f>F60/D60</f>
         <v>57.42904841402337</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C61" s="11" t="s">
+      <c r="P60">
+        <v>1230568</v>
+      </c>
+      <c r="Q60">
+        <v>29</v>
+      </c>
+      <c r="R60">
+        <v>22042</v>
+      </c>
+      <c r="S60">
+        <v>41786</v>
+      </c>
+      <c r="T60">
+        <v>3214</v>
+      </c>
+      <c r="U60">
+        <v>5</v>
+      </c>
+      <c r="V60">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="X60" s="10">
+        <f>F58/V60</f>
+        <v>0.97826086956521752</v>
+      </c>
+      <c r="Y60" s="10">
+        <f>D58/V60</f>
+        <v>43.513043478260869</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C61" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+    </row>
+    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B62" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G62" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I62" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J62" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>15</v>
-      </c>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="16"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B62" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F62" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H62" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I62" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>16</v>
       </c>
       <c r="B63">
         <v>24.869</v>
@@ -3844,20 +5409,21 @@
       <c r="E63">
         <v>34.033999999999999</v>
       </c>
-      <c r="F63" s="15"/>
-      <c r="G63">
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
+      <c r="H63">
         <v>23.254000000000001</v>
       </c>
-      <c r="H63">
+      <c r="I63">
         <v>26.04</v>
       </c>
-      <c r="I63">
+      <c r="J63">
         <v>24.026</v>
       </c>
     </row>
-    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B64">
         <v>75.131</v>
@@ -3871,20 +5437,21 @@
       <c r="E64">
         <v>65.965999999999994</v>
       </c>
-      <c r="F64" s="15"/>
-      <c r="G64">
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+      <c r="H64">
         <v>76.745999999999995</v>
       </c>
-      <c r="H64">
+      <c r="I64">
         <v>73.959999999999994</v>
       </c>
-      <c r="I64">
+      <c r="J64">
         <v>75.974000000000004</v>
       </c>
     </row>
-    <row r="65" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B65">
         <v>0.32</v>
@@ -3898,20 +5465,21 @@
       <c r="E65">
         <v>0.74</v>
       </c>
-      <c r="F65" s="15"/>
-      <c r="G65">
-        <v>0.56000000000000005</v>
-      </c>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
       <c r="H65">
         <v>0.56000000000000005</v>
       </c>
       <c r="I65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B66">
         <v>0.36</v>
@@ -3925,49 +5493,53 @@
       <c r="E66">
         <v>0.36</v>
       </c>
-      <c r="F66" s="15"/>
-      <c r="G66">
-        <v>0.36</v>
-      </c>
+      <c r="F66" s="12"/>
+      <c r="G66" s="12"/>
       <c r="H66">
         <v>0.36</v>
       </c>
       <c r="I66">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J66">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="67" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>23</v>
-      </c>
-      <c r="B67" s="19">
+        <v>22</v>
+      </c>
+      <c r="B67" s="16">
         <v>24.7</v>
       </c>
-      <c r="C67" s="19">
+      <c r="C67" s="16">
         <v>6.98</v>
       </c>
-      <c r="D67" s="19">
+      <c r="D67" s="16">
         <v>34</v>
       </c>
-      <c r="E67" s="19">
+      <c r="E67" s="16">
         <v>33.659999999999997</v>
       </c>
-      <c r="F67" s="15">
+      <c r="F67" s="12">
         <v>29</v>
       </c>
-      <c r="G67" s="19">
+      <c r="G67" s="11">
+        <v>0.38</v>
+      </c>
+      <c r="H67" s="16">
         <v>23.04</v>
       </c>
-      <c r="H67" s="19">
+      <c r="I67" s="16">
         <v>25.8</v>
       </c>
-      <c r="I67" s="19">
+      <c r="J67" s="16">
         <v>25</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B68" s="10">
         <v>0.83</v>
@@ -3981,26 +5553,27 @@
       <c r="E68" s="10">
         <v>1.85</v>
       </c>
-      <c r="F68" s="14">
+      <c r="F68" s="11">
         <v>0.61</v>
       </c>
-      <c r="G68" s="10">
+      <c r="G68" s="24"/>
+      <c r="H68" s="10">
         <v>0.32</v>
       </c>
-      <c r="H68" s="10">
+      <c r="I68" s="10">
         <v>6.52</v>
       </c>
-      <c r="I68" s="10">
+      <c r="J68" s="10">
         <v>1</v>
       </c>
-      <c r="M68" s="10">
+      <c r="N68" s="10">
         <f>D68/F68</f>
         <v>2.2295081967213117</v>
       </c>
     </row>
-    <row r="69" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B69" s="10">
         <v>8.5999999999999993E-2</v>
@@ -4014,20 +5587,21 @@
       <c r="E69" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F69" s="14"/>
-      <c r="G69" s="10">
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="10">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="H69" s="10">
+      <c r="I69" s="10">
         <v>0.27400000000000002</v>
       </c>
-      <c r="I69" s="10">
+      <c r="J69" s="10">
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B70" s="10">
         <v>0.56999999999999995</v>
@@ -4041,144 +5615,183 @@
       <c r="E70" s="10">
         <v>15</v>
       </c>
-      <c r="F70" s="14">
+      <c r="F70" s="11">
         <f>6.75*1000</f>
         <v>6750</v>
       </c>
-      <c r="G70" s="10">
+      <c r="G70" s="12">
+        <f>18.143*1000</f>
+        <v>18143</v>
+      </c>
+      <c r="H70" s="10">
         <v>0.78</v>
       </c>
-      <c r="H70" s="10">
+      <c r="I70" s="10">
         <v>1</v>
       </c>
-      <c r="I70" s="10">
+      <c r="J70" s="10">
         <v>7.21</v>
       </c>
-      <c r="L70" s="10">
+      <c r="M70" s="10">
         <f>F70/D70</f>
         <v>103.5117313295507</v>
       </c>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="Q71" s="1"/>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="Q72" s="1"/>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="Q73" s="1"/>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="Q74" s="1"/>
-    </row>
-    <row r="75" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P70">
+        <v>190412</v>
+      </c>
+      <c r="Q70">
+        <v>41</v>
+      </c>
+      <c r="R70">
+        <v>2591</v>
+      </c>
+      <c r="S70">
+        <v>4643</v>
+      </c>
+      <c r="T70">
+        <v>355</v>
+      </c>
+      <c r="U70">
+        <v>5</v>
+      </c>
+      <c r="V70">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="X70" s="10">
+        <f>F68/V70</f>
+        <v>2.1785714285714284</v>
+      </c>
+      <c r="Y70" s="10">
+        <f>D68/V70</f>
+        <v>4.8571428571428568</v>
+      </c>
+    </row>
+    <row r="71" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="S71" s="1"/>
+    </row>
+    <row r="72" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="S72" s="1"/>
+    </row>
+    <row r="73" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="S73" s="1"/>
+    </row>
+    <row r="74" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="S74" s="1"/>
+    </row>
+    <row r="75" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C75" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="S75" s="19"/>
+    </row>
+    <row r="76" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="D76" t="s">
+        <v>27</v>
+      </c>
+      <c r="H76" t="s">
+        <v>29</v>
+      </c>
+      <c r="S76" s="1"/>
+    </row>
+    <row r="77" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="D77">
+        <v>75</v>
+      </c>
+      <c r="E77" t="s">
+        <v>36</v>
+      </c>
+      <c r="H77">
+        <v>625</v>
+      </c>
+      <c r="I77" t="s">
         <v>31</v>
       </c>
-      <c r="Q75" s="22"/>
-    </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="D76" t="s">
-        <v>28</v>
-      </c>
-      <c r="G76" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q76" s="1"/>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="D77">
-        <v>26</v>
-      </c>
-      <c r="E77" t="s">
-        <v>37</v>
-      </c>
-      <c r="G77">
-        <v>625</v>
-      </c>
-      <c r="H77" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q77" s="1"/>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S77" s="1"/>
+    </row>
+    <row r="78" spans="1:25" x14ac:dyDescent="0.2">
       <c r="D78">
         <v>64</v>
       </c>
       <c r="E78" t="s">
-        <v>36</v>
-      </c>
-      <c r="G78">
+        <v>35</v>
+      </c>
+      <c r="H78">
         <v>122</v>
       </c>
-      <c r="H78" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q78" s="1"/>
-    </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I78" t="s">
+        <v>32</v>
+      </c>
+      <c r="S78" s="1"/>
+    </row>
+    <row r="79" spans="1:25" x14ac:dyDescent="0.2">
       <c r="D79">
         <f>12*8*8</f>
         <v>768</v>
       </c>
       <c r="E79" t="s">
-        <v>35</v>
-      </c>
-      <c r="G79">
-        <f>32+26*4*8</f>
-        <v>864</v>
-      </c>
-      <c r="H79" t="s">
         <v>34</v>
       </c>
-      <c r="Q79" s="1"/>
-    </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H79">
+        <f>32+75*4*8</f>
+        <v>2432</v>
+      </c>
+      <c r="I79" t="s">
+        <v>33</v>
+      </c>
+      <c r="S79" s="1"/>
+    </row>
+    <row r="80" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C80" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D80" s="3">
         <f>D77+D78+D79</f>
-        <v>858</v>
-      </c>
-      <c r="G80" s="3">
-        <f>G77+G78+G79</f>
-        <v>1611</v>
-      </c>
-      <c r="Q80" s="1"/>
-    </row>
-    <row r="81" spans="17:17" x14ac:dyDescent="0.2">
-      <c r="Q81" s="1"/>
-    </row>
-    <row r="82" spans="17:17" x14ac:dyDescent="0.2">
-      <c r="Q82" s="1"/>
-    </row>
-    <row r="83" spans="17:17" x14ac:dyDescent="0.2">
-      <c r="Q83" s="1"/>
-    </row>
-    <row r="84" spans="17:17" x14ac:dyDescent="0.2">
-      <c r="Q84" s="1"/>
-    </row>
-    <row r="85" spans="17:17" x14ac:dyDescent="0.2">
-      <c r="Q85" s="1"/>
-    </row>
-    <row r="86" spans="17:17" x14ac:dyDescent="0.2">
-      <c r="Q86" s="1"/>
-    </row>
-    <row r="87" spans="17:17" x14ac:dyDescent="0.2">
-      <c r="Q87" s="1"/>
-    </row>
-    <row r="88" spans="17:17" x14ac:dyDescent="0.2">
-      <c r="Q88" s="1"/>
-    </row>
-    <row r="89" spans="17:17" x14ac:dyDescent="0.2">
-      <c r="Q89" s="1"/>
-    </row>
-    <row r="90" spans="17:17" x14ac:dyDescent="0.2">
-      <c r="Q90" s="1"/>
-    </row>
-    <row r="91" spans="17:17" x14ac:dyDescent="0.2">
-      <c r="Q91" s="1"/>
+        <v>907</v>
+      </c>
+      <c r="H80" s="3">
+        <f>H77+H78+H79</f>
+        <v>3179</v>
+      </c>
+      <c r="S80" s="1"/>
+    </row>
+    <row r="81" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="S81" s="1"/>
+    </row>
+    <row r="82" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="D82" t="s">
+        <v>49</v>
+      </c>
+      <c r="S82" s="1"/>
+    </row>
+    <row r="83" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="O83" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S83" s="1"/>
+    </row>
+    <row r="84" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="S84" s="1"/>
+    </row>
+    <row r="85" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="S85" s="1"/>
+    </row>
+    <row r="86" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="S86" s="1"/>
+    </row>
+    <row r="87" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="S87" s="1"/>
+    </row>
+    <row r="88" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="S88" s="1"/>
+    </row>
+    <row r="89" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="S89" s="1"/>
+    </row>
+    <row r="90" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="S90" s="1"/>
+    </row>
+    <row r="91" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="S91" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -4192,5 +5805,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated running times in the spreadsheet according to the last changes which were done for the performance boost
</commit_message>
<xml_diff>
--- a/sbp-accuracy-other-predictors.xlsx
+++ b/sbp-accuracy-other-predictors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelktistakis/Repositories/sBP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63405D9B-628D-784F-B0AE-ABEC42A499F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF701E47-19DD-2E44-ACC3-733CF5E24CF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="460" windowWidth="38400" windowHeight="20060" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="460" windowWidth="38400" windowHeight="20060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="69">
   <si>
     <t>subSeq</t>
   </si>
@@ -234,6 +234,9 @@
   <si>
     <t>*** subSeq has one single parameter (maxPredictionCount); this parameters was not tuned in this experiment; We might get better resutls if we tune it</t>
   </si>
+  <si>
+    <t>subSeq (BWT implementation + wt_interval_scan + neighbour_scan_results_in_map + extra ranks correction)</t>
+  </si>
 </sst>
 </file>
 
@@ -1261,7 +1264,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1303,6 +1306,14 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1312,14 +1323,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="941">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2388,7 +2394,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$X$2</c:f>
+              <c:f>Sheet1!$Y$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2467,7 +2473,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$X$10,Sheet1!$X$20,Sheet1!$X$30,Sheet1!$X$40,Sheet1!$X$50,Sheet1!$X$60,Sheet1!$X$70)</c:f>
+              <c:f>(Sheet1!$Y$10,Sheet1!$Y$20,Sheet1!$Y$30,Sheet1!$Y$40,Sheet1!$Y$50,Sheet1!$Y$60,Sheet1!$Y$70)</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2506,7 +2512,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Y$2</c:f>
+              <c:f>Sheet1!$Z$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2585,7 +2591,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$Y$10,Sheet1!$Y$20,Sheet1!$Y$30,Sheet1!$Y$40,Sheet1!$Y$50,Sheet1!$Y$60,Sheet1!$Y$70)</c:f>
+              <c:f>(Sheet1!$Z$10,Sheet1!$Z$20,Sheet1!$Z$30,Sheet1!$Z$40,Sheet1!$Z$50,Sheet1!$Z$60,Sheet1!$Z$70)</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3566,11 +3572,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Memory</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t> / Binary Size</a:t>
+              <a:t> Accuracy</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -6580,13 +6582,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>196850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
+      <xdr:col>37</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
       <xdr:row>91</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -6616,13 +6618,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>61945</xdr:colOff>
       <xdr:row>93</xdr:row>
       <xdr:rowOff>133351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>39</xdr:col>
+      <xdr:col>40</xdr:col>
       <xdr:colOff>100045</xdr:colOff>
       <xdr:row>121</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6959,29 +6961,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y91"/>
+  <dimension ref="A1:Z91"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" zoomScaleNormal="44" workbookViewId="0">
-      <selection activeCell="AA70" sqref="AA70"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="44" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="6" max="7" width="10.83203125" style="5"/>
-    <col min="19" max="19" width="13.5" customWidth="1"/>
+    <col min="6" max="8" width="10.83203125" style="5"/>
+    <col min="20" max="20" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="23" t="s">
+    <row r="1" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
       <c r="F1" s="9"/>
-      <c r="G1" s="20"/>
-    </row>
-    <row r="2" spans="1:25" ht="80" x14ac:dyDescent="0.2">
+      <c r="G1" s="23"/>
+      <c r="H1" s="20"/>
+    </row>
+    <row r="2" spans="1:26" ht="187" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -6998,52 +7001,55 @@
         <v>22</v>
       </c>
       <c r="G2" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -7059,17 +7065,17 @@
       <c r="E3">
         <v>36.186</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>31.343</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>31.033999999999999</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>32.58</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -7085,17 +7091,17 @@
       <c r="E4">
         <v>63.814</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>68.656999999999996</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>68.965999999999994</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>67.42</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -7111,17 +7117,17 @@
       <c r="E5">
         <v>0.308</v>
       </c>
-      <c r="H5">
-        <v>0.185</v>
-      </c>
       <c r="I5">
         <v>0.185</v>
       </c>
       <c r="J5">
+        <v>0.185</v>
+      </c>
+      <c r="K5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -7137,17 +7143,17 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -7166,20 +7172,21 @@
       <c r="F7" s="12">
         <v>33</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="12"/>
+      <c r="H7" s="11">
         <v>0.19</v>
       </c>
-      <c r="H7" s="16">
+      <c r="I7" s="16">
         <v>30</v>
       </c>
-      <c r="I7" s="16">
+      <c r="J7" s="16">
         <v>30.975999999999999</v>
       </c>
-      <c r="J7" s="16">
+      <c r="K7" s="16">
         <v>32.58</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -7198,23 +7205,24 @@
       <c r="F8" s="11">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G8" s="21"/>
-      <c r="H8" s="10">
+      <c r="G8" s="11"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="10">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="I8" s="10">
+      <c r="J8" s="10">
         <v>1.07</v>
       </c>
-      <c r="J8" s="10">
+      <c r="K8" s="10">
         <v>0.23</v>
       </c>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10">
+      <c r="N8" s="10"/>
+      <c r="O8" s="10">
         <f>D8/F8</f>
         <v>2.6428571428571428</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -7231,20 +7239,21 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="F9" s="12"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="10">
+      <c r="G9" s="12"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="I9" s="10">
+      <c r="J9" s="10">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="J9" s="10">
+      <c r="K9" s="10">
         <v>1.4E-2</v>
       </c>
-      <c r="M9" s="10"/>
       <c r="N9" s="10"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="O9" s="10"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -7265,63 +7274,68 @@
         <v>3210</v>
       </c>
       <c r="G10" s="12">
+        <f>0.56*1000</f>
+        <v>560</v>
+      </c>
+      <c r="H10" s="12">
         <f>370.903*1000</f>
         <v>370903</v>
       </c>
-      <c r="H10" s="10">
+      <c r="I10" s="10">
         <v>0.35</v>
       </c>
-      <c r="I10" s="10">
+      <c r="J10" s="10">
         <v>1.21</v>
       </c>
-      <c r="J10" s="10">
+      <c r="K10" s="10">
         <v>3.14</v>
       </c>
-      <c r="M10" s="10">
+      <c r="N10" s="10">
         <f>F10/D10</f>
         <v>23.516483516483518</v>
       </c>
-      <c r="N10" s="10"/>
-      <c r="P10">
+      <c r="O10" s="10"/>
+      <c r="Q10">
         <v>54979</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>12</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>494</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>4518</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>347</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <v>5</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="X10" s="10">
-        <f>F8/V10</f>
+      <c r="Y10" s="10">
+        <f>F8/W10</f>
         <v>2.2950819672131151</v>
       </c>
-      <c r="Y10" s="10">
-        <f>D8/V10</f>
+      <c r="Z10" s="10">
+        <f>D8/W10</f>
         <v>6.0655737704918034</v>
       </c>
     </row>
-    <row r="11" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="24" t="s">
+    <row r="11" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H11" s="13"/>
+    </row>
+    <row r="12" spans="1:26" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
         <v>2</v>
       </c>
@@ -7337,20 +7351,21 @@
       <c r="F12" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="14"/>
+      <c r="H12" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="I12" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="J12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="K12" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -7368,17 +7383,18 @@
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
-      <c r="H13">
+      <c r="H13" s="12"/>
+      <c r="I13">
         <v>4.1100000000000003</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>8.2189999999999994</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>5.4790000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -7396,17 +7412,18 @@
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
-      <c r="H14">
+      <c r="H14" s="12"/>
+      <c r="I14">
         <v>95.89</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>91.781000000000006</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>94.521000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -7424,17 +7441,18 @@
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
-      <c r="H15">
-        <v>0</v>
-      </c>
+      <c r="H15" s="12"/>
       <c r="I15">
         <v>0</v>
       </c>
       <c r="J15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -7452,17 +7470,18 @@
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
-      <c r="H16">
-        <v>0</v>
-      </c>
+      <c r="H16" s="12"/>
       <c r="I16">
         <v>0</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="K16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -7481,20 +7500,21 @@
       <c r="F17" s="12">
         <v>23</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="12"/>
+      <c r="H17" s="12">
         <v>3.64</v>
       </c>
-      <c r="H17" s="16">
+      <c r="I17" s="16">
         <v>4.1100000000000003</v>
       </c>
-      <c r="I17" s="16">
+      <c r="J17" s="16">
         <v>7</v>
       </c>
-      <c r="J17" s="16">
+      <c r="K17" s="16">
         <v>5.4790000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -7513,22 +7533,23 @@
       <c r="F18" s="11">
         <v>0.22</v>
       </c>
-      <c r="G18" s="21"/>
-      <c r="H18" s="10">
+      <c r="G18" s="11"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="10">
         <v>0.12</v>
       </c>
-      <c r="I18" s="10">
+      <c r="J18" s="10">
         <v>2.7</v>
       </c>
-      <c r="J18" s="10">
+      <c r="K18" s="10">
         <v>0.36</v>
       </c>
-      <c r="N18" s="10">
+      <c r="O18" s="10">
         <f>D18/F18</f>
         <v>0.17272727272727273</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -7545,18 +7566,19 @@
         <v>2E-3</v>
       </c>
       <c r="F19" s="12"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="10">
+      <c r="G19" s="12"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="10">
         <v>2E-3</v>
       </c>
-      <c r="I19" s="10">
+      <c r="J19" s="10">
         <v>0.16900000000000001</v>
       </c>
-      <c r="J19" s="10">
+      <c r="K19" s="10">
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -7577,62 +7599,67 @@
         <v>1690</v>
       </c>
       <c r="G20" s="12">
+        <f>0.4*1000</f>
+        <v>400</v>
+      </c>
+      <c r="H20" s="12">
         <f>0.35*1000</f>
         <v>350</v>
       </c>
-      <c r="H20" s="10">
+      <c r="I20" s="10">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I20" s="10">
+      <c r="J20" s="10">
         <v>0.42</v>
       </c>
-      <c r="J20" s="10">
+      <c r="K20" s="10">
         <v>2.14</v>
       </c>
-      <c r="M20" s="18">
+      <c r="N20" s="18">
         <f>F20/D20</f>
         <v>52.128315854410857</v>
       </c>
-      <c r="P20">
+      <c r="Q20">
         <v>63586</v>
       </c>
-      <c r="Q20">
+      <c r="R20">
         <v>93</v>
       </c>
-      <c r="R20">
+      <c r="S20">
         <v>266</v>
       </c>
-      <c r="S20">
+      <c r="T20">
         <v>678</v>
       </c>
-      <c r="T20">
+      <c r="U20">
         <v>52</v>
       </c>
-      <c r="U20">
+      <c r="V20">
         <v>7</v>
       </c>
-      <c r="V20">
+      <c r="W20">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="X20" s="10">
-        <f>F18/V20</f>
+      <c r="Y20" s="10">
+        <f>F18/W20</f>
         <v>3.098591549295775</v>
       </c>
-      <c r="Y20" s="10">
-        <f>D18/V20</f>
+      <c r="Z20" s="10">
+        <f>D18/W20</f>
         <v>0.53521126760563387</v>
       </c>
     </row>
-    <row r="21" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C21" s="25" t="s">
+    <row r="21" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C21" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="H21" s="15"/>
+    </row>
+    <row r="22" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
         <v>2</v>
       </c>
@@ -7648,20 +7675,21 @@
       <c r="F22" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="G22" s="14"/>
+      <c r="H22" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="I22" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="J22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="K22" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -7679,17 +7707,18 @@
       </c>
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
-      <c r="H23">
+      <c r="H23" s="12"/>
+      <c r="I23">
         <v>38.06</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>47.38</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>43.3</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -7707,17 +7736,18 @@
       </c>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
-      <c r="H24">
+      <c r="H24" s="12"/>
+      <c r="I24">
         <v>61.94</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>52.62</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>56.7</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -7735,17 +7765,18 @@
       </c>
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
-      <c r="H25">
-        <v>0</v>
-      </c>
+      <c r="H25" s="12"/>
       <c r="I25">
         <v>0</v>
       </c>
       <c r="J25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -7763,17 +7794,18 @@
       </c>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
-      <c r="H26">
-        <v>0</v>
-      </c>
+      <c r="H26" s="12"/>
       <c r="I26">
         <v>0</v>
       </c>
       <c r="J26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="K26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -7792,20 +7824,21 @@
       <c r="F27" s="12">
         <v>64</v>
       </c>
-      <c r="G27" s="12">
+      <c r="G27" s="12"/>
+      <c r="H27" s="12">
         <v>29.57</v>
       </c>
-      <c r="H27" s="16">
+      <c r="I27" s="16">
         <v>38.06</v>
       </c>
-      <c r="I27" s="16">
+      <c r="J27" s="16">
         <v>48</v>
       </c>
-      <c r="J27" s="16">
+      <c r="K27" s="16">
         <v>43.3</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -7824,22 +7857,23 @@
       <c r="F28" s="11">
         <v>0.2</v>
       </c>
-      <c r="G28" s="21"/>
-      <c r="H28" s="17">
+      <c r="G28" s="11"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="17">
         <v>2E-3</v>
       </c>
-      <c r="I28" s="10">
+      <c r="J28" s="10">
         <v>0.43</v>
       </c>
-      <c r="J28" s="10">
+      <c r="K28" s="10">
         <v>0.13</v>
       </c>
-      <c r="N28" s="10">
+      <c r="O28" s="10">
         <f>D28/F28</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -7857,17 +7891,18 @@
       </c>
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
-      <c r="H29" s="10">
+      <c r="H29" s="12"/>
+      <c r="I29" s="10">
         <v>1E-3</v>
       </c>
-      <c r="I29" s="10">
+      <c r="J29" s="10">
         <v>0.03</v>
       </c>
-      <c r="J29" s="10">
+      <c r="K29" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -7891,59 +7926,64 @@
         <f>0.11*1000</f>
         <v>110</v>
       </c>
-      <c r="H30" s="10">
+      <c r="H30" s="12">
+        <f>0.11*1000</f>
+        <v>110</v>
+      </c>
+      <c r="I30" s="10">
         <v>0</v>
       </c>
-      <c r="I30" s="10">
+      <c r="J30" s="10">
         <v>0.64</v>
       </c>
-      <c r="J30" s="10">
+      <c r="K30" s="10">
         <v>3.07</v>
       </c>
-      <c r="M30" s="10">
+      <c r="N30" s="10">
         <f>F30/D30</f>
         <v>16.096579476861166</v>
       </c>
-      <c r="P30">
+      <c r="Q30">
         <v>54727</v>
       </c>
-      <c r="Q30">
+      <c r="R30">
         <v>11</v>
       </c>
-      <c r="R30">
+      <c r="S30">
         <v>18</v>
       </c>
-      <c r="S30">
+      <c r="T30">
         <v>4643</v>
       </c>
-      <c r="T30">
+      <c r="U30">
         <v>357</v>
       </c>
-      <c r="U30">
+      <c r="V30">
         <v>5</v>
       </c>
-      <c r="V30" s="17">
+      <c r="W30" s="17">
         <v>3.4200000000000001E-2</v>
       </c>
-      <c r="X30" s="10">
-        <f>F28/V30</f>
+      <c r="Y30" s="10">
+        <f>F28/W30</f>
         <v>5.8479532163742691</v>
       </c>
-      <c r="Y30" s="10">
-        <f>D28/V30</f>
+      <c r="Z30" s="10">
+        <f>D28/W30</f>
         <v>2.9239766081871346</v>
       </c>
     </row>
-    <row r="31" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C31" s="23" t="s">
+    <row r="31" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C31" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="H31" s="13"/>
+    </row>
+    <row r="32" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
         <v>2</v>
       </c>
@@ -7959,20 +7999,21 @@
       <c r="F32" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G32" s="14" t="s">
+      <c r="G32" s="14"/>
+      <c r="H32" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="I32" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I32" s="3" t="s">
+      <c r="J32" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J32" s="3" t="s">
+      <c r="K32" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -7990,17 +8031,18 @@
       </c>
       <c r="F33" s="12"/>
       <c r="G33" s="12"/>
-      <c r="H33">
+      <c r="H33" s="12"/>
+      <c r="I33">
         <v>11.561</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>31.068999999999999</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>17.13</v>
       </c>
     </row>
-    <row r="34" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -8018,17 +8060,18 @@
       </c>
       <c r="F34" s="12"/>
       <c r="G34" s="12"/>
-      <c r="H34">
+      <c r="H34" s="12"/>
+      <c r="I34">
         <v>88.438999999999993</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>68.930999999999997</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <v>82.87</v>
       </c>
     </row>
-    <row r="35" spans="1:25" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -8046,17 +8089,18 @@
       </c>
       <c r="F35" s="12"/>
       <c r="G35" s="12"/>
-      <c r="H35">
-        <v>1.804</v>
-      </c>
+      <c r="H35" s="12"/>
       <c r="I35">
         <v>1.804</v>
       </c>
       <c r="J35">
+        <v>1.804</v>
+      </c>
+      <c r="K35">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -8074,17 +8118,18 @@
       </c>
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
-      <c r="H36">
-        <v>0</v>
-      </c>
+      <c r="H36" s="12"/>
       <c r="I36">
         <v>0</v>
       </c>
       <c r="J36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="K36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -8103,20 +8148,21 @@
       <c r="F37" s="12">
         <v>29</v>
       </c>
-      <c r="G37" s="12">
+      <c r="G37" s="12"/>
+      <c r="H37" s="12">
         <v>2.1800000000000002</v>
       </c>
-      <c r="H37" s="16">
+      <c r="I37" s="16">
         <v>11.352</v>
       </c>
-      <c r="I37" s="16">
+      <c r="J37" s="16">
         <v>32</v>
       </c>
-      <c r="J37" s="16">
+      <c r="K37" s="16">
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -8135,22 +8181,23 @@
       <c r="F38" s="11">
         <v>0.26</v>
       </c>
-      <c r="G38" s="21"/>
-      <c r="H38" s="10">
+      <c r="G38" s="11"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="10">
         <v>0.26</v>
       </c>
-      <c r="I38" s="10">
+      <c r="J38" s="10">
         <v>3.19</v>
       </c>
-      <c r="J38" s="10">
+      <c r="K38" s="10">
         <v>0.52</v>
       </c>
-      <c r="N38" s="10">
+      <c r="O38" s="10">
         <f>D38/F38</f>
         <v>6.5384615384615383</v>
       </c>
     </row>
-    <row r="39" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -8168,17 +8215,18 @@
       </c>
       <c r="F39" s="12"/>
       <c r="G39" s="12"/>
-      <c r="H39" s="10">
+      <c r="H39" s="12"/>
+      <c r="I39" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="I39" s="10">
+      <c r="J39" s="10">
         <v>0.11700000000000001</v>
       </c>
-      <c r="J39" s="10">
+      <c r="K39" s="10">
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>23</v>
       </c>
@@ -8199,62 +8247,67 @@
         <v>590</v>
       </c>
       <c r="G40" s="12">
+        <f>0.31*1000</f>
+        <v>310</v>
+      </c>
+      <c r="H40" s="12">
         <f>26.4*1000</f>
         <v>26400</v>
       </c>
-      <c r="H40" s="10">
+      <c r="I40" s="10">
         <v>1.07</v>
       </c>
-      <c r="I40" s="10">
+      <c r="J40" s="10">
         <v>0.92</v>
       </c>
-      <c r="J40" s="10">
+      <c r="K40" s="10">
         <v>17.920000000000002</v>
       </c>
-      <c r="M40" s="10">
+      <c r="N40" s="10">
         <f>F40/D40</f>
         <v>8.4989916450590606</v>
       </c>
-      <c r="P40">
+      <c r="Q40">
         <v>98575</v>
       </c>
-      <c r="Q40">
+      <c r="R40">
         <v>21</v>
       </c>
-      <c r="R40">
+      <c r="S40">
         <v>5243</v>
       </c>
-      <c r="S40">
+      <c r="T40">
         <v>4581</v>
       </c>
-      <c r="T40">
+      <c r="U40">
         <v>352</v>
       </c>
-      <c r="U40">
+      <c r="V40">
         <v>3</v>
       </c>
-      <c r="V40">
+      <c r="W40">
         <v>0.16</v>
       </c>
-      <c r="X40" s="10">
-        <f>F38/V40</f>
+      <c r="Y40" s="10">
+        <f>F38/W40</f>
         <v>1.625</v>
       </c>
-      <c r="Y40" s="10">
-        <f>D38/V40</f>
+      <c r="Z40" s="10">
+        <f>D38/W40</f>
         <v>10.625</v>
       </c>
     </row>
-    <row r="41" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C41" s="23" t="s">
+    <row r="41" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C41" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="H41" s="13"/>
+    </row>
+    <row r="42" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="B42" s="3" t="s">
         <v>2</v>
       </c>
@@ -8270,20 +8323,21 @@
       <c r="F42" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G42" s="14" t="s">
+      <c r="G42" s="14"/>
+      <c r="H42" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="H42" s="3" t="s">
+      <c r="I42" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I42" s="3" t="s">
+      <c r="J42" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J42" s="3" t="s">
+      <c r="K42" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>15</v>
       </c>
@@ -8301,17 +8355,18 @@
       </c>
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
-      <c r="H43">
+      <c r="H43" s="12"/>
+      <c r="I43">
         <v>16.12</v>
       </c>
-      <c r="I43">
+      <c r="J43">
         <v>80.599999999999994</v>
       </c>
-      <c r="J43">
+      <c r="K43">
         <v>64.239999999999995</v>
       </c>
     </row>
-    <row r="44" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>16</v>
       </c>
@@ -8329,17 +8384,18 @@
       </c>
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
-      <c r="H44">
+      <c r="H44" s="12"/>
+      <c r="I44">
         <v>83.88</v>
       </c>
-      <c r="I44">
+      <c r="J44">
         <v>19.399999999999999</v>
       </c>
-      <c r="J44">
+      <c r="K44">
         <v>35.76</v>
       </c>
     </row>
-    <row r="45" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -8357,17 +8413,18 @@
       </c>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
-      <c r="H45">
-        <v>0</v>
-      </c>
+      <c r="H45" s="12"/>
       <c r="I45">
         <v>0</v>
       </c>
       <c r="J45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>18</v>
       </c>
@@ -8385,17 +8442,18 @@
       </c>
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
-      <c r="H46">
-        <v>0</v>
-      </c>
+      <c r="H46" s="12"/>
       <c r="I46">
         <v>0</v>
       </c>
       <c r="J46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="K46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>49</v>
       </c>
@@ -8414,20 +8472,21 @@
       <c r="F47" s="12">
         <v>88</v>
       </c>
-      <c r="G47" s="12">
+      <c r="G47" s="12"/>
+      <c r="H47" s="12">
         <v>6.24</v>
       </c>
-      <c r="H47" s="16">
+      <c r="I47" s="16">
         <v>16.12</v>
       </c>
-      <c r="I47" s="16">
+      <c r="J47" s="16">
         <v>80.599999999999994</v>
       </c>
-      <c r="J47" s="16">
+      <c r="K47" s="16">
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>19</v>
       </c>
@@ -8446,22 +8505,23 @@
       <c r="F48" s="11">
         <v>0.15</v>
       </c>
-      <c r="G48" s="21"/>
-      <c r="H48" s="10">
+      <c r="G48" s="11"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="I48" s="10">
+      <c r="J48" s="10">
         <v>1.68</v>
       </c>
-      <c r="J48" s="10">
+      <c r="K48" s="10">
         <v>1.39</v>
       </c>
-      <c r="N48" s="10">
+      <c r="O48" s="10">
         <f>D48/F48</f>
         <v>0.73333333333333339</v>
       </c>
     </row>
-    <row r="49" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>20</v>
       </c>
@@ -8479,17 +8539,18 @@
       </c>
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
-      <c r="H49" s="10">
+      <c r="H49" s="12"/>
+      <c r="I49" s="10">
         <v>1.6E-2</v>
       </c>
-      <c r="I49" s="10">
+      <c r="J49" s="10">
         <v>0.71699999999999997</v>
       </c>
-      <c r="J49" s="10">
+      <c r="K49" s="10">
         <v>0.158</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>23</v>
       </c>
@@ -8510,62 +8571,67 @@
         <v>430</v>
       </c>
       <c r="G50" s="12">
+        <f>0.08*1000</f>
+        <v>80</v>
+      </c>
+      <c r="H50" s="12">
         <f xml:space="preserve"> 0.77*1000</f>
         <v>770</v>
       </c>
-      <c r="H50" s="10">
+      <c r="I50" s="10">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I50" s="10">
+      <c r="J50" s="10">
         <v>0.21</v>
       </c>
-      <c r="J50" s="10">
+      <c r="K50" s="10">
         <v>4.1399999999999997</v>
       </c>
-      <c r="M50" s="10">
+      <c r="N50" s="10">
         <f>F50/D50</f>
         <v>27.388535031847134</v>
       </c>
-      <c r="P50">
+      <c r="Q50">
         <v>620521</v>
       </c>
-      <c r="Q50">
+      <c r="R50">
         <v>133</v>
       </c>
-      <c r="R50">
+      <c r="S50">
         <v>75</v>
       </c>
-      <c r="S50">
+      <c r="T50">
         <v>4643</v>
       </c>
-      <c r="T50">
+      <c r="U50">
         <v>357</v>
       </c>
-      <c r="U50">
+      <c r="V50">
         <v>5</v>
       </c>
-      <c r="V50">
+      <c r="W50">
         <v>0.54</v>
       </c>
-      <c r="X50" s="10">
-        <f>F48/V50</f>
+      <c r="Y50" s="10">
+        <f>F48/W50</f>
         <v>0.27777777777777773</v>
       </c>
-      <c r="Y50" s="10">
-        <f>D48/V50</f>
+      <c r="Z50" s="10">
+        <f>D48/W50</f>
         <v>0.20370370370370369</v>
       </c>
     </row>
-    <row r="51" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C51" s="23" t="s">
+    <row r="51" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C51" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="D51" s="23"/>
-      <c r="E51" s="23"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="27"/>
       <c r="F51" s="13"/>
       <c r="G51" s="13"/>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="H51" s="13"/>
+    </row>
+    <row r="52" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="B52" s="3" t="s">
         <v>2</v>
       </c>
@@ -8581,20 +8647,21 @@
       <c r="F52" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G52" s="14" t="s">
+      <c r="G52" s="14"/>
+      <c r="H52" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="H52" s="3" t="s">
+      <c r="I52" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I52" s="3" t="s">
+      <c r="J52" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J52" s="3" t="s">
+      <c r="K52" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>15</v>
       </c>
@@ -8612,17 +8679,18 @@
       </c>
       <c r="F53" s="12"/>
       <c r="G53" s="12"/>
-      <c r="H53">
+      <c r="H53" s="12"/>
+      <c r="I53">
         <v>25.684999999999999</v>
       </c>
-      <c r="I53">
+      <c r="J53">
         <v>22.35</v>
       </c>
-      <c r="J53">
+      <c r="K53">
         <v>24.228999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>16</v>
       </c>
@@ -8640,17 +8708,18 @@
       </c>
       <c r="F54" s="12"/>
       <c r="G54" s="12"/>
-      <c r="H54">
+      <c r="H54" s="12"/>
+      <c r="I54">
         <v>74.314999999999998</v>
       </c>
-      <c r="I54">
+      <c r="J54">
         <v>77.650000000000006</v>
       </c>
-      <c r="J54">
+      <c r="K54">
         <v>75.771000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>17</v>
       </c>
@@ -8668,17 +8737,18 @@
       </c>
       <c r="F55" s="12"/>
       <c r="G55" s="12"/>
-      <c r="H55">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="H55" s="12"/>
       <c r="I55">
         <v>1.1000000000000001</v>
       </c>
       <c r="J55">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K55">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -8696,17 +8766,18 @@
       </c>
       <c r="F56" s="12"/>
       <c r="G56" s="12"/>
-      <c r="H56">
-        <v>0</v>
-      </c>
+      <c r="H56" s="12"/>
       <c r="I56">
         <v>0</v>
       </c>
       <c r="J56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="K56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>49</v>
       </c>
@@ -8725,20 +8796,21 @@
       <c r="F57" s="12">
         <v>34</v>
       </c>
-      <c r="G57" s="22">
+      <c r="G57" s="12"/>
+      <c r="H57" s="22">
         <v>0.6</v>
       </c>
-      <c r="H57" s="16">
+      <c r="I57" s="16">
         <v>23</v>
-      </c>
-      <c r="I57" s="16">
-        <v>20</v>
       </c>
       <c r="J57" s="16">
         <v>20</v>
       </c>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="K57" s="16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>19</v>
       </c>
@@ -8757,22 +8829,23 @@
       <c r="F58" s="11">
         <v>2.25</v>
       </c>
-      <c r="G58" s="21"/>
-      <c r="H58" s="10">
+      <c r="G58" s="11"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="10">
         <v>26</v>
       </c>
-      <c r="I58" s="10">
+      <c r="J58" s="10">
         <v>37.6</v>
       </c>
-      <c r="J58" s="10">
+      <c r="K58" s="10">
         <v>5.97</v>
       </c>
-      <c r="N58" s="10">
+      <c r="O58" s="10">
         <f>D58/F58</f>
         <v>44.48</v>
       </c>
     </row>
-    <row r="59" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>20</v>
       </c>
@@ -8790,17 +8863,18 @@
       </c>
       <c r="F59" s="12"/>
       <c r="G59" s="12"/>
-      <c r="H59" s="10">
+      <c r="H59" s="12"/>
+      <c r="I59" s="10">
         <v>0.16300000000000001</v>
       </c>
-      <c r="I59" s="10">
+      <c r="J59" s="10">
         <v>2.38</v>
       </c>
-      <c r="J59" s="10">
+      <c r="K59" s="10">
         <v>0.40400000000000003</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>23</v>
       </c>
@@ -8821,62 +8895,67 @@
         <v>344000</v>
       </c>
       <c r="G60" s="12">
+        <f>102*1000</f>
+        <v>102000</v>
+      </c>
+      <c r="H60" s="12">
         <f>1992.633*1000</f>
         <v>1992633</v>
       </c>
-      <c r="H60" s="10">
+      <c r="I60" s="10">
         <v>23.92</v>
       </c>
-      <c r="I60" s="10">
+      <c r="J60" s="10">
         <v>9.92</v>
       </c>
-      <c r="J60" s="10">
+      <c r="K60" s="10">
         <v>434</v>
       </c>
-      <c r="M60" s="10">
+      <c r="N60" s="10">
         <f>F60/D60</f>
         <v>57.42904841402337</v>
       </c>
-      <c r="P60">
+      <c r="Q60">
         <v>1230568</v>
       </c>
-      <c r="Q60">
+      <c r="R60">
         <v>29</v>
       </c>
-      <c r="R60">
+      <c r="S60">
         <v>22042</v>
       </c>
-      <c r="S60">
+      <c r="T60">
         <v>41786</v>
       </c>
-      <c r="T60">
+      <c r="U60">
         <v>3214</v>
       </c>
-      <c r="U60">
+      <c r="V60">
         <v>5</v>
       </c>
-      <c r="V60">
+      <c r="W60">
         <v>2.2999999999999998</v>
       </c>
-      <c r="X60" s="10">
-        <f>F58/V60</f>
+      <c r="Y60" s="10">
+        <f>F58/W60</f>
         <v>0.97826086956521752</v>
       </c>
-      <c r="Y60" s="10">
-        <f>D58/V60</f>
+      <c r="Z60" s="10">
+        <f>D58/W60</f>
         <v>43.513043478260869</v>
       </c>
     </row>
-    <row r="61" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C61" s="23" t="s">
+    <row r="61" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C61" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D61" s="23"/>
-      <c r="E61" s="23"/>
+      <c r="D61" s="27"/>
+      <c r="E61" s="27"/>
       <c r="F61" s="13"/>
       <c r="G61" s="13"/>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="H61" s="13"/>
+    </row>
+    <row r="62" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="B62" s="3" t="s">
         <v>2</v>
       </c>
@@ -8892,20 +8971,21 @@
       <c r="F62" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G62" s="14" t="s">
+      <c r="G62" s="14"/>
+      <c r="H62" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="H62" s="3" t="s">
+      <c r="I62" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I62" s="3" t="s">
+      <c r="J62" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J62" s="3" t="s">
+      <c r="K62" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>15</v>
       </c>
@@ -8923,17 +9003,18 @@
       </c>
       <c r="F63" s="12"/>
       <c r="G63" s="12"/>
-      <c r="H63">
+      <c r="H63" s="12"/>
+      <c r="I63">
         <v>23.254000000000001</v>
       </c>
-      <c r="I63">
+      <c r="J63">
         <v>26.04</v>
       </c>
-      <c r="J63">
+      <c r="K63">
         <v>24.026</v>
       </c>
     </row>
-    <row r="64" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>16</v>
       </c>
@@ -8951,17 +9032,18 @@
       </c>
       <c r="F64" s="12"/>
       <c r="G64" s="12"/>
-      <c r="H64">
+      <c r="H64" s="12"/>
+      <c r="I64">
         <v>76.745999999999995</v>
       </c>
-      <c r="I64">
+      <c r="J64">
         <v>73.959999999999994</v>
       </c>
-      <c r="J64">
+      <c r="K64">
         <v>75.974000000000004</v>
       </c>
     </row>
-    <row r="65" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>17</v>
       </c>
@@ -8979,17 +9061,18 @@
       </c>
       <c r="F65" s="12"/>
       <c r="G65" s="12"/>
-      <c r="H65">
-        <v>0.56000000000000005</v>
-      </c>
+      <c r="H65" s="12"/>
       <c r="I65">
         <v>0.56000000000000005</v>
       </c>
       <c r="J65">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="K65">
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>18</v>
       </c>
@@ -9007,17 +9090,18 @@
       </c>
       <c r="F66" s="12"/>
       <c r="G66" s="12"/>
-      <c r="H66">
-        <v>0.36</v>
-      </c>
+      <c r="H66" s="12"/>
       <c r="I66">
         <v>0.36</v>
       </c>
       <c r="J66">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="K66">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>49</v>
       </c>
@@ -9036,20 +9120,21 @@
       <c r="F67" s="12">
         <v>29</v>
       </c>
-      <c r="G67" s="11">
+      <c r="G67" s="12"/>
+      <c r="H67" s="11">
         <v>0.38</v>
       </c>
-      <c r="H67" s="16">
+      <c r="I67" s="16">
         <v>23.04</v>
       </c>
-      <c r="I67" s="16">
+      <c r="J67" s="16">
         <v>25.8</v>
       </c>
-      <c r="J67" s="16">
+      <c r="K67" s="16">
         <v>25</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>19</v>
       </c>
@@ -9068,22 +9153,23 @@
       <c r="F68" s="11">
         <v>0.61</v>
       </c>
-      <c r="G68" s="21"/>
-      <c r="H68" s="10">
+      <c r="G68" s="11"/>
+      <c r="H68" s="21"/>
+      <c r="I68" s="10">
         <v>0.32</v>
       </c>
-      <c r="I68" s="10">
+      <c r="J68" s="10">
         <v>6.52</v>
       </c>
-      <c r="J68" s="10">
+      <c r="K68" s="10">
         <v>1</v>
       </c>
-      <c r="N68" s="10">
+      <c r="O68" s="10">
         <f>D68/F68</f>
         <v>2.2295081967213117</v>
       </c>
     </row>
-    <row r="69" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>20</v>
       </c>
@@ -9101,17 +9187,18 @@
       </c>
       <c r="F69" s="11"/>
       <c r="G69" s="11"/>
-      <c r="H69" s="10">
+      <c r="H69" s="11"/>
+      <c r="I69" s="10">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="I69" s="10">
+      <c r="J69" s="10">
         <v>0.27400000000000002</v>
       </c>
-      <c r="J69" s="10">
+      <c r="K69" s="10">
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>23</v>
       </c>
@@ -9131,111 +9218,115 @@
         <f>6.75*1000</f>
         <v>6750</v>
       </c>
-      <c r="G70" s="12">
+      <c r="G70" s="11">
+        <f>1.21*1000</f>
+        <v>1210</v>
+      </c>
+      <c r="H70" s="12">
         <f>18.143*1000</f>
         <v>18143</v>
       </c>
-      <c r="H70" s="10">
+      <c r="I70" s="10">
         <v>0.78</v>
       </c>
-      <c r="I70" s="10">
+      <c r="J70" s="10">
         <v>1</v>
       </c>
-      <c r="J70" s="10">
+      <c r="K70" s="10">
         <v>7.21</v>
       </c>
-      <c r="M70" s="10">
+      <c r="N70" s="10">
         <f>F70/D70</f>
         <v>103.5117313295507</v>
       </c>
-      <c r="P70">
+      <c r="Q70">
         <v>190412</v>
       </c>
-      <c r="Q70">
+      <c r="R70">
         <v>41</v>
       </c>
-      <c r="R70">
+      <c r="S70">
         <v>2591</v>
       </c>
-      <c r="S70">
+      <c r="T70">
         <v>4643</v>
       </c>
-      <c r="T70">
+      <c r="U70">
         <v>355</v>
       </c>
-      <c r="U70">
+      <c r="V70">
         <v>5</v>
       </c>
-      <c r="V70">
+      <c r="W70">
         <v>0.28000000000000003</v>
       </c>
-      <c r="X70" s="10">
-        <f>F68/V70</f>
+      <c r="Y70" s="10">
+        <f>F68/W70</f>
         <v>2.1785714285714284</v>
       </c>
-      <c r="Y70" s="10">
-        <f>D68/V70</f>
+      <c r="Z70" s="10">
+        <f>D68/W70</f>
         <v>4.8571428571428568</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="S71" s="1"/>
-    </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="S72" s="1"/>
-    </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="S73" s="1"/>
-    </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="S74" s="1"/>
-    </row>
-    <row r="75" spans="1:25" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="T71" s="1"/>
+    </row>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="T72" s="1"/>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="T73" s="1"/>
+    </row>
+    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="T74" s="1"/>
+    </row>
+    <row r="75" spans="1:26" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="C75" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="S75" s="19"/>
-    </row>
-    <row r="76" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+      <c r="T75" s="19"/>
+    </row>
+    <row r="76" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="D76" t="s">
         <v>24</v>
       </c>
-      <c r="H76" t="s">
+      <c r="I76" t="s">
         <v>26</v>
       </c>
-      <c r="S76" s="1"/>
-    </row>
-    <row r="77" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+      <c r="T76" s="1"/>
+    </row>
+    <row r="77" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="D77">
         <v>75</v>
       </c>
       <c r="E77" t="s">
         <v>33</v>
       </c>
-      <c r="H77">
+      <c r="I77">
         <v>625</v>
       </c>
-      <c r="I77" t="s">
+      <c r="J77" t="s">
         <v>28</v>
       </c>
-      <c r="S77" s="1"/>
-    </row>
-    <row r="78" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+      <c r="T77" s="1"/>
+    </row>
+    <row r="78" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="D78">
         <v>64</v>
       </c>
       <c r="E78" t="s">
         <v>32</v>
       </c>
-      <c r="H78">
+      <c r="I78">
         <v>122</v>
       </c>
-      <c r="I78" t="s">
+      <c r="J78" t="s">
         <v>29</v>
       </c>
-      <c r="S78" s="1"/>
-    </row>
-    <row r="79" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+      <c r="T78" s="1"/>
+    </row>
+    <row r="79" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="D79">
         <f>12*8*8</f>
         <v>768</v>
@@ -9243,16 +9334,16 @@
       <c r="E79" t="s">
         <v>31</v>
       </c>
-      <c r="H79">
+      <c r="I79">
         <f>32+75*4*8</f>
         <v>2432</v>
       </c>
-      <c r="I79" t="s">
+      <c r="J79" t="s">
         <v>30</v>
       </c>
-      <c r="S79" s="1"/>
-    </row>
-    <row r="80" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+      <c r="T79" s="1"/>
+    </row>
+    <row r="80" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="C80" t="s">
         <v>25</v>
       </c>
@@ -9260,50 +9351,50 @@
         <f>D77+D78+D79</f>
         <v>907</v>
       </c>
-      <c r="H80" s="3">
-        <f>H77+H78+H79</f>
+      <c r="I80" s="3">
+        <f>I77+I78+I79</f>
         <v>3179</v>
       </c>
-      <c r="S80" s="1"/>
-    </row>
-    <row r="81" spans="4:19" hidden="1" x14ac:dyDescent="0.2">
-      <c r="S81" s="1"/>
-    </row>
-    <row r="82" spans="4:19" hidden="1" x14ac:dyDescent="0.2">
+      <c r="T80" s="1"/>
+    </row>
+    <row r="81" spans="4:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="T81" s="1"/>
+    </row>
+    <row r="82" spans="4:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="D82" t="s">
         <v>43</v>
       </c>
-      <c r="S82" s="1"/>
-    </row>
-    <row r="83" spans="4:19" x14ac:dyDescent="0.2">
-      <c r="O83" s="3" t="s">
+      <c r="T82" s="1"/>
+    </row>
+    <row r="83" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="P83" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="S83" s="1"/>
-    </row>
-    <row r="84" spans="4:19" x14ac:dyDescent="0.2">
-      <c r="S84" s="1"/>
-    </row>
-    <row r="85" spans="4:19" x14ac:dyDescent="0.2">
-      <c r="S85" s="1"/>
-    </row>
-    <row r="86" spans="4:19" x14ac:dyDescent="0.2">
-      <c r="S86" s="1"/>
-    </row>
-    <row r="87" spans="4:19" x14ac:dyDescent="0.2">
-      <c r="S87" s="1"/>
-    </row>
-    <row r="88" spans="4:19" x14ac:dyDescent="0.2">
-      <c r="S88" s="1"/>
-    </row>
-    <row r="89" spans="4:19" x14ac:dyDescent="0.2">
-      <c r="S89" s="1"/>
-    </row>
-    <row r="90" spans="4:19" x14ac:dyDescent="0.2">
-      <c r="S90" s="1"/>
-    </row>
-    <row r="91" spans="4:19" x14ac:dyDescent="0.2">
-      <c r="S91" s="1"/>
+      <c r="T83" s="1"/>
+    </row>
+    <row r="84" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="T84" s="1"/>
+    </row>
+    <row r="85" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="T85" s="1"/>
+    </row>
+    <row r="86" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="T86" s="1"/>
+    </row>
+    <row r="87" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="T87" s="1"/>
+    </row>
+    <row r="88" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="T88" s="1"/>
+    </row>
+    <row r="89" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="T89" s="1"/>
+    </row>
+    <row r="90" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="T90" s="1"/>
+    </row>
+    <row r="91" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="T91" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -9325,8 +9416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="F80" sqref="F80"/>
+    <sheetView zoomScale="83" workbookViewId="0">
+      <selection activeCell="AJ3" sqref="AJ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9337,31 +9428,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26"/>
-      <c r="B1" s="26"/>
-      <c r="C1" s="27" t="s">
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:25" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="16"/>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="25" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="14" t="s">
@@ -9370,13 +9461,13 @@
       <c r="G2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="25" t="s">
         <v>7</v>
       </c>
       <c r="M2" s="2" t="s">
@@ -9508,18 +9599,18 @@
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="27" t="s">
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -9538,16 +9629,16 @@
     </row>
     <row r="7" spans="1:25" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="25" t="s">
         <v>3</v>
       </c>
       <c r="F7" s="14" t="s">
@@ -9556,13 +9647,13 @@
       <c r="G7" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="28" t="s">
+      <c r="H7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="28" t="s">
+      <c r="I7" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="28" t="s">
+      <c r="J7" s="25" t="s">
         <v>7</v>
       </c>
       <c r="M7" s="2" t="s">
@@ -9693,18 +9784,18 @@
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="27" t="s">
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
@@ -9723,16 +9814,16 @@
     </row>
     <row r="12" spans="1:25" ht="85" x14ac:dyDescent="0.2">
       <c r="A12" s="16"/>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="25" t="s">
         <v>3</v>
       </c>
       <c r="F12" s="14" t="s">
@@ -9741,13 +9832,13 @@
       <c r="G12" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="28" t="s">
+      <c r="H12" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="28" t="s">
+      <c r="I12" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="J12" s="28" t="s">
+      <c r="J12" s="25" t="s">
         <v>7</v>
       </c>
       <c r="M12" s="2" t="s">
@@ -9878,18 +9969,18 @@
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="27" t="s">
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
@@ -9908,16 +9999,16 @@
     </row>
     <row r="17" spans="1:25" ht="85" x14ac:dyDescent="0.2">
       <c r="A17" s="16"/>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="25" t="s">
         <v>3</v>
       </c>
       <c r="F17" s="14" t="s">
@@ -9926,13 +10017,13 @@
       <c r="G17" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H17" s="28" t="s">
+      <c r="H17" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I17" s="28" t="s">
+      <c r="I17" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="J17" s="28" t="s">
+      <c r="J17" s="25" t="s">
         <v>7</v>
       </c>
       <c r="M17" s="2" t="s">
@@ -10056,18 +10147,18 @@
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="27" t="s">
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
@@ -10086,16 +10177,16 @@
     </row>
     <row r="22" spans="1:25" ht="85" x14ac:dyDescent="0.2">
       <c r="A22" s="16"/>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="25" t="s">
         <v>3</v>
       </c>
       <c r="F22" s="14" t="s">
@@ -10104,13 +10195,13 @@
       <c r="G22" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H22" s="28" t="s">
+      <c r="H22" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I22" s="28" t="s">
+      <c r="I22" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="J22" s="28" t="s">
+      <c r="J22" s="25" t="s">
         <v>7</v>
       </c>
       <c r="M22" s="2" t="s">
@@ -10234,18 +10325,18 @@
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="27" t="s">
+      <c r="A26" s="24"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
@@ -10264,16 +10355,16 @@
     </row>
     <row r="27" spans="1:25" ht="85" x14ac:dyDescent="0.2">
       <c r="A27" s="16"/>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="28" t="s">
+      <c r="D27" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="28" t="s">
+      <c r="E27" s="25" t="s">
         <v>3</v>
       </c>
       <c r="F27" s="14" t="s">
@@ -10282,13 +10373,13 @@
       <c r="G27" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H27" s="28" t="s">
+      <c r="H27" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I27" s="28" t="s">
+      <c r="I27" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="J27" s="28" t="s">
+      <c r="J27" s="25" t="s">
         <v>7</v>
       </c>
       <c r="M27" s="2" t="s">
@@ -10412,18 +10503,18 @@
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A31" s="26"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="27" t="s">
+      <c r="A31" s="24"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
@@ -10442,16 +10533,16 @@
     </row>
     <row r="32" spans="1:25" ht="85" x14ac:dyDescent="0.2">
       <c r="A32" s="16"/>
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="C32" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D32" s="28" t="s">
+      <c r="D32" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E32" s="28" t="s">
+      <c r="E32" s="25" t="s">
         <v>3</v>
       </c>
       <c r="F32" s="14" t="s">
@@ -10460,13 +10551,13 @@
       <c r="G32" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H32" s="28" t="s">
+      <c r="H32" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I32" s="28" t="s">
+      <c r="I32" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="J32" s="28" t="s">
+      <c r="J32" s="25" t="s">
         <v>7</v>
       </c>
       <c r="M32" s="2" t="s">
@@ -10590,18 +10681,18 @@
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A36" s="26"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="27" t="s">
+      <c r="A36" s="24"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
       <c r="F36" s="13"/>
       <c r="G36" s="13"/>
-      <c r="H36" s="26"/>
-      <c r="I36" s="26"/>
-      <c r="J36" s="26"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
@@ -10620,16 +10711,16 @@
     </row>
     <row r="37" spans="1:25" ht="85" x14ac:dyDescent="0.2">
       <c r="A37" s="16"/>
-      <c r="B37" s="28" t="s">
+      <c r="B37" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C37" s="28" t="s">
+      <c r="C37" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D37" s="28" t="s">
+      <c r="D37" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E37" s="28" t="s">
+      <c r="E37" s="25" t="s">
         <v>3</v>
       </c>
       <c r="F37" s="14" t="s">
@@ -10638,13 +10729,13 @@
       <c r="G37" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H37" s="28" t="s">
+      <c r="H37" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I37" s="28" t="s">
+      <c r="I37" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="J37" s="28" t="s">
+      <c r="J37" s="25" t="s">
         <v>7</v>
       </c>
       <c r="M37" s="2" t="s">
@@ -10769,18 +10860,18 @@
       </c>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A41" s="26"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="27" t="s">
+      <c r="A41" s="24"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="30"/>
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
-      <c r="H41" s="26"/>
-      <c r="I41" s="26"/>
-      <c r="J41" s="26"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
@@ -10799,16 +10890,16 @@
     </row>
     <row r="42" spans="1:25" ht="85" x14ac:dyDescent="0.2">
       <c r="A42" s="16"/>
-      <c r="B42" s="28" t="s">
+      <c r="B42" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C42" s="28" t="s">
+      <c r="C42" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D42" s="28" t="s">
+      <c r="D42" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E42" s="28" t="s">
+      <c r="E42" s="25" t="s">
         <v>3</v>
       </c>
       <c r="F42" s="14" t="s">
@@ -10817,13 +10908,13 @@
       <c r="G42" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H42" s="28" t="s">
+      <c r="H42" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I42" s="28" t="s">
+      <c r="I42" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="J42" s="28" t="s">
+      <c r="J42" s="25" t="s">
         <v>7</v>
       </c>
       <c r="M42" s="2" t="s">
@@ -10948,18 +11039,18 @@
       </c>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="27" t="s">
+      <c r="A46" s="24"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="D46" s="27"/>
-      <c r="E46" s="27"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
       <c r="F46" s="13"/>
       <c r="G46" s="13"/>
-      <c r="H46" s="26"/>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="24"/>
+      <c r="J46" s="24"/>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
@@ -10978,16 +11069,16 @@
     </row>
     <row r="47" spans="1:25" ht="85" x14ac:dyDescent="0.2">
       <c r="A47" s="16"/>
-      <c r="B47" s="28" t="s">
+      <c r="B47" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="28" t="s">
+      <c r="C47" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D47" s="28" t="s">
+      <c r="D47" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E47" s="28" t="s">
+      <c r="E47" s="25" t="s">
         <v>3</v>
       </c>
       <c r="F47" s="14" t="s">
@@ -10996,13 +11087,13 @@
       <c r="G47" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H47" s="28" t="s">
+      <c r="H47" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I47" s="28" t="s">
+      <c r="I47" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="J47" s="28" t="s">
+      <c r="J47" s="25" t="s">
         <v>7</v>
       </c>
       <c r="M47" s="2" t="s">
@@ -11127,18 +11218,18 @@
       </c>
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A51" s="26"/>
-      <c r="B51" s="26"/>
-      <c r="C51" s="27" t="s">
+      <c r="A51" s="24"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="D51" s="27"/>
-      <c r="E51" s="27"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="30"/>
       <c r="F51" s="13"/>
       <c r="G51" s="13"/>
-      <c r="H51" s="26"/>
-      <c r="I51" s="26"/>
-      <c r="J51" s="26"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="24"/>
+      <c r="J51" s="24"/>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
@@ -11157,16 +11248,16 @@
     </row>
     <row r="52" spans="1:25" ht="85" x14ac:dyDescent="0.2">
       <c r="A52" s="16"/>
-      <c r="B52" s="28" t="s">
+      <c r="B52" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C52" s="28" t="s">
+      <c r="C52" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D52" s="28" t="s">
+      <c r="D52" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E52" s="28" t="s">
+      <c r="E52" s="25" t="s">
         <v>3</v>
       </c>
       <c r="F52" s="14" t="s">
@@ -11175,13 +11266,13 @@
       <c r="G52" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H52" s="28" t="s">
+      <c r="H52" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I52" s="28" t="s">
+      <c r="I52" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="J52" s="28" t="s">
+      <c r="J52" s="25" t="s">
         <v>7</v>
       </c>
       <c r="M52" s="2" t="s">
@@ -11269,7 +11360,7 @@
       <c r="F54" s="12">
         <v>0.56000000000000005</v>
       </c>
-      <c r="G54" s="29"/>
+      <c r="G54" s="26"/>
       <c r="H54" s="11">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -11306,18 +11397,18 @@
       </c>
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A56" s="26"/>
-      <c r="B56" s="26"/>
-      <c r="C56" s="27" t="s">
+      <c r="A56" s="24"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="D56" s="27"/>
-      <c r="E56" s="27"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="30"/>
       <c r="F56" s="13"/>
       <c r="G56" s="13"/>
-      <c r="H56" s="26"/>
-      <c r="I56" s="26"/>
-      <c r="J56" s="26"/>
+      <c r="H56" s="24"/>
+      <c r="I56" s="24"/>
+      <c r="J56" s="24"/>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
@@ -11336,16 +11427,16 @@
     </row>
     <row r="57" spans="1:25" ht="85" x14ac:dyDescent="0.2">
       <c r="A57" s="16"/>
-      <c r="B57" s="28" t="s">
+      <c r="B57" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="28" t="s">
+      <c r="C57" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D57" s="28" t="s">
+      <c r="D57" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E57" s="28" t="s">
+      <c r="E57" s="25" t="s">
         <v>3</v>
       </c>
       <c r="F57" s="14" t="s">
@@ -11354,13 +11445,13 @@
       <c r="G57" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H57" s="28" t="s">
+      <c r="H57" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I57" s="28" t="s">
+      <c r="I57" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="J57" s="28" t="s">
+      <c r="J57" s="25" t="s">
         <v>7</v>
       </c>
       <c r="M57" s="2" t="s">
@@ -11485,18 +11576,18 @@
       </c>
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A61" s="26"/>
-      <c r="B61" s="26"/>
-      <c r="C61" s="27" t="s">
+      <c r="A61" s="24"/>
+      <c r="B61" s="24"/>
+      <c r="C61" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="D61" s="27"/>
-      <c r="E61" s="27"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="30"/>
       <c r="F61" s="13"/>
       <c r="G61" s="13"/>
-      <c r="H61" s="26"/>
-      <c r="I61" s="26"/>
-      <c r="J61" s="26"/>
+      <c r="H61" s="24"/>
+      <c r="I61" s="24"/>
+      <c r="J61" s="24"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
@@ -11515,16 +11606,16 @@
     </row>
     <row r="62" spans="1:25" ht="85" x14ac:dyDescent="0.2">
       <c r="A62" s="16"/>
-      <c r="B62" s="28" t="s">
+      <c r="B62" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C62" s="28" t="s">
+      <c r="C62" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D62" s="28" t="s">
+      <c r="D62" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E62" s="28" t="s">
+      <c r="E62" s="25" t="s">
         <v>3</v>
       </c>
       <c r="F62" s="14" t="s">
@@ -11533,13 +11624,13 @@
       <c r="G62" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H62" s="28" t="s">
+      <c r="H62" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I62" s="28" t="s">
+      <c r="I62" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="J62" s="28" t="s">
+      <c r="J62" s="25" t="s">
         <v>7</v>
       </c>
       <c r="M62" s="2" t="s">
@@ -11664,18 +11755,18 @@
       </c>
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A66" s="26"/>
-      <c r="B66" s="26"/>
-      <c r="C66" s="27" t="s">
+      <c r="A66" s="24"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="D66" s="27"/>
-      <c r="E66" s="27"/>
+      <c r="D66" s="30"/>
+      <c r="E66" s="30"/>
       <c r="F66" s="13"/>
       <c r="G66" s="13"/>
-      <c r="H66" s="26"/>
-      <c r="I66" s="26"/>
-      <c r="J66" s="26"/>
+      <c r="H66" s="24"/>
+      <c r="I66" s="24"/>
+      <c r="J66" s="24"/>
       <c r="K66" s="4"/>
       <c r="L66" s="4"/>
       <c r="M66" s="4"/>
@@ -11694,16 +11785,16 @@
     </row>
     <row r="67" spans="1:25" ht="85" x14ac:dyDescent="0.2">
       <c r="A67" s="16"/>
-      <c r="B67" s="28" t="s">
+      <c r="B67" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C67" s="28" t="s">
+      <c r="C67" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D67" s="28" t="s">
+      <c r="D67" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E67" s="28" t="s">
+      <c r="E67" s="25" t="s">
         <v>3</v>
       </c>
       <c r="F67" s="14" t="s">
@@ -11712,13 +11803,13 @@
       <c r="G67" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H67" s="28" t="s">
+      <c r="H67" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I67" s="28" t="s">
+      <c r="I67" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="J67" s="28" t="s">
+      <c r="J67" s="25" t="s">
         <v>7</v>
       </c>
       <c r="M67" s="2" t="s">
@@ -11843,18 +11934,18 @@
       </c>
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A71" s="26"/>
-      <c r="B71" s="26"/>
-      <c r="C71" s="27" t="s">
+      <c r="A71" s="24"/>
+      <c r="B71" s="24"/>
+      <c r="C71" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="D71" s="27"/>
-      <c r="E71" s="27"/>
+      <c r="D71" s="30"/>
+      <c r="E71" s="30"/>
       <c r="F71" s="13"/>
       <c r="G71" s="13"/>
-      <c r="H71" s="26"/>
-      <c r="I71" s="26"/>
-      <c r="J71" s="26"/>
+      <c r="H71" s="24"/>
+      <c r="I71" s="24"/>
+      <c r="J71" s="24"/>
       <c r="K71" s="4"/>
       <c r="L71" s="4"/>
       <c r="M71" s="4"/>
@@ -11873,16 +11964,16 @@
     </row>
     <row r="72" spans="1:25" ht="85" x14ac:dyDescent="0.2">
       <c r="A72" s="16"/>
-      <c r="B72" s="28" t="s">
+      <c r="B72" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C72" s="28" t="s">
+      <c r="C72" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D72" s="28" t="s">
+      <c r="D72" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E72" s="28" t="s">
+      <c r="E72" s="25" t="s">
         <v>3</v>
       </c>
       <c r="F72" s="14" t="s">
@@ -11891,13 +11982,13 @@
       <c r="G72" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H72" s="28" t="s">
+      <c r="H72" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I72" s="28" t="s">
+      <c r="I72" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="J72" s="28" t="s">
+      <c r="J72" s="25" t="s">
         <v>7</v>
       </c>
       <c r="M72" s="2" t="s">
@@ -12022,18 +12113,18 @@
       </c>
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A76" s="26"/>
-      <c r="B76" s="26"/>
-      <c r="C76" s="27" t="s">
+      <c r="A76" s="24"/>
+      <c r="B76" s="24"/>
+      <c r="C76" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="D76" s="27"/>
-      <c r="E76" s="27"/>
+      <c r="D76" s="30"/>
+      <c r="E76" s="30"/>
       <c r="F76" s="13"/>
       <c r="G76" s="13"/>
-      <c r="H76" s="26"/>
-      <c r="I76" s="26"/>
-      <c r="J76" s="26"/>
+      <c r="H76" s="24"/>
+      <c r="I76" s="24"/>
+      <c r="J76" s="24"/>
       <c r="K76" s="4"/>
       <c r="L76" s="4"/>
       <c r="M76" s="4"/>
@@ -12052,16 +12143,16 @@
     </row>
     <row r="77" spans="1:25" ht="85" x14ac:dyDescent="0.2">
       <c r="A77" s="16"/>
-      <c r="B77" s="28" t="s">
+      <c r="B77" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C77" s="28" t="s">
+      <c r="C77" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D77" s="28" t="s">
+      <c r="D77" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E77" s="28" t="s">
+      <c r="E77" s="25" t="s">
         <v>3</v>
       </c>
       <c r="F77" s="14" t="s">
@@ -12070,13 +12161,13 @@
       <c r="G77" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H77" s="28" t="s">
+      <c r="H77" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I77" s="28" t="s">
+      <c r="I77" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="J77" s="28" t="s">
+      <c r="J77" s="25" t="s">
         <v>7</v>
       </c>
       <c r="M77" s="2" t="s">

</xml_diff>

<commit_message>
The sbp-accuracy now shows the incremental improvement that has been so far achieved in subSeq; a quick memory estimation is attached in a spreadsheet for a new optimisation proposal
</commit_message>
<xml_diff>
--- a/sbp-accuracy-other-predictors.xlsx
+++ b/sbp-accuracy-other-predictors.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelktistakis/Repositories/sBP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelktistakis/Library/Containers/com.microsoft.Excel/Data/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF701E47-19DD-2E44-ACC3-733CF5E24CF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E72398A-863A-714C-9132-13F71309E7A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="460" windowWidth="38400" windowHeight="20060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16600" yWindow="4540" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="75">
   <si>
     <t>subSeq</t>
   </si>
@@ -235,7 +235,25 @@
     <t>*** subSeq has one single parameter (maxPredictionCount); this parameters was not tuned in this experiment; We might get better resutls if we tune it</t>
   </si>
   <si>
-    <t>subSeq (BWT implementation + wt_interval_scan + neighbour_scan_results_in_map + extra ranks correction)</t>
+    <t>/+Opt1: subSeq (keeping neighbour expansion results in map per query)</t>
+  </si>
+  <si>
+    <t>/+OPT1': subSeq bugfix in getting consequents; extra ranks removed</t>
+  </si>
+  <si>
+    <t>/+OPT2   : subSeq (scan uses sdsl::wt.interval_symbols)</t>
+  </si>
+  <si>
+    <t>/+OPT3   : subSeq (scan threshold between wt.interval_symbols &amp; loop access)</t>
+  </si>
+  <si>
+    <t>/+OPT4   : subSeq (LplusOne is used in getting consequents)</t>
+  </si>
+  <si>
+    <t>0.25 test base again</t>
+  </si>
+  <si>
+    <t>0.42 ???</t>
   </si>
 </sst>
 </file>
@@ -286,7 +304,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -311,8 +329,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -320,8 +344,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="941">
+  <cellStyleXfs count="949">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1263,8 +1302,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1314,6 +1361,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1327,7 +1382,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="941">
+  <cellStyles count="949">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1798,6 +1853,10 @@
     <cellStyle name="Followed Hyperlink" xfId="936" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="938" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="940" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="942" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="944" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="946" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="948" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2268,6 +2327,10 @@
     <cellStyle name="Hyperlink" xfId="935" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="937" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="939" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="941" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="943" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="945" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="947" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2394,7 +2457,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Y$2</c:f>
+              <c:f>Sheet1!$AC$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2473,7 +2536,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$Y$10,Sheet1!$Y$20,Sheet1!$Y$30,Sheet1!$Y$40,Sheet1!$Y$50,Sheet1!$Y$60,Sheet1!$Y$70)</c:f>
+              <c:f>(Sheet1!$AC$10,Sheet1!$AC$20,Sheet1!$AC$30,Sheet1!$AC$40,Sheet1!$AC$50,Sheet1!$AC$60,Sheet1!$AC$70)</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2512,7 +2575,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Z$2</c:f>
+              <c:f>Sheet1!$AD$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2591,7 +2654,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$Z$10,Sheet1!$Z$20,Sheet1!$Z$30,Sheet1!$Z$40,Sheet1!$Z$50,Sheet1!$Z$60,Sheet1!$Z$70)</c:f>
+              <c:f>(Sheet1!$AD$10,Sheet1!$AD$20,Sheet1!$AD$30,Sheet1!$AD$40,Sheet1!$AD$50,Sheet1!$AD$60,Sheet1!$AD$70)</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2634,11 +2697,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-29452320"/>
-        <c:axId val="30443104"/>
+        <c:axId val="-881482688"/>
+        <c:axId val="-886322928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-29452320"/>
+        <c:axId val="-881482688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2680,7 +2743,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30443104"/>
+        <c:crossAx val="-886322928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2688,7 +2751,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30443104"/>
+        <c:axId val="-886322928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2791,7 +2854,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-29452320"/>
+        <c:crossAx val="-881482688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3332,11 +3395,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="37624272"/>
-        <c:axId val="27581408"/>
+        <c:axId val="-881466048"/>
+        <c:axId val="-881463840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="37624272"/>
+        <c:axId val="-881466048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3378,7 +3441,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27581408"/>
+        <c:crossAx val="-881463840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3386,7 +3449,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="27581408"/>
+        <c:axId val="-881463840"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3437,7 +3500,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37624272"/>
+        <c:crossAx val="-881466048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4747,11 +4810,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="93112656"/>
-        <c:axId val="92349696"/>
+        <c:axId val="-881388784"/>
+        <c:axId val="-881386032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="93112656"/>
+        <c:axId val="-881388784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4793,7 +4856,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92349696"/>
+        <c:crossAx val="-881386032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4801,7 +4864,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92349696"/>
+        <c:axId val="-881386032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4880,7 +4943,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93112656"/>
+        <c:crossAx val="-881388784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6582,15 +6645,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>387350</xdr:colOff>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>196850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>91</xdr:row>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>92</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6618,13 +6681,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>61945</xdr:colOff>
       <xdr:row>93</xdr:row>
       <xdr:rowOff>133351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>40</xdr:col>
+      <xdr:col>44</xdr:col>
       <xdr:colOff>100045</xdr:colOff>
       <xdr:row>121</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6961,30 +7024,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z91"/>
+  <dimension ref="A1:AM91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="44" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="86" zoomScaleNormal="44" zoomScalePageLayoutView="44" workbookViewId="0">
+      <selection activeCell="R70" sqref="R70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="6" max="8" width="10.83203125" style="5"/>
-    <col min="20" max="20" width="13.5" customWidth="1"/>
+    <col min="6" max="12" width="10.83203125" style="5"/>
+    <col min="24" max="24" width="13.5" customWidth="1"/>
+    <col min="34" max="34" width="10.83203125" customWidth="1"/>
+    <col min="39" max="39" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="27" t="s">
+    <row r="1" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
       <c r="F1" s="9"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="20"/>
-    </row>
-    <row r="2" spans="1:26" ht="187" x14ac:dyDescent="0.2">
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="20"/>
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
+      <c r="AI1" s="29"/>
+      <c r="AJ1" s="29"/>
+      <c r="AK1" s="29"/>
+      <c r="AL1" s="29"/>
+      <c r="AM1" s="29"/>
+    </row>
+    <row r="2" spans="1:39" ht="153" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -7004,52 +7080,71 @@
         <v>68</v>
       </c>
       <c r="H2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG2" s="29"/>
+      <c r="AH2" s="29"/>
+      <c r="AI2" s="29"/>
+      <c r="AJ2" s="29"/>
+      <c r="AK2" s="29"/>
+      <c r="AL2" s="29"/>
+      <c r="AM2" s="29"/>
+    </row>
+    <row r="3" spans="1:39" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -7065,17 +7160,24 @@
       <c r="E3">
         <v>36.186</v>
       </c>
-      <c r="I3">
+      <c r="M3">
         <v>31.343</v>
       </c>
-      <c r="J3">
+      <c r="N3">
         <v>31.033999999999999</v>
       </c>
-      <c r="K3">
+      <c r="O3">
         <v>32.58</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG3" s="29"/>
+      <c r="AH3" s="29"/>
+      <c r="AI3" s="29"/>
+      <c r="AJ3" s="29"/>
+      <c r="AK3" s="29"/>
+      <c r="AL3" s="29"/>
+      <c r="AM3" s="29"/>
+    </row>
+    <row r="4" spans="1:39" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -7091,17 +7193,24 @@
       <c r="E4">
         <v>63.814</v>
       </c>
-      <c r="I4">
+      <c r="M4">
         <v>68.656999999999996</v>
       </c>
-      <c r="J4">
+      <c r="N4">
         <v>68.965999999999994</v>
       </c>
-      <c r="K4">
+      <c r="O4">
         <v>67.42</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG4" s="29"/>
+      <c r="AH4" s="29"/>
+      <c r="AI4" s="29"/>
+      <c r="AJ4" s="29"/>
+      <c r="AK4" s="29"/>
+      <c r="AL4" s="29"/>
+      <c r="AM4" s="29"/>
+    </row>
+    <row r="5" spans="1:39" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -7117,17 +7226,24 @@
       <c r="E5">
         <v>0.308</v>
       </c>
-      <c r="I5">
+      <c r="M5">
         <v>0.185</v>
       </c>
-      <c r="J5">
+      <c r="N5">
         <v>0.185</v>
       </c>
-      <c r="K5">
+      <c r="O5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG5" s="29"/>
+      <c r="AH5" s="29"/>
+      <c r="AI5" s="29"/>
+      <c r="AJ5" s="29"/>
+      <c r="AK5" s="29"/>
+      <c r="AL5" s="29"/>
+      <c r="AM5" s="29"/>
+    </row>
+    <row r="6" spans="1:39" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -7143,17 +7259,24 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="I6">
+      <c r="M6">
         <v>0</v>
       </c>
-      <c r="J6">
+      <c r="N6">
         <v>0</v>
       </c>
-      <c r="K6">
+      <c r="O6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AG6" s="29"/>
+      <c r="AH6" s="29"/>
+      <c r="AI6" s="29"/>
+      <c r="AJ6" s="29"/>
+      <c r="AK6" s="29"/>
+      <c r="AL6" s="29"/>
+      <c r="AM6" s="29"/>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -7173,20 +7296,31 @@
         <v>33</v>
       </c>
       <c r="G7" s="12"/>
-      <c r="H7" s="11">
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="11">
         <v>0.19</v>
       </c>
-      <c r="I7" s="16">
+      <c r="M7" s="16">
         <v>30</v>
       </c>
-      <c r="J7" s="16">
+      <c r="N7" s="16">
         <v>30.975999999999999</v>
       </c>
-      <c r="K7" s="16">
+      <c r="O7" s="16">
         <v>32.58</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AG7" s="29"/>
+      <c r="AH7" s="29"/>
+      <c r="AI7" s="29"/>
+      <c r="AJ7" s="29"/>
+      <c r="AK7" s="29"/>
+      <c r="AL7" s="29"/>
+      <c r="AM7" s="29"/>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -7206,23 +7340,36 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="G8" s="11"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="10">
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="L8" s="21"/>
+      <c r="M8" s="10">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="J8" s="10">
+      <c r="N8" s="10">
         <v>1.07</v>
       </c>
-      <c r="K8" s="10">
+      <c r="O8" s="10">
         <v>0.23</v>
       </c>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10">
+      <c r="R8" s="10"/>
+      <c r="S8" s="10">
         <f>D8/F8</f>
         <v>2.6428571428571428</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG8" s="29"/>
+      <c r="AH8" s="29"/>
+      <c r="AI8" s="29"/>
+      <c r="AJ8" s="29"/>
+      <c r="AK8" s="29"/>
+      <c r="AL8" s="29"/>
+      <c r="AM8" s="29"/>
+    </row>
+    <row r="9" spans="1:39" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -7240,20 +7387,31 @@
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="10">
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J9" s="10">
+      <c r="N9" s="10">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="K9" s="10">
+      <c r="O9" s="10">
         <v>1.4E-2</v>
       </c>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="AG9" s="29"/>
+      <c r="AH9" s="29"/>
+      <c r="AI9" s="29"/>
+      <c r="AJ9" s="29"/>
+      <c r="AK9" s="29"/>
+      <c r="AL9" s="29"/>
+      <c r="AM9" s="29"/>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -7274,68 +7432,102 @@
         <v>3210</v>
       </c>
       <c r="G10" s="12">
-        <f>0.56*1000</f>
-        <v>560</v>
+        <f>0.89*1000</f>
+        <v>890</v>
       </c>
       <c r="H10" s="12">
+        <f>0.889*1000</f>
+        <v>889</v>
+      </c>
+      <c r="I10" s="12">
+        <f>0.6*1000</f>
+        <v>600</v>
+      </c>
+      <c r="J10" s="12">
+        <f>0.59*1000</f>
+        <v>590</v>
+      </c>
+      <c r="K10" s="12">
+        <f>0.57*1000</f>
+        <v>570</v>
+      </c>
+      <c r="L10" s="12">
         <f>370.903*1000</f>
         <v>370903</v>
       </c>
-      <c r="I10" s="10">
+      <c r="M10" s="10">
         <v>0.35</v>
       </c>
-      <c r="J10" s="10">
+      <c r="N10" s="10">
         <v>1.21</v>
       </c>
-      <c r="K10" s="10">
+      <c r="O10" s="10">
         <v>3.14</v>
       </c>
-      <c r="N10" s="10">
-        <f>F10/D10</f>
-        <v>23.516483516483518</v>
-      </c>
-      <c r="O10" s="10"/>
-      <c r="Q10">
+      <c r="R10" s="10">
+        <f>J10/D10</f>
+        <v>4.3223443223443221</v>
+      </c>
+      <c r="S10" s="10"/>
+      <c r="U10">
         <v>54979</v>
       </c>
-      <c r="R10">
+      <c r="V10">
         <v>12</v>
       </c>
-      <c r="S10">
+      <c r="W10">
         <v>494</v>
       </c>
-      <c r="T10">
+      <c r="X10">
         <v>4518</v>
       </c>
-      <c r="U10">
+      <c r="Y10">
         <v>347</v>
       </c>
-      <c r="V10">
+      <c r="Z10">
         <v>5</v>
       </c>
-      <c r="W10">
+      <c r="AA10">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="Y10" s="10">
-        <f>F8/W10</f>
+      <c r="AC10" s="10">
+        <f>F8/AA10</f>
         <v>2.2950819672131151</v>
       </c>
-      <c r="Z10" s="10">
-        <f>D8/W10</f>
+      <c r="AD10" s="10">
+        <f>D8/AA10</f>
         <v>6.0655737704918034</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="28" t="s">
+      <c r="AG10" s="29"/>
+      <c r="AH10" s="29"/>
+      <c r="AI10" s="29"/>
+      <c r="AJ10" s="29"/>
+      <c r="AK10" s="29"/>
+      <c r="AL10" s="29"/>
+      <c r="AM10" s="30"/>
+    </row>
+    <row r="11" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
-    </row>
-    <row r="12" spans="1:26" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="AG11" s="29"/>
+      <c r="AH11" s="29"/>
+      <c r="AI11" s="29"/>
+      <c r="AJ11" s="29"/>
+      <c r="AK11" s="29"/>
+      <c r="AL11" s="29"/>
+      <c r="AM11" s="30"/>
+    </row>
+    <row r="12" spans="1:39" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
         <v>2</v>
       </c>
@@ -7352,20 +7544,31 @@
         <v>0</v>
       </c>
       <c r="G12" s="14"/>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="M12" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="N12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K12" s="6" t="s">
+      <c r="O12" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG12" s="29"/>
+      <c r="AH12" s="29"/>
+      <c r="AI12" s="29"/>
+      <c r="AJ12" s="29"/>
+      <c r="AK12" s="29"/>
+      <c r="AL12" s="29"/>
+      <c r="AM12" s="30"/>
+    </row>
+    <row r="13" spans="1:39" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -7384,17 +7587,28 @@
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
-      <c r="I13">
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13">
         <v>4.1100000000000003</v>
       </c>
-      <c r="J13">
+      <c r="N13">
         <v>8.2189999999999994</v>
       </c>
-      <c r="K13">
+      <c r="O13">
         <v>5.4790000000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG13" s="29"/>
+      <c r="AH13" s="29"/>
+      <c r="AI13" s="29"/>
+      <c r="AJ13" s="29"/>
+      <c r="AK13" s="29"/>
+      <c r="AL13" s="29"/>
+      <c r="AM13" s="30"/>
+    </row>
+    <row r="14" spans="1:39" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -7413,17 +7627,28 @@
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
-      <c r="I14">
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14">
         <v>95.89</v>
       </c>
-      <c r="J14">
+      <c r="N14">
         <v>91.781000000000006</v>
       </c>
-      <c r="K14">
+      <c r="O14">
         <v>94.521000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG14" s="29"/>
+      <c r="AH14" s="29"/>
+      <c r="AI14" s="29"/>
+      <c r="AJ14" s="29"/>
+      <c r="AK14" s="29"/>
+      <c r="AL14" s="29"/>
+      <c r="AM14" s="30"/>
+    </row>
+    <row r="15" spans="1:39" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -7442,17 +7667,28 @@
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
-      <c r="I15">
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15">
         <v>0</v>
       </c>
-      <c r="J15">
+      <c r="N15">
         <v>0</v>
       </c>
-      <c r="K15">
+      <c r="O15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG15" s="29"/>
+      <c r="AH15" s="29"/>
+      <c r="AI15" s="29"/>
+      <c r="AJ15" s="29"/>
+      <c r="AK15" s="29"/>
+      <c r="AL15" s="29"/>
+      <c r="AM15" s="30"/>
+    </row>
+    <row r="16" spans="1:39" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -7471,17 +7707,28 @@
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
-      <c r="I16">
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16">
         <v>0</v>
       </c>
-      <c r="J16">
+      <c r="N16">
         <v>0</v>
       </c>
-      <c r="K16">
+      <c r="O16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AG16" s="29"/>
+      <c r="AH16" s="29"/>
+      <c r="AI16" s="29"/>
+      <c r="AJ16" s="29"/>
+      <c r="AK16" s="29"/>
+      <c r="AL16" s="29"/>
+      <c r="AM16" s="30"/>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -7501,20 +7748,31 @@
         <v>23</v>
       </c>
       <c r="G17" s="12"/>
-      <c r="H17" s="12">
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12">
         <v>3.64</v>
       </c>
-      <c r="I17" s="16">
+      <c r="M17" s="16">
         <v>4.1100000000000003</v>
       </c>
-      <c r="J17" s="16">
+      <c r="N17" s="16">
         <v>7</v>
       </c>
-      <c r="K17" s="16">
+      <c r="O17" s="16">
         <v>5.4790000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG17" s="29"/>
+      <c r="AH17" s="29"/>
+      <c r="AI17" s="29"/>
+      <c r="AJ17" s="29"/>
+      <c r="AK17" s="29"/>
+      <c r="AL17" s="29"/>
+      <c r="AM17" s="30"/>
+    </row>
+    <row r="18" spans="1:39" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -7534,22 +7792,35 @@
         <v>0.22</v>
       </c>
       <c r="G18" s="11"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="10">
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11">
+        <v>0.46</v>
+      </c>
+      <c r="L18" s="21"/>
+      <c r="M18" s="10">
         <v>0.12</v>
       </c>
-      <c r="J18" s="10">
+      <c r="N18" s="10">
         <v>2.7</v>
       </c>
-      <c r="K18" s="10">
+      <c r="O18" s="10">
         <v>0.36</v>
       </c>
-      <c r="O18" s="10">
+      <c r="S18" s="10">
         <f>D18/F18</f>
         <v>0.17272727272727273</v>
       </c>
-    </row>
-    <row r="19" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG18" s="29"/>
+      <c r="AH18" s="29"/>
+      <c r="AI18" s="29"/>
+      <c r="AJ18" s="29"/>
+      <c r="AK18" s="29"/>
+      <c r="AL18" s="29"/>
+      <c r="AM18" s="30"/>
+    </row>
+    <row r="19" spans="1:39" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -7567,18 +7838,29 @@
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="10">
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="10">
         <v>2E-3</v>
       </c>
-      <c r="J19" s="10">
+      <c r="N19" s="10">
         <v>0.16900000000000001</v>
       </c>
-      <c r="K19" s="10">
+      <c r="O19" s="10">
         <v>2.4E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG19" s="29"/>
+      <c r="AH19" s="29"/>
+      <c r="AI19" s="29"/>
+      <c r="AJ19" s="29"/>
+      <c r="AK19" s="29"/>
+      <c r="AL19" s="29"/>
+      <c r="AM19" s="30"/>
+    </row>
+    <row r="20" spans="1:39" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -7599,67 +7881,101 @@
         <v>1690</v>
       </c>
       <c r="G20" s="12">
-        <f>0.4*1000</f>
-        <v>400</v>
+        <f>0.65*1000</f>
+        <v>650</v>
       </c>
       <c r="H20" s="12">
+        <f>0.65*1000</f>
+        <v>650</v>
+      </c>
+      <c r="I20" s="12">
+        <f>0.42*1000</f>
+        <v>420</v>
+      </c>
+      <c r="J20" s="12">
+        <f>0.42*1000</f>
+        <v>420</v>
+      </c>
+      <c r="K20" s="12">
+        <f>0.42*1000</f>
+        <v>420</v>
+      </c>
+      <c r="L20" s="12">
         <f>0.35*1000</f>
         <v>350</v>
       </c>
-      <c r="I20" s="10">
+      <c r="M20" s="10">
         <v>0.28000000000000003</v>
       </c>
-      <c r="J20" s="10">
+      <c r="N20" s="10">
         <v>0.42</v>
       </c>
-      <c r="K20" s="10">
+      <c r="O20" s="10">
         <v>2.14</v>
       </c>
-      <c r="N20" s="18">
-        <f>F20/D20</f>
-        <v>52.128315854410857</v>
-      </c>
-      <c r="Q20">
+      <c r="R20" s="10">
+        <f>J20/D20</f>
+        <v>12.954966070326957</v>
+      </c>
+      <c r="U20">
         <v>63586</v>
       </c>
-      <c r="R20">
+      <c r="V20">
         <v>93</v>
       </c>
-      <c r="S20">
+      <c r="W20">
         <v>266</v>
       </c>
-      <c r="T20">
+      <c r="X20">
         <v>678</v>
       </c>
-      <c r="U20">
+      <c r="Y20">
         <v>52</v>
       </c>
-      <c r="V20">
+      <c r="Z20">
         <v>7</v>
       </c>
-      <c r="W20">
+      <c r="AA20">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="Y20" s="10">
-        <f>F18/W20</f>
+      <c r="AC20" s="10">
+        <f>F18/AA20</f>
         <v>3.098591549295775</v>
       </c>
-      <c r="Z20" s="10">
-        <f>D18/W20</f>
+      <c r="AD20" s="10">
+        <f>D18/AA20</f>
         <v>0.53521126760563387</v>
       </c>
-    </row>
-    <row r="21" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C21" s="29" t="s">
+      <c r="AG20" s="29"/>
+      <c r="AH20" s="29"/>
+      <c r="AI20" s="29"/>
+      <c r="AJ20" s="29"/>
+      <c r="AK20" s="29"/>
+      <c r="AL20" s="29"/>
+      <c r="AM20" s="30"/>
+    </row>
+    <row r="21" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C21" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
-    </row>
-    <row r="22" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="AG21" s="29"/>
+      <c r="AH21" s="29"/>
+      <c r="AI21" s="29"/>
+      <c r="AJ21" s="29"/>
+      <c r="AK21" s="29"/>
+      <c r="AL21" s="29"/>
+      <c r="AM21" s="30"/>
+    </row>
+    <row r="22" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
         <v>2</v>
       </c>
@@ -7676,20 +7992,31 @@
         <v>0</v>
       </c>
       <c r="G22" s="14"/>
-      <c r="H22" s="14" t="s">
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="M22" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="N22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K22" s="3" t="s">
+      <c r="O22" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG22" s="29"/>
+      <c r="AH22" s="29"/>
+      <c r="AI22" s="29"/>
+      <c r="AJ22" s="29"/>
+      <c r="AK22" s="29"/>
+      <c r="AL22" s="29"/>
+      <c r="AM22" s="30"/>
+    </row>
+    <row r="23" spans="1:39" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -7708,17 +8035,28 @@
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
-      <c r="I23">
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23">
         <v>38.06</v>
       </c>
-      <c r="J23">
+      <c r="N23">
         <v>47.38</v>
       </c>
-      <c r="K23">
+      <c r="O23">
         <v>43.3</v>
       </c>
-    </row>
-    <row r="24" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG23" s="29"/>
+      <c r="AH23" s="29"/>
+      <c r="AI23" s="29"/>
+      <c r="AJ23" s="29"/>
+      <c r="AK23" s="29"/>
+      <c r="AL23" s="29"/>
+      <c r="AM23" s="30"/>
+    </row>
+    <row r="24" spans="1:39" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -7737,17 +8075,28 @@
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
-      <c r="I24">
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24">
         <v>61.94</v>
       </c>
-      <c r="J24">
+      <c r="N24">
         <v>52.62</v>
       </c>
-      <c r="K24">
+      <c r="O24">
         <v>56.7</v>
       </c>
-    </row>
-    <row r="25" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG24" s="29"/>
+      <c r="AH24" s="29"/>
+      <c r="AI24" s="29"/>
+      <c r="AJ24" s="29"/>
+      <c r="AK24" s="29"/>
+      <c r="AL24" s="29"/>
+      <c r="AM24" s="30"/>
+    </row>
+    <row r="25" spans="1:39" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -7766,17 +8115,28 @@
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
-      <c r="I25">
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25">
         <v>0</v>
       </c>
-      <c r="J25">
+      <c r="N25">
         <v>0</v>
       </c>
-      <c r="K25">
+      <c r="O25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG25" s="29"/>
+      <c r="AH25" s="29"/>
+      <c r="AI25" s="29"/>
+      <c r="AJ25" s="29"/>
+      <c r="AK25" s="29"/>
+      <c r="AL25" s="29"/>
+      <c r="AM25" s="30"/>
+    </row>
+    <row r="26" spans="1:39" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -7795,17 +8155,28 @@
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
       <c r="H26" s="12"/>
-      <c r="I26">
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26">
         <v>0</v>
       </c>
-      <c r="J26">
+      <c r="N26">
         <v>0</v>
       </c>
-      <c r="K26">
+      <c r="O26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AG26" s="29"/>
+      <c r="AH26" s="29"/>
+      <c r="AI26" s="29"/>
+      <c r="AJ26" s="29"/>
+      <c r="AK26" s="29"/>
+      <c r="AL26" s="29"/>
+      <c r="AM26" s="30"/>
+    </row>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -7825,20 +8196,31 @@
         <v>64</v>
       </c>
       <c r="G27" s="12"/>
-      <c r="H27" s="12">
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12">
         <v>29.57</v>
       </c>
-      <c r="I27" s="16">
+      <c r="M27" s="16">
         <v>38.06</v>
       </c>
-      <c r="J27" s="16">
+      <c r="N27" s="16">
         <v>48</v>
       </c>
-      <c r="K27" s="16">
+      <c r="O27" s="16">
         <v>43.3</v>
       </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AG27" s="29"/>
+      <c r="AH27" s="29"/>
+      <c r="AI27" s="29"/>
+      <c r="AJ27" s="29"/>
+      <c r="AK27" s="29"/>
+      <c r="AL27" s="29"/>
+      <c r="AM27" s="30"/>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -7858,22 +8240,35 @@
         <v>0.2</v>
       </c>
       <c r="G28" s="11"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="17">
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="L28" s="21"/>
+      <c r="M28" s="17">
         <v>2E-3</v>
       </c>
-      <c r="J28" s="10">
+      <c r="N28" s="10">
         <v>0.43</v>
       </c>
-      <c r="K28" s="10">
+      <c r="O28" s="10">
         <v>0.13</v>
       </c>
-      <c r="O28" s="10">
+      <c r="S28" s="10">
         <f>D28/F28</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG28" s="29"/>
+      <c r="AH28" s="29"/>
+      <c r="AI28" s="29"/>
+      <c r="AJ28" s="29"/>
+      <c r="AK28" s="29"/>
+      <c r="AL28" s="29"/>
+      <c r="AM28" s="30"/>
+    </row>
+    <row r="29" spans="1:39" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -7892,17 +8287,28 @@
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
       <c r="H29" s="12"/>
-      <c r="I29" s="10">
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="10">
         <v>1E-3</v>
       </c>
-      <c r="J29" s="10">
+      <c r="N29" s="10">
         <v>0.03</v>
       </c>
-      <c r="K29" s="10">
+      <c r="O29" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AG29" s="29"/>
+      <c r="AH29" s="29"/>
+      <c r="AI29" s="29"/>
+      <c r="AJ29" s="29"/>
+      <c r="AK29" s="29"/>
+      <c r="AL29" s="29"/>
+      <c r="AM29" s="30"/>
+    </row>
+    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -7923,67 +8329,101 @@
         <v>800</v>
       </c>
       <c r="G30" s="12">
+        <f>0.174*1000</f>
+        <v>174</v>
+      </c>
+      <c r="H30" s="12">
+        <f>0.15*1000</f>
+        <v>150</v>
+      </c>
+      <c r="I30" s="12">
+        <f>0.118*1000</f>
+        <v>118</v>
+      </c>
+      <c r="J30" s="12">
+        <f>0.119*1000</f>
+        <v>119</v>
+      </c>
+      <c r="K30" s="12">
+        <f>0.104*1000</f>
+        <v>104</v>
+      </c>
+      <c r="L30" s="12">
         <f>0.11*1000</f>
         <v>110</v>
       </c>
-      <c r="H30" s="12">
-        <f>0.11*1000</f>
-        <v>110</v>
-      </c>
-      <c r="I30" s="10">
+      <c r="M30" s="10">
         <v>0</v>
       </c>
-      <c r="J30" s="10">
+      <c r="N30" s="10">
         <v>0.64</v>
       </c>
-      <c r="K30" s="10">
+      <c r="O30" s="10">
         <v>3.07</v>
       </c>
-      <c r="N30" s="10">
-        <f>F30/D30</f>
-        <v>16.096579476861166</v>
-      </c>
-      <c r="Q30">
+      <c r="R30" s="10">
+        <f>J30/D30</f>
+        <v>2.3943661971830985</v>
+      </c>
+      <c r="U30">
         <v>54727</v>
       </c>
-      <c r="R30">
+      <c r="V30">
         <v>11</v>
       </c>
-      <c r="S30">
+      <c r="W30">
         <v>18</v>
       </c>
-      <c r="T30">
+      <c r="X30">
         <v>4643</v>
       </c>
-      <c r="U30">
+      <c r="Y30">
         <v>357</v>
       </c>
-      <c r="V30">
+      <c r="Z30">
         <v>5</v>
       </c>
-      <c r="W30" s="17">
+      <c r="AA30" s="17">
         <v>3.4200000000000001E-2</v>
       </c>
-      <c r="Y30" s="10">
-        <f>F28/W30</f>
+      <c r="AC30" s="10">
+        <f>F28/AA30</f>
         <v>5.8479532163742691</v>
       </c>
-      <c r="Z30" s="10">
-        <f>D28/W30</f>
+      <c r="AD30" s="10">
+        <f>D28/AA30</f>
         <v>2.9239766081871346</v>
       </c>
-    </row>
-    <row r="31" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C31" s="27" t="s">
+      <c r="AG30" s="29"/>
+      <c r="AH30" s="29"/>
+      <c r="AI30" s="29"/>
+      <c r="AJ30" s="29"/>
+      <c r="AK30" s="29"/>
+      <c r="AL30" s="29"/>
+      <c r="AM30" s="30"/>
+    </row>
+    <row r="31" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C31" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
-    </row>
-    <row r="32" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="AG31" s="29"/>
+      <c r="AH31" s="29"/>
+      <c r="AI31" s="29"/>
+      <c r="AJ31" s="29"/>
+      <c r="AK31" s="29"/>
+      <c r="AL31" s="29"/>
+      <c r="AM31" s="30"/>
+    </row>
+    <row r="32" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
         <v>2</v>
       </c>
@@ -8000,20 +8440,31 @@
         <v>0</v>
       </c>
       <c r="G32" s="14"/>
-      <c r="H32" s="14" t="s">
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="I32" s="3" t="s">
+      <c r="M32" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J32" s="3" t="s">
+      <c r="N32" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K32" s="3" t="s">
+      <c r="O32" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG32" s="29"/>
+      <c r="AH32" s="29"/>
+      <c r="AI32" s="29"/>
+      <c r="AJ32" s="29"/>
+      <c r="AK32" s="29"/>
+      <c r="AL32" s="29"/>
+      <c r="AM32" s="30"/>
+    </row>
+    <row r="33" spans="1:39" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -8032,17 +8483,28 @@
       <c r="F33" s="12"/>
       <c r="G33" s="12"/>
       <c r="H33" s="12"/>
-      <c r="I33">
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33">
         <v>11.561</v>
       </c>
-      <c r="J33">
+      <c r="N33">
         <v>31.068999999999999</v>
       </c>
-      <c r="K33">
+      <c r="O33">
         <v>17.13</v>
       </c>
-    </row>
-    <row r="34" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG33" s="29"/>
+      <c r="AH33" s="29"/>
+      <c r="AI33" s="29"/>
+      <c r="AJ33" s="29"/>
+      <c r="AK33" s="29"/>
+      <c r="AL33" s="29"/>
+      <c r="AM33" s="30"/>
+    </row>
+    <row r="34" spans="1:39" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -8061,17 +8523,28 @@
       <c r="F34" s="12"/>
       <c r="G34" s="12"/>
       <c r="H34" s="12"/>
-      <c r="I34">
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34">
         <v>88.438999999999993</v>
       </c>
-      <c r="J34">
+      <c r="N34">
         <v>68.930999999999997</v>
       </c>
-      <c r="K34">
+      <c r="O34">
         <v>82.87</v>
       </c>
-    </row>
-    <row r="35" spans="1:26" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG34" s="29"/>
+      <c r="AH34" s="29"/>
+      <c r="AI34" s="29"/>
+      <c r="AJ34" s="29"/>
+      <c r="AK34" s="29"/>
+      <c r="AL34" s="29"/>
+      <c r="AM34" s="30"/>
+    </row>
+    <row r="35" spans="1:39" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -8090,17 +8563,28 @@
       <c r="F35" s="12"/>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
-      <c r="I35">
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35">
         <v>1.804</v>
       </c>
-      <c r="J35">
+      <c r="N35">
         <v>1.804</v>
       </c>
-      <c r="K35">
+      <c r="O35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AG35" s="29"/>
+      <c r="AH35" s="29"/>
+      <c r="AI35" s="29"/>
+      <c r="AJ35" s="29"/>
+      <c r="AK35" s="29"/>
+      <c r="AL35" s="29"/>
+      <c r="AM35" s="30"/>
+    </row>
+    <row r="36" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -8119,17 +8603,28 @@
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
-      <c r="I36">
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36">
         <v>0</v>
       </c>
-      <c r="J36">
+      <c r="N36">
         <v>0</v>
       </c>
-      <c r="K36">
+      <c r="O36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AG36" s="29"/>
+      <c r="AH36" s="29"/>
+      <c r="AI36" s="29"/>
+      <c r="AJ36" s="29"/>
+      <c r="AK36" s="29"/>
+      <c r="AL36" s="29"/>
+      <c r="AM36" s="30"/>
+    </row>
+    <row r="37" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -8149,20 +8644,31 @@
         <v>29</v>
       </c>
       <c r="G37" s="12"/>
-      <c r="H37" s="12">
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="12">
         <v>2.1800000000000002</v>
       </c>
-      <c r="I37" s="16">
+      <c r="M37" s="16">
         <v>11.352</v>
       </c>
-      <c r="J37" s="16">
+      <c r="N37" s="16">
         <v>32</v>
       </c>
-      <c r="K37" s="16">
+      <c r="O37" s="16">
         <v>18</v>
       </c>
-    </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AG37" s="29"/>
+      <c r="AH37" s="29"/>
+      <c r="AI37" s="29"/>
+      <c r="AJ37" s="29"/>
+      <c r="AK37" s="29"/>
+      <c r="AL37" s="29"/>
+      <c r="AM37" s="30"/>
+    </row>
+    <row r="38" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -8182,22 +8688,35 @@
         <v>0.26</v>
       </c>
       <c r="G38" s="11"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="10">
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="L38" s="21"/>
+      <c r="M38" s="10">
         <v>0.26</v>
       </c>
-      <c r="J38" s="10">
+      <c r="N38" s="10">
         <v>3.19</v>
       </c>
-      <c r="K38" s="10">
+      <c r="O38" s="10">
         <v>0.52</v>
       </c>
-      <c r="O38" s="10">
+      <c r="S38" s="10">
         <f>D38/F38</f>
         <v>6.5384615384615383</v>
       </c>
-    </row>
-    <row r="39" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AG38" s="29"/>
+      <c r="AH38" s="29"/>
+      <c r="AI38" s="29"/>
+      <c r="AJ38" s="29"/>
+      <c r="AK38" s="29"/>
+      <c r="AL38" s="29"/>
+      <c r="AM38" s="30"/>
+    </row>
+    <row r="39" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -8216,17 +8735,28 @@
       <c r="F39" s="12"/>
       <c r="G39" s="12"/>
       <c r="H39" s="12"/>
-      <c r="I39" s="10">
+      <c r="I39" s="12"/>
+      <c r="J39" s="12"/>
+      <c r="K39" s="12"/>
+      <c r="L39" s="12"/>
+      <c r="M39" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J39" s="10">
+      <c r="N39" s="10">
         <v>0.11700000000000001</v>
       </c>
-      <c r="K39" s="10">
+      <c r="O39" s="10">
         <v>3.6999999999999998E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AG39" s="29"/>
+      <c r="AH39" s="29"/>
+      <c r="AI39" s="29"/>
+      <c r="AJ39" s="29"/>
+      <c r="AK39" s="29"/>
+      <c r="AL39" s="29"/>
+      <c r="AM39" s="30"/>
+    </row>
+    <row r="40" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>23</v>
       </c>
@@ -8247,67 +8777,101 @@
         <v>590</v>
       </c>
       <c r="G40" s="12">
-        <f>0.31*1000</f>
-        <v>310</v>
+        <f>0.5*1000</f>
+        <v>500</v>
       </c>
       <c r="H40" s="12">
+        <f>0.46*1000</f>
+        <v>460</v>
+      </c>
+      <c r="I40" s="12">
+        <f>0.34*1000</f>
+        <v>340</v>
+      </c>
+      <c r="J40" s="12">
+        <f>0.33*1000</f>
+        <v>330</v>
+      </c>
+      <c r="K40" s="12">
+        <f>0.27*1000</f>
+        <v>270</v>
+      </c>
+      <c r="L40" s="12">
         <f>26.4*1000</f>
         <v>26400</v>
       </c>
-      <c r="I40" s="10">
+      <c r="M40" s="10">
         <v>1.07</v>
       </c>
-      <c r="J40" s="10">
+      <c r="N40" s="10">
         <v>0.92</v>
       </c>
-      <c r="K40" s="10">
+      <c r="O40" s="10">
         <v>17.920000000000002</v>
       </c>
-      <c r="N40" s="10">
-        <f>F40/D40</f>
-        <v>8.4989916450590606</v>
-      </c>
-      <c r="Q40">
+      <c r="R40" s="10">
+        <f>J40/D40</f>
+        <v>4.7536732929991352</v>
+      </c>
+      <c r="U40">
         <v>98575</v>
       </c>
-      <c r="R40">
+      <c r="V40">
         <v>21</v>
       </c>
-      <c r="S40">
+      <c r="W40">
         <v>5243</v>
       </c>
-      <c r="T40">
+      <c r="X40">
         <v>4581</v>
       </c>
-      <c r="U40">
+      <c r="Y40">
         <v>352</v>
       </c>
-      <c r="V40">
+      <c r="Z40">
         <v>3</v>
       </c>
-      <c r="W40">
+      <c r="AA40">
         <v>0.16</v>
       </c>
-      <c r="Y40" s="10">
-        <f>F38/W40</f>
+      <c r="AC40" s="10">
+        <f>F38/AA40</f>
         <v>1.625</v>
       </c>
-      <c r="Z40" s="10">
-        <f>D38/W40</f>
+      <c r="AD40" s="10">
+        <f>D38/AA40</f>
         <v>10.625</v>
       </c>
-    </row>
-    <row r="41" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C41" s="27" t="s">
+      <c r="AG40" s="29"/>
+      <c r="AH40" s="29"/>
+      <c r="AI40" s="29"/>
+      <c r="AJ40" s="29"/>
+      <c r="AK40" s="29"/>
+      <c r="AL40" s="29"/>
+      <c r="AM40" s="30"/>
+    </row>
+    <row r="41" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C41" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
-    </row>
-    <row r="42" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="AG41" s="29"/>
+      <c r="AH41" s="29"/>
+      <c r="AI41" s="29"/>
+      <c r="AJ41" s="29"/>
+      <c r="AK41" s="29"/>
+      <c r="AL41" s="29"/>
+      <c r="AM41" s="30"/>
+    </row>
+    <row r="42" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="B42" s="3" t="s">
         <v>2</v>
       </c>
@@ -8324,20 +8888,31 @@
         <v>0</v>
       </c>
       <c r="G42" s="14"/>
-      <c r="H42" s="14" t="s">
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="I42" s="3" t="s">
+      <c r="M42" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J42" s="3" t="s">
+      <c r="N42" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K42" s="3" t="s">
+      <c r="O42" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="43" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AG42" s="29"/>
+      <c r="AH42" s="29"/>
+      <c r="AI42" s="29"/>
+      <c r="AJ42" s="29"/>
+      <c r="AK42" s="29"/>
+      <c r="AL42" s="29"/>
+      <c r="AM42" s="30"/>
+    </row>
+    <row r="43" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>15</v>
       </c>
@@ -8356,17 +8931,28 @@
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
       <c r="H43" s="12"/>
-      <c r="I43">
+      <c r="I43" s="12"/>
+      <c r="J43" s="12"/>
+      <c r="K43" s="12"/>
+      <c r="L43" s="12"/>
+      <c r="M43">
         <v>16.12</v>
       </c>
-      <c r="J43">
+      <c r="N43">
         <v>80.599999999999994</v>
       </c>
-      <c r="K43">
+      <c r="O43">
         <v>64.239999999999995</v>
       </c>
-    </row>
-    <row r="44" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AG43" s="29"/>
+      <c r="AH43" s="29"/>
+      <c r="AI43" s="29"/>
+      <c r="AJ43" s="29"/>
+      <c r="AK43" s="29"/>
+      <c r="AL43" s="29"/>
+      <c r="AM43" s="30"/>
+    </row>
+    <row r="44" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>16</v>
       </c>
@@ -8385,17 +8971,28 @@
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
       <c r="H44" s="12"/>
-      <c r="I44">
+      <c r="I44" s="12"/>
+      <c r="J44" s="12"/>
+      <c r="K44" s="12"/>
+      <c r="L44" s="12"/>
+      <c r="M44">
         <v>83.88</v>
       </c>
-      <c r="J44">
+      <c r="N44">
         <v>19.399999999999999</v>
       </c>
-      <c r="K44">
+      <c r="O44">
         <v>35.76</v>
       </c>
-    </row>
-    <row r="45" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AG44" s="29"/>
+      <c r="AH44" s="29"/>
+      <c r="AI44" s="29"/>
+      <c r="AJ44" s="29"/>
+      <c r="AK44" s="29"/>
+      <c r="AL44" s="29"/>
+      <c r="AM44" s="30"/>
+    </row>
+    <row r="45" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -8414,17 +9011,28 @@
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
       <c r="H45" s="12"/>
-      <c r="I45">
+      <c r="I45" s="12"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="12"/>
+      <c r="L45" s="12"/>
+      <c r="M45">
         <v>0</v>
       </c>
-      <c r="J45">
+      <c r="N45">
         <v>0</v>
       </c>
-      <c r="K45">
+      <c r="O45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AG45" s="29"/>
+      <c r="AH45" s="29"/>
+      <c r="AI45" s="29"/>
+      <c r="AJ45" s="29"/>
+      <c r="AK45" s="29"/>
+      <c r="AL45" s="29"/>
+      <c r="AM45" s="30"/>
+    </row>
+    <row r="46" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>18</v>
       </c>
@@ -8443,17 +9051,28 @@
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
-      <c r="I46">
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="12"/>
+      <c r="L46" s="12"/>
+      <c r="M46">
         <v>0</v>
       </c>
-      <c r="J46">
+      <c r="N46">
         <v>0</v>
       </c>
-      <c r="K46">
+      <c r="O46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AG46" s="29"/>
+      <c r="AH46" s="29"/>
+      <c r="AI46" s="29"/>
+      <c r="AJ46" s="29"/>
+      <c r="AK46" s="29"/>
+      <c r="AL46" s="29"/>
+      <c r="AM46" s="30"/>
+    </row>
+    <row r="47" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>49</v>
       </c>
@@ -8473,20 +9092,31 @@
         <v>88</v>
       </c>
       <c r="G47" s="12"/>
-      <c r="H47" s="12">
+      <c r="H47" s="12"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="12"/>
+      <c r="K47" s="12"/>
+      <c r="L47" s="12">
         <v>6.24</v>
       </c>
-      <c r="I47" s="16">
+      <c r="M47" s="16">
         <v>16.12</v>
       </c>
-      <c r="J47" s="16">
+      <c r="N47" s="16">
         <v>80.599999999999994</v>
       </c>
-      <c r="K47" s="16">
+      <c r="O47" s="16">
         <v>65</v>
       </c>
-    </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AG47" s="29"/>
+      <c r="AH47" s="29"/>
+      <c r="AI47" s="29"/>
+      <c r="AJ47" s="29"/>
+      <c r="AK47" s="29"/>
+      <c r="AL47" s="29"/>
+      <c r="AM47" s="30"/>
+    </row>
+    <row r="48" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>19</v>
       </c>
@@ -8506,22 +9136,35 @@
         <v>0.15</v>
       </c>
       <c r="G48" s="11"/>
-      <c r="H48" s="21"/>
-      <c r="I48" s="10">
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11">
+        <v>0.31</v>
+      </c>
+      <c r="L48" s="21"/>
+      <c r="M48" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="J48" s="10">
+      <c r="N48" s="10">
         <v>1.68</v>
       </c>
-      <c r="K48" s="10">
+      <c r="O48" s="10">
         <v>1.39</v>
       </c>
-      <c r="O48" s="10">
+      <c r="S48" s="10">
         <f>D48/F48</f>
         <v>0.73333333333333339</v>
       </c>
-    </row>
-    <row r="49" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AG48" s="29"/>
+      <c r="AH48" s="29"/>
+      <c r="AI48" s="29"/>
+      <c r="AJ48" s="29"/>
+      <c r="AK48" s="29"/>
+      <c r="AL48" s="29"/>
+      <c r="AM48" s="30"/>
+    </row>
+    <row r="49" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>20</v>
       </c>
@@ -8540,17 +9183,28 @@
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
       <c r="H49" s="12"/>
-      <c r="I49" s="10">
+      <c r="I49" s="12"/>
+      <c r="J49" s="12"/>
+      <c r="K49" s="12"/>
+      <c r="L49" s="12"/>
+      <c r="M49" s="10">
         <v>1.6E-2</v>
       </c>
-      <c r="J49" s="10">
+      <c r="N49" s="10">
         <v>0.71699999999999997</v>
       </c>
-      <c r="K49" s="10">
+      <c r="O49" s="10">
         <v>0.158</v>
       </c>
-    </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AG49" s="29"/>
+      <c r="AH49" s="29"/>
+      <c r="AI49" s="29"/>
+      <c r="AJ49" s="29"/>
+      <c r="AK49" s="29"/>
+      <c r="AL49" s="29"/>
+      <c r="AM49" s="30"/>
+    </row>
+    <row r="50" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>23</v>
       </c>
@@ -8571,67 +9225,101 @@
         <v>430</v>
       </c>
       <c r="G50" s="12">
-        <f>0.08*1000</f>
-        <v>80</v>
+        <f>0.13*1000</f>
+        <v>130</v>
       </c>
       <c r="H50" s="12">
+        <f>0.125*1000</f>
+        <v>125</v>
+      </c>
+      <c r="I50" s="12">
+        <f>0.087*1000</f>
+        <v>87</v>
+      </c>
+      <c r="J50" s="12">
+        <f>0.085*1000</f>
+        <v>85</v>
+      </c>
+      <c r="K50" s="12">
+        <f>0.062*1000</f>
+        <v>62</v>
+      </c>
+      <c r="L50" s="12">
         <f xml:space="preserve"> 0.77*1000</f>
         <v>770</v>
       </c>
-      <c r="I50" s="10">
+      <c r="M50" s="10">
         <v>0.14000000000000001</v>
       </c>
-      <c r="J50" s="10">
+      <c r="N50" s="10">
         <v>0.21</v>
       </c>
-      <c r="K50" s="10">
+      <c r="O50" s="10">
         <v>4.1399999999999997</v>
       </c>
-      <c r="N50" s="10">
-        <f>F50/D50</f>
-        <v>27.388535031847134</v>
-      </c>
-      <c r="Q50">
+      <c r="R50" s="10">
+        <f>J50/D50</f>
+        <v>5.4140127388535033</v>
+      </c>
+      <c r="U50">
         <v>620521</v>
       </c>
-      <c r="R50">
+      <c r="V50">
         <v>133</v>
       </c>
-      <c r="S50">
+      <c r="W50">
         <v>75</v>
       </c>
-      <c r="T50">
+      <c r="X50">
         <v>4643</v>
       </c>
-      <c r="U50">
+      <c r="Y50">
         <v>357</v>
       </c>
-      <c r="V50">
+      <c r="Z50">
         <v>5</v>
       </c>
-      <c r="W50">
+      <c r="AA50">
         <v>0.54</v>
       </c>
-      <c r="Y50" s="10">
-        <f>F48/W50</f>
+      <c r="AC50" s="10">
+        <f>F48/AA50</f>
         <v>0.27777777777777773</v>
       </c>
-      <c r="Z50" s="10">
-        <f>D48/W50</f>
+      <c r="AD50" s="10">
+        <f>D48/AA50</f>
         <v>0.20370370370370369</v>
       </c>
-    </row>
-    <row r="51" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C51" s="27" t="s">
+      <c r="AG50" s="29"/>
+      <c r="AH50" s="29"/>
+      <c r="AI50" s="29"/>
+      <c r="AJ50" s="29"/>
+      <c r="AK50" s="29"/>
+      <c r="AL50" s="29"/>
+      <c r="AM50" s="30"/>
+    </row>
+    <row r="51" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C51" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D51" s="27"/>
-      <c r="E51" s="27"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="31"/>
       <c r="F51" s="13"/>
       <c r="G51" s="13"/>
       <c r="H51" s="13"/>
-    </row>
-    <row r="52" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="I51" s="13"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="13"/>
+      <c r="AG51" s="29"/>
+      <c r="AH51" s="29"/>
+      <c r="AI51" s="29"/>
+      <c r="AJ51" s="29"/>
+      <c r="AK51" s="29"/>
+      <c r="AL51" s="29"/>
+      <c r="AM51" s="30"/>
+    </row>
+    <row r="52" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="B52" s="3" t="s">
         <v>2</v>
       </c>
@@ -8648,20 +9336,31 @@
         <v>0</v>
       </c>
       <c r="G52" s="14"/>
-      <c r="H52" s="14" t="s">
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="14"/>
+      <c r="L52" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="I52" s="3" t="s">
+      <c r="M52" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J52" s="3" t="s">
+      <c r="N52" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K52" s="3" t="s">
+      <c r="O52" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="53" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AG52" s="29"/>
+      <c r="AH52" s="29"/>
+      <c r="AI52" s="29"/>
+      <c r="AJ52" s="29"/>
+      <c r="AK52" s="29"/>
+      <c r="AL52" s="29"/>
+      <c r="AM52" s="30"/>
+    </row>
+    <row r="53" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>15</v>
       </c>
@@ -8680,17 +9379,28 @@
       <c r="F53" s="12"/>
       <c r="G53" s="12"/>
       <c r="H53" s="12"/>
-      <c r="I53">
+      <c r="I53" s="12"/>
+      <c r="J53" s="12"/>
+      <c r="K53" s="12"/>
+      <c r="L53" s="12"/>
+      <c r="M53">
         <v>25.684999999999999</v>
       </c>
-      <c r="J53">
+      <c r="N53">
         <v>22.35</v>
       </c>
-      <c r="K53">
+      <c r="O53">
         <v>24.228999999999999</v>
       </c>
-    </row>
-    <row r="54" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AG53" s="29"/>
+      <c r="AH53" s="29"/>
+      <c r="AI53" s="29"/>
+      <c r="AJ53" s="29"/>
+      <c r="AK53" s="29"/>
+      <c r="AL53" s="29"/>
+      <c r="AM53" s="30"/>
+    </row>
+    <row r="54" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>16</v>
       </c>
@@ -8709,17 +9419,28 @@
       <c r="F54" s="12"/>
       <c r="G54" s="12"/>
       <c r="H54" s="12"/>
-      <c r="I54">
+      <c r="I54" s="12"/>
+      <c r="J54" s="12"/>
+      <c r="K54" s="12"/>
+      <c r="L54" s="12"/>
+      <c r="M54">
         <v>74.314999999999998</v>
       </c>
-      <c r="J54">
+      <c r="N54">
         <v>77.650000000000006</v>
       </c>
-      <c r="K54">
+      <c r="O54">
         <v>75.771000000000001</v>
       </c>
-    </row>
-    <row r="55" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AG54" s="29"/>
+      <c r="AH54" s="29"/>
+      <c r="AI54" s="29"/>
+      <c r="AJ54" s="29"/>
+      <c r="AK54" s="29"/>
+      <c r="AL54" s="29"/>
+      <c r="AM54" s="30"/>
+    </row>
+    <row r="55" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>17</v>
       </c>
@@ -8738,17 +9459,28 @@
       <c r="F55" s="12"/>
       <c r="G55" s="12"/>
       <c r="H55" s="12"/>
-      <c r="I55">
+      <c r="I55" s="12"/>
+      <c r="J55" s="12"/>
+      <c r="K55" s="12"/>
+      <c r="L55" s="12"/>
+      <c r="M55">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J55">
+      <c r="N55">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K55">
+      <c r="O55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AG55" s="29"/>
+      <c r="AH55" s="29"/>
+      <c r="AI55" s="29"/>
+      <c r="AJ55" s="29"/>
+      <c r="AK55" s="29"/>
+      <c r="AL55" s="29"/>
+      <c r="AM55" s="30"/>
+    </row>
+    <row r="56" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -8767,17 +9499,28 @@
       <c r="F56" s="12"/>
       <c r="G56" s="12"/>
       <c r="H56" s="12"/>
-      <c r="I56">
+      <c r="I56" s="12"/>
+      <c r="J56" s="12"/>
+      <c r="K56" s="12"/>
+      <c r="L56" s="12"/>
+      <c r="M56">
         <v>0</v>
       </c>
-      <c r="J56">
+      <c r="N56">
         <v>0</v>
       </c>
-      <c r="K56">
+      <c r="O56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AG56" s="29"/>
+      <c r="AH56" s="29"/>
+      <c r="AI56" s="29"/>
+      <c r="AJ56" s="29"/>
+      <c r="AK56" s="29"/>
+      <c r="AL56" s="29"/>
+      <c r="AM56" s="30"/>
+    </row>
+    <row r="57" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>49</v>
       </c>
@@ -8797,20 +9540,31 @@
         <v>34</v>
       </c>
       <c r="G57" s="12"/>
-      <c r="H57" s="22">
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="12"/>
+      <c r="K57" s="12"/>
+      <c r="L57" s="22">
         <v>0.6</v>
       </c>
-      <c r="I57" s="16">
+      <c r="M57" s="16">
         <v>23</v>
       </c>
-      <c r="J57" s="16">
+      <c r="N57" s="16">
         <v>20</v>
       </c>
-      <c r="K57" s="16">
+      <c r="O57" s="16">
         <v>20</v>
       </c>
-    </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AG57" s="29"/>
+      <c r="AH57" s="29"/>
+      <c r="AI57" s="29"/>
+      <c r="AJ57" s="29"/>
+      <c r="AK57" s="29"/>
+      <c r="AL57" s="29"/>
+      <c r="AM57" s="30"/>
+    </row>
+    <row r="58" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>19</v>
       </c>
@@ -8830,22 +9584,35 @@
         <v>2.25</v>
       </c>
       <c r="G58" s="11"/>
-      <c r="H58" s="21"/>
-      <c r="I58" s="10">
+      <c r="H58" s="11"/>
+      <c r="I58" s="11"/>
+      <c r="J58" s="11"/>
+      <c r="K58" s="11">
+        <v>4.91</v>
+      </c>
+      <c r="L58" s="21"/>
+      <c r="M58" s="10">
         <v>26</v>
       </c>
-      <c r="J58" s="10">
+      <c r="N58" s="10">
         <v>37.6</v>
       </c>
-      <c r="K58" s="10">
+      <c r="O58" s="10">
         <v>5.97</v>
       </c>
-      <c r="O58" s="10">
+      <c r="S58" s="10">
         <f>D58/F58</f>
         <v>44.48</v>
       </c>
-    </row>
-    <row r="59" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AG58" s="29"/>
+      <c r="AH58" s="29"/>
+      <c r="AI58" s="29"/>
+      <c r="AJ58" s="29"/>
+      <c r="AK58" s="29"/>
+      <c r="AL58" s="29"/>
+      <c r="AM58" s="30"/>
+    </row>
+    <row r="59" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>20</v>
       </c>
@@ -8864,17 +9631,28 @@
       <c r="F59" s="12"/>
       <c r="G59" s="12"/>
       <c r="H59" s="12"/>
-      <c r="I59" s="10">
+      <c r="I59" s="12"/>
+      <c r="J59" s="12"/>
+      <c r="K59" s="12"/>
+      <c r="L59" s="12"/>
+      <c r="M59" s="10">
         <v>0.16300000000000001</v>
       </c>
-      <c r="J59" s="10">
+      <c r="N59" s="10">
         <v>2.38</v>
       </c>
-      <c r="K59" s="10">
+      <c r="O59" s="10">
         <v>0.40400000000000003</v>
       </c>
-    </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AG59" s="29"/>
+      <c r="AH59" s="29"/>
+      <c r="AI59" s="29"/>
+      <c r="AJ59" s="29"/>
+      <c r="AK59" s="29"/>
+      <c r="AL59" s="29"/>
+      <c r="AM59" s="30"/>
+    </row>
+    <row r="60" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>23</v>
       </c>
@@ -8895,67 +9673,101 @@
         <v>344000</v>
       </c>
       <c r="G60" s="12">
-        <f>102*1000</f>
-        <v>102000</v>
+        <f>168.36*1000</f>
+        <v>168360</v>
       </c>
       <c r="H60" s="12">
+        <f>163.8*1000</f>
+        <v>163800</v>
+      </c>
+      <c r="I60" s="11">
+        <f>97.11*1000</f>
+        <v>97110</v>
+      </c>
+      <c r="J60" s="11">
+        <f>99*1000</f>
+        <v>99000</v>
+      </c>
+      <c r="K60" s="11">
+        <f>97*1000</f>
+        <v>97000</v>
+      </c>
+      <c r="L60" s="12">
         <f>1992.633*1000</f>
         <v>1992633</v>
       </c>
-      <c r="I60" s="10">
+      <c r="M60" s="10">
         <v>23.92</v>
       </c>
-      <c r="J60" s="10">
+      <c r="N60" s="10">
         <v>9.92</v>
       </c>
-      <c r="K60" s="10">
+      <c r="O60" s="10">
         <v>434</v>
       </c>
-      <c r="N60" s="10">
-        <f>F60/D60</f>
-        <v>57.42904841402337</v>
-      </c>
-      <c r="Q60">
+      <c r="R60" s="10">
+        <f>J60/D60</f>
+        <v>16.527545909849749</v>
+      </c>
+      <c r="U60">
         <v>1230568</v>
       </c>
-      <c r="R60">
+      <c r="V60">
         <v>29</v>
       </c>
-      <c r="S60">
+      <c r="W60">
         <v>22042</v>
       </c>
-      <c r="T60">
+      <c r="X60">
         <v>41786</v>
       </c>
-      <c r="U60">
+      <c r="Y60">
         <v>3214</v>
       </c>
-      <c r="V60">
+      <c r="Z60">
         <v>5</v>
       </c>
-      <c r="W60">
+      <c r="AA60">
         <v>2.2999999999999998</v>
       </c>
-      <c r="Y60" s="10">
-        <f>F58/W60</f>
+      <c r="AC60" s="10">
+        <f>F58/AA60</f>
         <v>0.97826086956521752</v>
       </c>
-      <c r="Z60" s="10">
-        <f>D58/W60</f>
+      <c r="AD60" s="10">
+        <f>D58/AA60</f>
         <v>43.513043478260869</v>
       </c>
-    </row>
-    <row r="61" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C61" s="27" t="s">
+      <c r="AG60" s="29"/>
+      <c r="AH60" s="29"/>
+      <c r="AI60" s="29"/>
+      <c r="AJ60" s="29"/>
+      <c r="AK60" s="29"/>
+      <c r="AL60" s="29"/>
+      <c r="AM60" s="30"/>
+    </row>
+    <row r="61" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C61" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="D61" s="27"/>
-      <c r="E61" s="27"/>
+      <c r="D61" s="31"/>
+      <c r="E61" s="31"/>
       <c r="F61" s="13"/>
       <c r="G61" s="13"/>
       <c r="H61" s="13"/>
-    </row>
-    <row r="62" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="I61" s="13"/>
+      <c r="J61" s="13"/>
+      <c r="K61" s="13"/>
+      <c r="L61" s="13"/>
+      <c r="AG61" s="29"/>
+      <c r="AH61" s="29"/>
+      <c r="AI61" s="29"/>
+      <c r="AJ61" s="29"/>
+      <c r="AK61" s="29"/>
+      <c r="AL61" s="29"/>
+      <c r="AM61" s="30"/>
+    </row>
+    <row r="62" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="B62" s="3" t="s">
         <v>2</v>
       </c>
@@ -8972,20 +9784,31 @@
         <v>0</v>
       </c>
       <c r="G62" s="14"/>
-      <c r="H62" s="14" t="s">
+      <c r="H62" s="14"/>
+      <c r="I62" s="14"/>
+      <c r="J62" s="14"/>
+      <c r="K62" s="14"/>
+      <c r="L62" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="I62" s="3" t="s">
+      <c r="M62" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J62" s="3" t="s">
+      <c r="N62" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K62" s="3" t="s">
+      <c r="O62" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="63" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AG62" s="29"/>
+      <c r="AH62" s="29"/>
+      <c r="AI62" s="29"/>
+      <c r="AJ62" s="29"/>
+      <c r="AK62" s="29"/>
+      <c r="AL62" s="29"/>
+      <c r="AM62" s="30"/>
+    </row>
+    <row r="63" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>15</v>
       </c>
@@ -9004,17 +9827,28 @@
       <c r="F63" s="12"/>
       <c r="G63" s="12"/>
       <c r="H63" s="12"/>
-      <c r="I63">
+      <c r="I63" s="12"/>
+      <c r="J63" s="12"/>
+      <c r="K63" s="12"/>
+      <c r="L63" s="12"/>
+      <c r="M63">
         <v>23.254000000000001</v>
       </c>
-      <c r="J63">
+      <c r="N63">
         <v>26.04</v>
       </c>
-      <c r="K63">
+      <c r="O63">
         <v>24.026</v>
       </c>
-    </row>
-    <row r="64" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AG63" s="29"/>
+      <c r="AH63" s="29"/>
+      <c r="AI63" s="29"/>
+      <c r="AJ63" s="29"/>
+      <c r="AK63" s="29"/>
+      <c r="AL63" s="29"/>
+      <c r="AM63" s="30"/>
+    </row>
+    <row r="64" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>16</v>
       </c>
@@ -9033,17 +9867,28 @@
       <c r="F64" s="12"/>
       <c r="G64" s="12"/>
       <c r="H64" s="12"/>
-      <c r="I64">
+      <c r="I64" s="12"/>
+      <c r="J64" s="12"/>
+      <c r="K64" s="12"/>
+      <c r="L64" s="12"/>
+      <c r="M64">
         <v>76.745999999999995</v>
       </c>
-      <c r="J64">
+      <c r="N64">
         <v>73.959999999999994</v>
       </c>
-      <c r="K64">
+      <c r="O64">
         <v>75.974000000000004</v>
       </c>
-    </row>
-    <row r="65" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AG64" s="29"/>
+      <c r="AH64" s="29"/>
+      <c r="AI64" s="29"/>
+      <c r="AJ64" s="29"/>
+      <c r="AK64" s="29"/>
+      <c r="AL64" s="29"/>
+      <c r="AM64" s="30"/>
+    </row>
+    <row r="65" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>17</v>
       </c>
@@ -9062,17 +9907,28 @@
       <c r="F65" s="12"/>
       <c r="G65" s="12"/>
       <c r="H65" s="12"/>
-      <c r="I65">
+      <c r="I65" s="12"/>
+      <c r="J65" s="12"/>
+      <c r="K65" s="12"/>
+      <c r="L65" s="12"/>
+      <c r="M65">
         <v>0.56000000000000005</v>
       </c>
-      <c r="J65">
+      <c r="N65">
         <v>0.56000000000000005</v>
       </c>
-      <c r="K65">
+      <c r="O65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AG65" s="29"/>
+      <c r="AH65" s="29"/>
+      <c r="AI65" s="29"/>
+      <c r="AJ65" s="29"/>
+      <c r="AK65" s="29"/>
+      <c r="AL65" s="29"/>
+      <c r="AM65" s="30"/>
+    </row>
+    <row r="66" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>18</v>
       </c>
@@ -9091,17 +9947,28 @@
       <c r="F66" s="12"/>
       <c r="G66" s="12"/>
       <c r="H66" s="12"/>
-      <c r="I66">
+      <c r="I66" s="12"/>
+      <c r="J66" s="12"/>
+      <c r="K66" s="12"/>
+      <c r="L66" s="12"/>
+      <c r="M66">
         <v>0.36</v>
       </c>
-      <c r="J66">
+      <c r="N66">
         <v>0.36</v>
       </c>
-      <c r="K66">
+      <c r="O66">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AG66" s="29"/>
+      <c r="AH66" s="29"/>
+      <c r="AI66" s="29"/>
+      <c r="AJ66" s="29"/>
+      <c r="AK66" s="29"/>
+      <c r="AL66" s="29"/>
+      <c r="AM66" s="30"/>
+    </row>
+    <row r="67" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>49</v>
       </c>
@@ -9121,20 +9988,31 @@
         <v>29</v>
       </c>
       <c r="G67" s="12"/>
-      <c r="H67" s="11">
+      <c r="H67" s="12"/>
+      <c r="I67" s="12"/>
+      <c r="J67" s="12"/>
+      <c r="K67" s="12"/>
+      <c r="L67" s="11">
         <v>0.38</v>
       </c>
-      <c r="I67" s="16">
+      <c r="M67" s="16">
         <v>23.04</v>
       </c>
-      <c r="J67" s="16">
+      <c r="N67" s="16">
         <v>25.8</v>
       </c>
-      <c r="K67" s="16">
+      <c r="O67" s="16">
         <v>25</v>
       </c>
-    </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AG67" s="29"/>
+      <c r="AH67" s="29"/>
+      <c r="AI67" s="29"/>
+      <c r="AJ67" s="29"/>
+      <c r="AK67" s="29"/>
+      <c r="AL67" s="29"/>
+      <c r="AM67" s="30"/>
+    </row>
+    <row r="68" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>19</v>
       </c>
@@ -9154,22 +10032,35 @@
         <v>0.61</v>
       </c>
       <c r="G68" s="11"/>
-      <c r="H68" s="21"/>
-      <c r="I68" s="10">
+      <c r="H68" s="11"/>
+      <c r="I68" s="11"/>
+      <c r="J68" s="11"/>
+      <c r="K68" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="L68" s="21"/>
+      <c r="M68" s="10">
         <v>0.32</v>
       </c>
-      <c r="J68" s="10">
+      <c r="N68" s="10">
         <v>6.52</v>
       </c>
-      <c r="K68" s="10">
+      <c r="O68" s="10">
         <v>1</v>
       </c>
-      <c r="O68" s="10">
+      <c r="S68" s="10">
         <f>D68/F68</f>
         <v>2.2295081967213117</v>
       </c>
-    </row>
-    <row r="69" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AG68" s="29"/>
+      <c r="AH68" s="29"/>
+      <c r="AI68" s="29"/>
+      <c r="AJ68" s="29"/>
+      <c r="AK68" s="29"/>
+      <c r="AL68" s="29"/>
+      <c r="AM68" s="30"/>
+    </row>
+    <row r="69" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>20</v>
       </c>
@@ -9188,17 +10079,28 @@
       <c r="F69" s="11"/>
       <c r="G69" s="11"/>
       <c r="H69" s="11"/>
-      <c r="I69" s="10">
+      <c r="I69" s="11"/>
+      <c r="J69" s="11"/>
+      <c r="K69" s="11"/>
+      <c r="L69" s="11"/>
+      <c r="M69" s="10">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="J69" s="10">
+      <c r="N69" s="10">
         <v>0.27400000000000002</v>
       </c>
-      <c r="K69" s="10">
+      <c r="O69" s="10">
         <v>4.1000000000000002E-2</v>
       </c>
-    </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AG69" s="29"/>
+      <c r="AH69" s="29"/>
+      <c r="AI69" s="29"/>
+      <c r="AJ69" s="29"/>
+      <c r="AK69" s="29"/>
+      <c r="AL69" s="29"/>
+      <c r="AM69" s="30"/>
+    </row>
+    <row r="70" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>23</v>
       </c>
@@ -9219,114 +10121,137 @@
         <v>6750</v>
       </c>
       <c r="G70" s="11">
-        <f>1.21*1000</f>
-        <v>1210</v>
-      </c>
-      <c r="H70" s="12">
+        <f>2.17*1000</f>
+        <v>2170</v>
+      </c>
+      <c r="H70" s="11">
+        <f>2.16*1000</f>
+        <v>2160</v>
+      </c>
+      <c r="I70" s="5">
+        <f>1.19*1000</f>
+        <v>1190</v>
+      </c>
+      <c r="J70" s="5">
+        <f>1.1*1000</f>
+        <v>1100</v>
+      </c>
+      <c r="K70" s="5">
+        <f>1.1*1000</f>
+        <v>1100</v>
+      </c>
+      <c r="L70" s="12">
         <f>18.143*1000</f>
         <v>18143</v>
       </c>
-      <c r="I70" s="10">
+      <c r="M70" s="10">
         <v>0.78</v>
       </c>
-      <c r="J70" s="10">
+      <c r="N70" s="10">
         <v>1</v>
       </c>
-      <c r="K70" s="10">
+      <c r="O70" s="10">
         <v>7.21</v>
       </c>
-      <c r="N70" s="10">
-        <f>F70/D70</f>
-        <v>103.5117313295507</v>
-      </c>
-      <c r="Q70">
+      <c r="R70" s="10">
+        <f>J70/D70</f>
+        <v>16.868578438889742</v>
+      </c>
+      <c r="U70">
         <v>190412</v>
       </c>
-      <c r="R70">
+      <c r="V70">
         <v>41</v>
       </c>
-      <c r="S70">
+      <c r="W70">
         <v>2591</v>
       </c>
-      <c r="T70">
+      <c r="X70">
         <v>4643</v>
       </c>
-      <c r="U70">
+      <c r="Y70">
         <v>355</v>
       </c>
-      <c r="V70">
+      <c r="Z70">
         <v>5</v>
       </c>
-      <c r="W70">
+      <c r="AA70">
         <v>0.28000000000000003</v>
       </c>
-      <c r="Y70" s="10">
-        <f>F68/W70</f>
+      <c r="AC70" s="10">
+        <f>F68/AA70</f>
         <v>2.1785714285714284</v>
       </c>
-      <c r="Z70" s="10">
-        <f>D68/W70</f>
+      <c r="AD70" s="10">
+        <f>D68/AA70</f>
         <v>4.8571428571428568</v>
       </c>
-    </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="T71" s="1"/>
-    </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="T72" s="1"/>
-    </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="T73" s="1"/>
-    </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="T74" s="1"/>
-    </row>
-    <row r="75" spans="1:26" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AG70" s="29"/>
+      <c r="AH70" s="29"/>
+      <c r="AI70" s="29"/>
+      <c r="AJ70" s="29"/>
+      <c r="AK70" s="29"/>
+      <c r="AL70" s="29"/>
+      <c r="AM70" s="30"/>
+    </row>
+    <row r="71" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="X71" s="1"/>
+    </row>
+    <row r="72" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="X72" s="1"/>
+    </row>
+    <row r="73" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="X73" s="1"/>
+    </row>
+    <row r="74" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="X74" s="1"/>
+    </row>
+    <row r="75" spans="1:39" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="C75" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="T75" s="19"/>
-    </row>
-    <row r="76" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+      <c r="X75" s="19"/>
+    </row>
+    <row r="76" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="D76" t="s">
         <v>24</v>
       </c>
-      <c r="I76" t="s">
+      <c r="M76" t="s">
         <v>26</v>
       </c>
-      <c r="T76" s="1"/>
-    </row>
-    <row r="77" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+      <c r="X76" s="1"/>
+    </row>
+    <row r="77" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="D77">
         <v>75</v>
       </c>
       <c r="E77" t="s">
         <v>33</v>
       </c>
-      <c r="I77">
+      <c r="M77">
         <v>625</v>
       </c>
-      <c r="J77" t="s">
+      <c r="N77" t="s">
         <v>28</v>
       </c>
-      <c r="T77" s="1"/>
-    </row>
-    <row r="78" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+      <c r="X77" s="1"/>
+    </row>
+    <row r="78" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="D78">
         <v>64</v>
       </c>
       <c r="E78" t="s">
         <v>32</v>
       </c>
-      <c r="I78">
+      <c r="M78">
         <v>122</v>
       </c>
-      <c r="J78" t="s">
+      <c r="N78" t="s">
         <v>29</v>
       </c>
-      <c r="T78" s="1"/>
-    </row>
-    <row r="79" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+      <c r="X78" s="1"/>
+    </row>
+    <row r="79" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="D79">
         <f>12*8*8</f>
         <v>768</v>
@@ -9334,16 +10259,16 @@
       <c r="E79" t="s">
         <v>31</v>
       </c>
-      <c r="I79">
+      <c r="M79">
         <f>32+75*4*8</f>
         <v>2432</v>
       </c>
-      <c r="J79" t="s">
+      <c r="N79" t="s">
         <v>30</v>
       </c>
-      <c r="T79" s="1"/>
-    </row>
-    <row r="80" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+      <c r="X79" s="1"/>
+    </row>
+    <row r="80" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="C80" t="s">
         <v>25</v>
       </c>
@@ -9351,50 +10276,50 @@
         <f>D77+D78+D79</f>
         <v>907</v>
       </c>
-      <c r="I80" s="3">
-        <f>I77+I78+I79</f>
+      <c r="M80" s="3">
+        <f>M77+M78+M79</f>
         <v>3179</v>
       </c>
-      <c r="T80" s="1"/>
-    </row>
-    <row r="81" spans="4:20" hidden="1" x14ac:dyDescent="0.2">
-      <c r="T81" s="1"/>
-    </row>
-    <row r="82" spans="4:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="X80" s="1"/>
+    </row>
+    <row r="81" spans="4:24" hidden="1" x14ac:dyDescent="0.2">
+      <c r="X81" s="1"/>
+    </row>
+    <row r="82" spans="4:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="D82" t="s">
         <v>43</v>
       </c>
-      <c r="T82" s="1"/>
-    </row>
-    <row r="83" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="P83" s="3" t="s">
+      <c r="X82" s="1"/>
+    </row>
+    <row r="83" spans="4:24" x14ac:dyDescent="0.2">
+      <c r="T83" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="T83" s="1"/>
-    </row>
-    <row r="84" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="T84" s="1"/>
-    </row>
-    <row r="85" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="T85" s="1"/>
-    </row>
-    <row r="86" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="T86" s="1"/>
-    </row>
-    <row r="87" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="T87" s="1"/>
-    </row>
-    <row r="88" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="T88" s="1"/>
-    </row>
-    <row r="89" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="T89" s="1"/>
-    </row>
-    <row r="90" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="T90" s="1"/>
-    </row>
-    <row r="91" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="T91" s="1"/>
+      <c r="X83" s="1"/>
+    </row>
+    <row r="84" spans="4:24" x14ac:dyDescent="0.2">
+      <c r="X84" s="1"/>
+    </row>
+    <row r="85" spans="4:24" x14ac:dyDescent="0.2">
+      <c r="X85" s="1"/>
+    </row>
+    <row r="86" spans="4:24" x14ac:dyDescent="0.2">
+      <c r="X86" s="1"/>
+    </row>
+    <row r="87" spans="4:24" x14ac:dyDescent="0.2">
+      <c r="X87" s="1"/>
+    </row>
+    <row r="88" spans="4:24" x14ac:dyDescent="0.2">
+      <c r="X88" s="1"/>
+    </row>
+    <row r="89" spans="4:24" x14ac:dyDescent="0.2">
+      <c r="X89" s="1"/>
+    </row>
+    <row r="90" spans="4:24" x14ac:dyDescent="0.2">
+      <c r="X90" s="1"/>
+    </row>
+    <row r="91" spans="4:24" x14ac:dyDescent="0.2">
+      <c r="X91" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -9430,18 +10355,18 @@
     <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="24"/>
       <c r="B1" s="24"/>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
     </row>
-    <row r="2" spans="1:25" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" ht="80" x14ac:dyDescent="0.2">
       <c r="A2" s="16"/>
       <c r="B2" s="25" t="s">
         <v>2</v>
@@ -9601,11 +10526,11 @@
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="24"/>
       <c r="B6" s="24"/>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="24"/>
@@ -9627,7 +10552,7 @@
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
     </row>
-    <row r="7" spans="1:25" ht="85" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" ht="80" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
       <c r="B7" s="25" t="s">
         <v>2</v>
@@ -9786,11 +10711,11 @@
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="24"/>
       <c r="B11" s="24"/>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="24"/>
@@ -9812,7 +10737,7 @@
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
     </row>
-    <row r="12" spans="1:25" ht="85" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" ht="80" x14ac:dyDescent="0.2">
       <c r="A12" s="16"/>
       <c r="B12" s="25" t="s">
         <v>2</v>
@@ -9971,11 +10896,11 @@
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="24"/>
       <c r="B16" s="24"/>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
       <c r="H16" s="24"/>
@@ -9997,7 +10922,7 @@
       <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
     </row>
-    <row r="17" spans="1:25" ht="85" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" ht="80" x14ac:dyDescent="0.2">
       <c r="A17" s="16"/>
       <c r="B17" s="25" t="s">
         <v>2</v>
@@ -10149,11 +11074,11 @@
     <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" s="24"/>
       <c r="B21" s="24"/>
-      <c r="C21" s="30" t="s">
+      <c r="C21" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
       <c r="H21" s="24"/>
@@ -10175,7 +11100,7 @@
       <c r="X21" s="4"/>
       <c r="Y21" s="4"/>
     </row>
-    <row r="22" spans="1:25" ht="85" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" ht="80" x14ac:dyDescent="0.2">
       <c r="A22" s="16"/>
       <c r="B22" s="25" t="s">
         <v>2</v>
@@ -10327,11 +11252,11 @@
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" s="24"/>
       <c r="B26" s="24"/>
-      <c r="C26" s="30" t="s">
+      <c r="C26" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
       <c r="H26" s="24"/>
@@ -10353,7 +11278,7 @@
       <c r="X26" s="4"/>
       <c r="Y26" s="4"/>
     </row>
-    <row r="27" spans="1:25" ht="85" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" ht="80" x14ac:dyDescent="0.2">
       <c r="A27" s="16"/>
       <c r="B27" s="25" t="s">
         <v>2</v>
@@ -10505,11 +11430,11 @@
     <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" s="24"/>
       <c r="B31" s="24"/>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
       <c r="H31" s="24"/>
@@ -10531,7 +11456,7 @@
       <c r="X31" s="4"/>
       <c r="Y31" s="4"/>
     </row>
-    <row r="32" spans="1:25" ht="85" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" ht="80" x14ac:dyDescent="0.2">
       <c r="A32" s="16"/>
       <c r="B32" s="25" t="s">
         <v>2</v>
@@ -10683,11 +11608,11 @@
     <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" s="24"/>
       <c r="B36" s="24"/>
-      <c r="C36" s="30" t="s">
+      <c r="C36" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
       <c r="F36" s="13"/>
       <c r="G36" s="13"/>
       <c r="H36" s="24"/>
@@ -10862,11 +11787,11 @@
     <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41" s="24"/>
       <c r="B41" s="24"/>
-      <c r="C41" s="30" t="s">
+      <c r="C41" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="D41" s="30"/>
-      <c r="E41" s="30"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
       <c r="H41" s="24"/>
@@ -11041,11 +11966,11 @@
     <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A46" s="24"/>
       <c r="B46" s="24"/>
-      <c r="C46" s="30" t="s">
+      <c r="C46" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="D46" s="30"/>
-      <c r="E46" s="30"/>
+      <c r="D46" s="34"/>
+      <c r="E46" s="34"/>
       <c r="F46" s="13"/>
       <c r="G46" s="13"/>
       <c r="H46" s="24"/>
@@ -11220,11 +12145,11 @@
     <row r="51" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A51" s="24"/>
       <c r="B51" s="24"/>
-      <c r="C51" s="30" t="s">
+      <c r="C51" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="D51" s="30"/>
-      <c r="E51" s="30"/>
+      <c r="D51" s="34"/>
+      <c r="E51" s="34"/>
       <c r="F51" s="13"/>
       <c r="G51" s="13"/>
       <c r="H51" s="24"/>
@@ -11399,11 +12324,11 @@
     <row r="56" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A56" s="24"/>
       <c r="B56" s="24"/>
-      <c r="C56" s="30" t="s">
+      <c r="C56" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="D56" s="30"/>
-      <c r="E56" s="30"/>
+      <c r="D56" s="34"/>
+      <c r="E56" s="34"/>
       <c r="F56" s="13"/>
       <c r="G56" s="13"/>
       <c r="H56" s="24"/>
@@ -11578,11 +12503,11 @@
     <row r="61" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A61" s="24"/>
       <c r="B61" s="24"/>
-      <c r="C61" s="30" t="s">
+      <c r="C61" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="D61" s="30"/>
-      <c r="E61" s="30"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="34"/>
       <c r="F61" s="13"/>
       <c r="G61" s="13"/>
       <c r="H61" s="24"/>
@@ -11757,11 +12682,11 @@
     <row r="66" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A66" s="24"/>
       <c r="B66" s="24"/>
-      <c r="C66" s="30" t="s">
+      <c r="C66" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="D66" s="30"/>
-      <c r="E66" s="30"/>
+      <c r="D66" s="34"/>
+      <c r="E66" s="34"/>
       <c r="F66" s="13"/>
       <c r="G66" s="13"/>
       <c r="H66" s="24"/>
@@ -11936,11 +12861,11 @@
     <row r="71" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A71" s="24"/>
       <c r="B71" s="24"/>
-      <c r="C71" s="30" t="s">
+      <c r="C71" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="D71" s="30"/>
-      <c r="E71" s="30"/>
+      <c r="D71" s="34"/>
+      <c r="E71" s="34"/>
       <c r="F71" s="13"/>
       <c r="G71" s="13"/>
       <c r="H71" s="24"/>
@@ -12115,11 +13040,11 @@
     <row r="76" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A76" s="24"/>
       <c r="B76" s="24"/>
-      <c r="C76" s="30" t="s">
+      <c r="C76" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="D76" s="30"/>
-      <c r="E76" s="30"/>
+      <c r="D76" s="34"/>
+      <c r="E76" s="34"/>
       <c r="F76" s="13"/>
       <c r="G76" s="13"/>
       <c r="H76" s="24"/>
@@ -12298,6 +13223,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C76:E76"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C71:E71"/>
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="C36:E36"/>
     <mergeCell ref="C41:E41"/>
@@ -12307,13 +13239,6 @@
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C21:E21"/>
     <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C76:E76"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C71:E71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
in the predictor I was calculating the the score of a prediction according based on a weight; this weight is its frequency. this frequency was obtained through a rank call; now I just access the uint64_t* alphabetCounters
</commit_message>
<xml_diff>
--- a/sbp-accuracy-other-predictors.xlsx
+++ b/sbp-accuracy-other-predictors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelktistakis/Repositories/sBP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CAC895-7E17-FB4D-A84C-F2E5CB591D51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A642C9-3176-404E-A1A6-35A79B3D847A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="56240" yWindow="1440" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -256,7 +256,7 @@
     <t>0.42 ???</t>
   </si>
   <si>
-    <t>/+OPT4   : mapped input [0,sigma), alphabetCounters is unit64[], alphabet is removed, no alaphabet selects, removed extra L[] accesses</t>
+    <t>/+OPT4   : mapped input [0,sigma), alphabetCounters is unit64[], alphabet is removed, no alaphabet selects, removed extra L[] accesses, predictor confidence ranks removed</t>
   </si>
 </sst>
 </file>
@@ -7033,13 +7033,15 @@
   <dimension ref="A1:AN91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="86" zoomScaleNormal="44" zoomScalePageLayoutView="44" workbookViewId="0">
-      <selection activeCell="L70" sqref="L70"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="6" max="13" width="10.83203125" style="5"/>
+    <col min="6" max="11" width="10.83203125" style="5"/>
+    <col min="12" max="12" width="24.83203125" style="5" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" style="5"/>
     <col min="25" max="25" width="13.5" customWidth="1"/>
     <col min="35" max="35" width="10.83203125" customWidth="1"/>
     <col min="40" max="40" width="12.6640625" bestFit="1" customWidth="1"/>
@@ -7067,7 +7069,7 @@
       <c r="AM1" s="29"/>
       <c r="AN1" s="29"/>
     </row>
-    <row r="2" spans="1:40" ht="255" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:40" ht="323" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -7465,7 +7467,7 @@
         <v>570</v>
       </c>
       <c r="L10" s="16">
-        <v>319.92857142857144</v>
+        <v>153.78</v>
       </c>
       <c r="M10" s="12">
         <f>370.903*1000</f>
@@ -7926,7 +7928,7 @@
         <v>420</v>
       </c>
       <c r="L20" s="12">
-        <v>178</v>
+        <v>120.85</v>
       </c>
       <c r="M20" s="12">
         <f>0.35*1000</f>
@@ -8386,7 +8388,7 @@
         <v>104</v>
       </c>
       <c r="L30" s="12">
-        <v>65</v>
+        <v>21.92</v>
       </c>
       <c r="M30" s="12">
         <f>0.11*1000</f>
@@ -8846,7 +8848,7 @@
         <v>270</v>
       </c>
       <c r="L40" s="12">
-        <v>442</v>
+        <v>102.35</v>
       </c>
       <c r="M40" s="12">
         <f>26.4*1000</f>
@@ -9306,7 +9308,7 @@
         <v>62</v>
       </c>
       <c r="L50" s="12">
-        <v>77</v>
+        <v>17.14</v>
       </c>
       <c r="M50" s="12">
         <f xml:space="preserve"> 0.77*1000</f>
@@ -9766,7 +9768,7 @@
         <v>97000</v>
       </c>
       <c r="L60" s="12">
-        <v>83174</v>
+        <v>48014</v>
       </c>
       <c r="M60" s="12">
         <f>1992.633*1000</f>
@@ -10226,7 +10228,7 @@
         <v>1100</v>
       </c>
       <c r="L70" s="12">
-        <v>741</v>
+        <v>341.14</v>
       </c>
       <c r="M70" s="12">
         <f>18.143*1000</f>

</xml_diff>

<commit_message>
Patter of the form ??abc is not part of the prediction process anymore
</commit_message>
<xml_diff>
--- a/sbp-accuracy-other-predictors.xlsx
+++ b/sbp-accuracy-other-predictors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelktistakis/Repositories/sBP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A642C9-3176-404E-A1A6-35A79B3D847A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8003B3EB-024A-D045-B6CF-699AE7A269A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="56240" yWindow="1440" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7033,7 +7033,7 @@
   <dimension ref="A1:AN91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="86" zoomScaleNormal="44" zoomScalePageLayoutView="44" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="L70" activeCellId="6" sqref="L10 L20 L30 L40 L50 L60 L70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7467,7 +7467,7 @@
         <v>570</v>
       </c>
       <c r="L10" s="16">
-        <v>153.78</v>
+        <v>152</v>
       </c>
       <c r="M10" s="12">
         <f>370.903*1000</f>
@@ -10228,7 +10228,7 @@
         <v>1100</v>
       </c>
       <c r="L70" s="12">
-        <v>341.14</v>
+        <v>340</v>
       </c>
       <c r="M70" s="12">
         <f>18.143*1000</f>

</xml_diff>